<commit_message>
Revert "passage à JXLS"
This reverts commit 976cccd6913cf1696d9f2a6c2172484d5dcaedc6.
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D851667A-9B8F-44EB-9B66-981C77FF571E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BED1B3-07C2-4B10-9CDD-0BFBC9B243A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="555" windowWidth="22770" windowHeight="13695" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="4005" yWindow="1815" windowWidth="24915" windowHeight="13320" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -48,30 +48,6 @@
     <author>Sébastien</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3443014A-917C-4C38-93C1-54CFC94D92F9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:area(lastCell="AX3")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="J1" authorId="0" shapeId="0" xr:uid="{46CD7ABF-224E-46F0-A443-9BFA12BC8FFF}">
       <text>
         <r>
@@ -751,198 +727,6 @@
           </rPr>
           <t xml:space="preserve">
 Age suivant la règle SGDF : 19 pour les LJ, SG et 21 ans pour les PK</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{319C0CDA-DBC9-4113-8E4F-422603518754}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="chefs" var="chef" orderBy="codestructure;fonction;nom" lastCell="AX2")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{189A9F99-E599-47EA-8FF2-3AF12E72E480}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:if(condition="${chef.qualif.dirsf.aetaetetitulaire}" ifArea="J2")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{04ABEDBF-64D8-4525-92EB-17CA058D2D8D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:if(condition="${chef.qualif.dirsf.pasok}" ifArea="K2")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{B4ADD871-E32F-4D5A-8B4E-9F0465977AFB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:if(condition="chef.bafapotentiel == true" ifArea="$AZ$2")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{CCF6586A-C102-4AD2-8EE4-064DAE99525B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="compas" var="chef" orderBy="codestructure;fonction;nom" lastCell="AX3")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{4A5E05D7-A542-4662-9D18-E81959ED0AD7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:if(condition="${chef.qualif.dirsf.aetaetetitulaire}" ifArea="J3")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{898E24B5-0DAB-4681-9DD6-FEFFA674969E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:if(condition="${chef.qualif.dirsf.pasok}" ifArea="K3")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{7042F557-4712-4A23-BA92-4C893E39A4EB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:if(condition="chef.bafapotentiel == true" ifArea="$AZ$2")</t>
         </r>
       </text>
     </comment>
@@ -951,7 +735,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="196">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -1130,6 +914,12 @@
     <t>Directeur</t>
   </si>
   <si>
+    <t>&lt;jt:if test="${chef.qualif.animsf.ok}"&gt;${chef.qualif.animsf.finvalidite}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${chef.qualif.animsf.pasok}"&gt;${chef.qualif.animsf.finvalidite}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
     <t>Théorique</t>
   </si>
   <si>
@@ -1148,6 +938,9 @@
     <t>Stagiaire BAFA potentiel</t>
   </si>
   <si>
+    <t>&lt;jt:if test="${chef.bafapotentiel}"&gt;Oui&lt;/jt:if&gt;</t>
+  </si>
+  <si>
     <t>Code Structure</t>
   </si>
   <si>
@@ -1157,6 +950,9 @@
     <t>${unite.codestructure}</t>
   </si>
   <si>
+    <t>&lt;jt:if test="${chef.qualif.dirsf.pasok}"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
     <t>${global.groupe}</t>
   </si>
   <si>
@@ -1184,6 +980,9 @@
     <t>Anim SF stagiaire</t>
   </si>
   <si>
+    <t>&lt;jt:forEach items="${chefs}" var="chef" orderBy="codestructure;fonction;nom"&gt;${chef.codetext}</t>
+  </si>
+  <si>
     <t>Code Groupe</t>
   </si>
   <si>
@@ -1191,6 +990,9 @@
   </si>
   <si>
     <t>${unite.codegroupe}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${compas}" var="chef" orderBy="codestructure;fonction;nom"&gt;${chef.codetext}</t>
   </si>
   <si>
     <t>Version</t>
@@ -1311,6 +1113,9 @@
   </si>
   <si>
     <t>$[CEILING($D4*0.8/12,1)+1]</t>
+  </si>
+  <si>
+    <t>${chef.ageok}&lt;/jt:forEach&gt;</t>
   </si>
   <si>
     <t>$[M4-L4]</t>
@@ -1527,28 +1332,13 @@
     <t>${chef.formation.accueil_scoutisme_rg.datefin}</t>
   </si>
   <si>
+    <t>&lt;jt:if test="${chef.qualif.dirsf.aetaetetitulaire}" onProcessed="org.leplan73.outilssgdf.gui.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
     <t>Fonction secondaire</t>
   </si>
   <si>
     <t>${chef.fonctionsecondairecomplet}</t>
-  </si>
-  <si>
-    <t>${chef.codetext}</t>
-  </si>
-  <si>
-    <t>${chef.ageok}</t>
-  </si>
-  <si>
-    <t>${chef.qualif.dirsf.finvalidite}</t>
-  </si>
-  <si>
-    <t>${chef.qualif.animsf.finvalidite}</t>
-  </si>
-  <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t>Non</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1773,97 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2173,97 +2053,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF007E39"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2711,10 +2501,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:BA3"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,7 +2547,7 @@
     <col min="50" max="50" width="14.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2768,67 +2561,67 @@
         <v>18</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>54</v>
       </c>
       <c r="H1" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="X1" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="U1" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="V1" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="W1" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="X1" s="29" t="s">
-        <v>179</v>
-      </c>
       <c r="Y1" s="29" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="Z1" s="29" t="s">
         <v>9</v>
@@ -2837,19 +2630,19 @@
         <v>10</v>
       </c>
       <c r="AB1" s="29" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="AC1" s="29" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="AD1" s="29" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="AE1" s="29" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="AF1" s="29" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="AG1" s="29" t="s">
         <v>11</v>
@@ -2858,19 +2651,19 @@
         <v>12</v>
       </c>
       <c r="AI1" s="29" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="AJ1" s="29" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="AK1" s="29" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="AL1" s="29" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="AM1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AN1" s="30" t="s">
         <v>13</v>
@@ -2894,21 +2687,21 @@
         <v>17</v>
       </c>
       <c r="AU1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AV1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="AW1" s="15" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="AX1" s="15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>188</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2920,58 +2713,60 @@
         <v>56</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>190</v>
+        <v>71</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>191</v>
+        <v>59</v>
       </c>
       <c r="M2" s="28" t="s">
-        <v>191</v>
+        <v>60</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="Q2" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="R2" s="3"/>
       <c r="S2" s="28" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="T2" s="28" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="U2" s="28" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="V2" s="28" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="W2" s="28" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="X2" s="28" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="Y2" s="28" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="Z2" s="28" t="s">
         <v>44</v>
@@ -2980,19 +2775,19 @@
         <v>45</v>
       </c>
       <c r="AB2" s="28" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="AC2" s="28" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="AD2" s="28" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="AE2" s="28" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="AF2" s="28" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="AG2" s="28" t="s">
         <v>46</v>
@@ -3001,16 +2796,16 @@
         <v>47</v>
       </c>
       <c r="AI2" s="28" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AJ2" s="28" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="AK2" s="28" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="AL2" s="28" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="AM2" s="3"/>
       <c r="AN2" s="28" t="s">
@@ -3032,28 +2827,22 @@
         <v>52</v>
       </c>
       <c r="AT2" s="28" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="AU2" s="3"/>
       <c r="AV2" s="26" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>192</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>193</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -3065,58 +2854,60 @@
         <v>56</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>190</v>
+        <v>71</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>191</v>
+        <v>59</v>
       </c>
       <c r="M3" s="28" t="s">
-        <v>191</v>
+        <v>60</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="R3" s="3"/>
       <c r="S3" s="28" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="T3" s="28" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="U3" s="28" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="V3" s="28" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="W3" s="28" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="X3" s="28" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="Y3" s="28" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="Z3" s="28" t="s">
         <v>44</v>
@@ -3125,19 +2916,19 @@
         <v>45</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="AC3" s="28" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="AD3" s="28" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="AE3" s="28" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="AF3" s="28" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="AG3" s="28" t="s">
         <v>46</v>
@@ -3146,16 +2937,16 @@
         <v>47</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AJ3" s="28" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="AK3" s="28" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="AL3" s="28" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="AM3" s="3"/>
       <c r="AN3" s="28" t="s">
@@ -3177,17 +2968,17 @@
         <v>52</v>
       </c>
       <c r="AT3" s="28" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="AU3" s="3"/>
       <c r="AV3" s="26" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AW3" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="AX3" s="3" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3235,34 +3026,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H65536">
-    <cfRule type="beginsWith" dxfId="28" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(H2,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="27" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(H2,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="7" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(H2,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="25" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="6" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(H2,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="5" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(H2,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="23" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="4" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(H2,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(H2,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(H2,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(H2,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(H2,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3312,13 +3103,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>19</v>
@@ -3330,7 +3121,7 @@
         <v>21</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>23</v>
@@ -3339,7 +3130,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L1" s="29" t="s">
         <v>8</v>
@@ -3351,22 +3142,22 @@
         <v>10</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="Q1" s="29" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="S1" s="29" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="U1" s="19" t="s">
         <v>27</v>
@@ -3386,13 +3177,13 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
@@ -3422,19 +3213,19 @@
         <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="2" t="s">
@@ -3520,49 +3311,49 @@
       <c r="C1" s="8"/>
       <c r="E1" s="2"/>
       <c r="F1" s="15" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="M1" s="48"/>
       <c r="N1" s="49"/>
       <c r="O1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="P1" s="47" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="Q1" s="50"/>
       <c r="R1" s="51"/>
       <c r="S1" s="31"/>
       <c r="T1" s="47" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="U1" s="50"/>
       <c r="V1" s="51"/>
       <c r="W1" s="50" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="X1" s="50"/>
       <c r="Y1" s="51"/>
       <c r="Z1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AA1" s="52" t="s">
         <v>42</v>
@@ -3600,162 +3391,162 @@
     </row>
     <row r="3" spans="1:29" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L3" s="43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M3" s="43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="P3" s="43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q3" s="43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R3" s="43" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="T3" s="43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="U3" s="43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="W3" s="34" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="X3" s="43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Y3" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="Z3" s="23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AA3" s="43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2">
         <v>1</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
@@ -3773,47 +3564,47 @@
     <mergeCell ref="AA1:AC1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F65536">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G65536">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H65536">
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I65536">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J65536">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N65536">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:V65536">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4:Y65536">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC65536">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3878,22 +3669,22 @@
       <c r="D1" s="54"/>
       <c r="E1" s="55"/>
       <c r="G1" s="15" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>27</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M1" s="52" t="s">
         <v>58</v>
@@ -3901,27 +3692,27 @@
       <c r="N1" s="48"/>
       <c r="O1" s="49"/>
       <c r="P1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Q1" s="47" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="R1" s="50"/>
       <c r="S1" s="51"/>
       <c r="T1" s="31"/>
       <c r="U1" s="47" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="V1" s="50"/>
       <c r="W1" s="51"/>
       <c r="X1" s="44"/>
       <c r="Y1" s="47" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="Z1" s="50"/>
       <c r="AA1" s="51"/>
       <c r="AB1" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AC1" s="52" t="s">
         <v>42</v>
@@ -3966,10 +3757,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>19</v>
@@ -3978,93 +3769,93 @@
         <v>20</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="I3" s="46" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="J3" s="46" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="L3" s="45" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="N3" s="22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="P3" s="45" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="S3" s="22" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="T3" s="45" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="U3" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="V3" s="22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="W3" s="22" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Z3" s="22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AA3" s="22" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="AB3" s="45" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AC3" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AD3" s="22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AE3" s="22" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
@@ -4073,65 +3864,65 @@
         <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="35" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="N4" s="35" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="AC4" s="2">
         <v>1</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4145,52 +3936,52 @@
     <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="O4:O65537">
-    <cfRule type="cellIs" dxfId="9" priority="14" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:S65537">
-    <cfRule type="cellIs" dxfId="8" priority="13" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="13" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4:W65537">
-    <cfRule type="cellIs" dxfId="7" priority="12" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="12" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA4:AA65537">
-    <cfRule type="cellIs" dxfId="6" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AE65537">
-    <cfRule type="cellIs" dxfId="5" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G65537">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H65537">
-    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I65537">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J65537">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K65537">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4213,10 +4004,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C1" s="6"/>
     </row>
@@ -4267,10 +4058,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des formations FIF et FCF
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BED1B3-07C2-4B10-9CDD-0BFBC9B243A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1379AB5D-05A9-4414-8DDC-D9CEA5CDC883}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="1815" windowWidth="24915" windowHeight="13320" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="795" yWindow="690" windowWidth="21810" windowHeight="13680" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Quotas Année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Quotas Camps'!$A$3:$AE$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AX$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AZ$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Synthèse par unité'!$A$1:$AE$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -490,7 +490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
       <text>
         <r>
           <rPr>
@@ -514,7 +514,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
+    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
+    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
       <text>
         <r>
           <rPr>
@@ -562,7 +562,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
+    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
       <text>
         <r>
           <rPr>
@@ -586,7 +586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
+    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
       <text>
         <r>
           <rPr>
@@ -610,7 +610,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
       <text>
         <r>
           <rPr>
@@ -634,7 +634,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
       <text>
         <r>
           <rPr>
@@ -658,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
+    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
       <text>
         <r>
           <rPr>
@@ -682,7 +682,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
+    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
       <text>
         <r>
           <rPr>
@@ -706,7 +706,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
+    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
       <text>
         <r>
           <rPr>
@@ -735,7 +735,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="200">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -1332,13 +1332,25 @@
     <t>${chef.formation.accueil_scoutisme_rg.datefin}</t>
   </si>
   <si>
-    <t>&lt;jt:if test="${chef.qualif.dirsf.aetaetetitulaire}" onProcessed="org.leplan73.outilssgdf.gui.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
-  </si>
-  <si>
     <t>Fonction secondaire</t>
   </si>
   <si>
     <t>${chef.fonctionsecondairecomplet}</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${chef.qualif.dirsf.aetaetetitulaire}" onProcessed="org.leplan73.outilssgdf.outils.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>FORMATION INITIALE DE FORMATEURS</t>
+  </si>
+  <si>
+    <t>FORMATION CONTINUE DE FORMATEURS</t>
+  </si>
+  <si>
+    <t>${chef.formation.fif.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.fcf.datefin}</t>
   </si>
 </sst>
 </file>
@@ -1773,97 +1785,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF007E39"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2053,7 +1975,97 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2501,13 +2513,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:AZ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,15 +2551,17 @@
     <col min="31" max="32" width="13" style="28" customWidth="1"/>
     <col min="33" max="37" width="11.42578125" style="28" customWidth="1"/>
     <col min="38" max="38" width="17.5703125" style="28" customWidth="1"/>
-    <col min="39" max="39" width="3.140625" style="2" customWidth="1"/>
-    <col min="40" max="46" width="11.42578125" style="28" customWidth="1"/>
-    <col min="47" max="47" width="4" style="2" customWidth="1"/>
-    <col min="48" max="48" width="12.7109375" style="2" customWidth="1"/>
-    <col min="49" max="49" width="15" style="2" customWidth="1"/>
-    <col min="50" max="50" width="14.140625" style="2" customWidth="1"/>
+    <col min="39" max="39" width="15.28515625" style="28" customWidth="1"/>
+    <col min="40" max="40" width="12.5703125" style="28" customWidth="1"/>
+    <col min="41" max="41" width="3.140625" style="2" customWidth="1"/>
+    <col min="42" max="48" width="11.42578125" style="28" customWidth="1"/>
+    <col min="49" max="49" width="4" style="2" customWidth="1"/>
+    <col min="50" max="50" width="12.7109375" style="2" customWidth="1"/>
+    <col min="51" max="51" width="15" style="2" customWidth="1"/>
+    <col min="52" max="52" width="14.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2570,7 +2584,7 @@
         <v>54</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I1" s="21" t="s">
         <v>76</v>
@@ -2662,44 +2676,50 @@
       <c r="AL1" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="AM1" s="21" t="s">
+      <c r="AM1" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="AN1" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="AO1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="AN1" s="30" t="s">
+      <c r="AP1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AO1" s="30" t="s">
+      <c r="AQ1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AP1" s="30" t="s">
+      <c r="AR1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AQ1" s="30" t="s">
+      <c r="AS1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="AR1" s="30" t="s">
+      <c r="AT1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AS1" s="30" t="s">
+      <c r="AU1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="AT1" s="30" t="s">
+      <c r="AV1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="AU1" s="21" t="s">
+      <c r="AW1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AX1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AW1" s="15" t="s">
+      <c r="AY1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="AX1" s="15" t="s">
+      <c r="AZ1" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>81</v>
       </c>
@@ -2722,10 +2742,10 @@
         <v>64</v>
       </c>
       <c r="H2" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>195</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>193</v>
       </c>
       <c r="K2" s="28" t="s">
         <v>71</v>
@@ -2807,40 +2827,46 @@
       <c r="AL2" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="AM2" s="3"/>
+      <c r="AM2" s="28" t="s">
+        <v>198</v>
+      </c>
       <c r="AN2" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="AO2" s="28" t="s">
+      <c r="AQ2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="AP2" s="28" t="s">
+      <c r="AR2" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="AQ2" s="28" t="s">
+      <c r="AS2" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="AR2" s="28" t="s">
+      <c r="AT2" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="AS2" s="28" t="s">
+      <c r="AU2" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="AT2" s="28" t="s">
+      <c r="AV2" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="26" t="s">
+      <c r="AW2" s="3"/>
+      <c r="AX2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AY2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>85</v>
       </c>
@@ -2863,10 +2889,10 @@
         <v>64</v>
       </c>
       <c r="H3" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="J3" s="28" t="s">
         <v>195</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>193</v>
       </c>
       <c r="K3" s="28" t="s">
         <v>71</v>
@@ -2948,47 +2974,53 @@
       <c r="AL3" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="AM3" s="3"/>
+      <c r="AM3" s="28" t="s">
+        <v>198</v>
+      </c>
       <c r="AN3" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="AO3" s="28" t="s">
+      <c r="AQ3" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="AP3" s="28" t="s">
+      <c r="AR3" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="AQ3" s="28" t="s">
+      <c r="AS3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="AR3" s="28" t="s">
+      <c r="AT3" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="AS3" s="28" t="s">
+      <c r="AU3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="AT3" s="28" t="s">
+      <c r="AV3" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="AU3" s="3"/>
-      <c r="AV3" s="26" t="s">
+      <c r="AW3" s="3"/>
+      <c r="AX3" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="AW3" s="3" t="s">
+      <c r="AY3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AX3" s="3" t="s">
+      <c r="AZ3" s="3" t="s">
         <v>125</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AX3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <conditionalFormatting sqref="AX2:AX65536">
+  <autoFilter ref="A1:AZ3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <conditionalFormatting sqref="AZ2:AZ65536">
     <cfRule type="cellIs" dxfId="40" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW2:AW65536">
+  <conditionalFormatting sqref="AY2:AY65536">
     <cfRule type="cellIs" dxfId="39" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -3026,34 +3058,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H65536">
-    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="28" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(H2,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="27" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(H2,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="26" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(H2,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="25" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(H2,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="24" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(H2,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="23" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(H2,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="22" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(H2,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="21" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(H2,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="20" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(H2,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="19" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(H2,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3074,7 +3106,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3564,47 +3596,47 @@
     <mergeCell ref="AA1:AC1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F65536">
-    <cfRule type="cellIs" dxfId="28" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G65536">
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H65536">
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I65536">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J65536">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N65536">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:V65536">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4:Y65536">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC65536">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3936,52 +3968,52 @@
     <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="O4:O65537">
-    <cfRule type="cellIs" dxfId="19" priority="14" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:S65537">
-    <cfRule type="cellIs" dxfId="18" priority="13" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="13" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4:W65537">
-    <cfRule type="cellIs" dxfId="17" priority="12" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="12" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA4:AA65537">
-    <cfRule type="cellIs" dxfId="16" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AE65537">
-    <cfRule type="cellIs" dxfId="15" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G65537">
-    <cfRule type="cellIs" dxfId="14" priority="5" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H65537">
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I65537">
-    <cfRule type="cellIs" dxfId="12" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J65537">
-    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K65537">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Filtrage du unité "non-jeune" dans les quotas de camp Filtrage du unité "non-jeune" dans les quotas de camp
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1379AB5D-05A9-4414-8DDC-D9CEA5CDC883}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E15DB37-F36F-4973-A6EA-1F865DECA3A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="690" windowWidth="21810" windowHeight="13680" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
-    <sheet name="Synthèse par unité" sheetId="3" r:id="rId2"/>
-    <sheet name="Quotas Année" sheetId="8" r:id="rId3"/>
-    <sheet name="Quotas Camps" sheetId="2" r:id="rId4"/>
-    <sheet name="Global" sheetId="9" r:id="rId5"/>
-    <sheet name="Général" sheetId="10" r:id="rId6"/>
-    <sheet name="Aide" sheetId="4" r:id="rId7"/>
+    <sheet name="Qualifications" sheetId="12" r:id="rId2"/>
+    <sheet name="Formations" sheetId="13" r:id="rId3"/>
+    <sheet name="Diplômes" sheetId="11" r:id="rId4"/>
+    <sheet name="Synthèse par unité" sheetId="3" r:id="rId5"/>
+    <sheet name="Quotas Année" sheetId="8" r:id="rId6"/>
+    <sheet name="Quotas Camps" sheetId="2" r:id="rId7"/>
+    <sheet name="Global" sheetId="9" r:id="rId8"/>
+    <sheet name="Général" sheetId="10" r:id="rId9"/>
+    <sheet name="Aide" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Quotas Année'!$A$3:$AC$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Quotas Camps'!$A$3:$AE$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AZ$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Synthèse par unité'!$A$1:$AE$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Diplômes!$A$1:$L$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Formations!$A$1:$AA$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Qualifications!$A$1:$N$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Quotas Année'!$A$3:$AC$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quotas Camps'!$A$3:$AE$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$L$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Synthèse par unité'!$A$1:$AE$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +54,89 @@
     <author>Sébastien</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{46CD7ABF-224E-46F0-A443-9BFA12BC8FFF}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Age aujourd'hui</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Age au 1er juillet prochain</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Age suivant la règle SGDF : 19 pour les LJ, SG et 21 ans pour les PK</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sébastien</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{905C7348-F4B2-4963-9D43-F692C6BCB07E}">
       <text>
         <r>
           <rPr>
@@ -72,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{E1578AE2-3E3D-4BF6-BDA1-0E6F28CF9A3F}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{A3B3A2F3-DC17-4DC7-94F8-B179C2728450}">
       <text>
         <r>
           <rPr>
@@ -96,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{85A87D93-DCFF-4024-A69F-EC8165F611A2}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{8B58F3BB-A36A-4A98-A40C-91AA8FD2F679}">
       <text>
         <r>
           <rPr>
@@ -120,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{C1BA196E-6BE0-448D-B5DF-539830267ED2}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{C24EDFC6-6157-43E5-833C-76817656A6CF}">
       <text>
         <r>
           <rPr>
@@ -144,7 +232,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{E61AC8E6-5369-486E-BB2A-CFC3F3BBFC62}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sébastien</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{60E4E0F6-7DF8-4A49-8516-9CA0D5538197}">
       <text>
         <r>
           <rPr>
@@ -168,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{BD73F079-BD47-4A9B-9DB9-888F403257F2}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{44FEFEDC-A3B6-4440-A607-CA059DB1D796}">
       <text>
         <r>
           <rPr>
@@ -192,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{4EEDDAC8-2343-467D-9346-63590EC6F6AE}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{1B3E1A7C-0680-43B6-A451-B9AD30B871AA}">
       <text>
         <r>
           <rPr>
@@ -216,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{6A99CB9E-35A8-4FA1-BC9B-4D96C495F872}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9CEDF5E2-D139-4510-A103-13F24DE204C2}">
       <text>
         <r>
           <rPr>
@@ -240,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{86FD4D1A-31E9-4CF5-B839-4DB3C6578C7B}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{2A55408E-B129-432E-95A2-3D62178E53C8}">
       <text>
         <r>
           <rPr>
@@ -264,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{D4CB2E41-2D86-492F-A896-A7F2621165D9}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{0DD2F092-25CF-43A2-8C2E-3982770EFBCF}">
       <text>
         <r>
           <rPr>
@@ -288,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{55CC420A-73E2-4858-9D36-083E75638385}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{AC82776C-F530-4190-B75F-397D22581B23}">
       <text>
         <r>
           <rPr>
@@ -312,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{E842F17D-4EA4-46A7-8AA9-D11373D8D411}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{EEC66E3F-8B4A-467C-8A5C-B64083AA3370}">
       <text>
         <r>
           <rPr>
@@ -336,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{83C77407-EDE7-4503-93FD-393628AE54E4}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{2D4538CE-D3F1-4FF9-ACD5-AAC67EC52826}">
       <text>
         <r>
           <rPr>
@@ -360,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{83CCAF6B-404B-4C1D-92E5-BE497427DD7D}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{E2F6D111-FFD2-44BA-9F41-49F796F2947E}">
       <text>
         <r>
           <rPr>
@@ -384,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{156BCBB7-1FAF-413C-8ECC-A4A9CA20E3FD}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{77306F0C-F710-4452-BAF6-5C1D346D28EC}">
       <text>
         <r>
           <rPr>
@@ -418,7 +516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{2C5F74EA-D518-4557-AC0F-8BFFC404907C}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{4466B097-0290-42E9-B624-B1A0AD9D1C42}">
       <text>
         <r>
           <rPr>
@@ -442,7 +540,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{6045E9B0-AA1D-41B4-9C3C-BC746D9BC589}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{957A0E74-9F8C-4A5B-9184-FE95E02D667F}">
       <text>
         <r>
           <rPr>
@@ -466,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{1F3E1ACB-E2A6-4A98-A36E-7ABE327D55F6}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{A20B21DD-1881-441A-A5A4-C77419ED7E93}">
       <text>
         <r>
           <rPr>
@@ -490,7 +588,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sébastien</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E72231DA-93D3-4418-B8D7-76AE634C1E08}">
       <text>
         <r>
           <rPr>
@@ -514,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{D775B390-A3E7-4B49-97AA-2086091F8E1A}">
       <text>
         <r>
           <rPr>
@@ -538,7 +646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{62B9A651-BDE7-475F-9529-41A0A2DFFE4C}">
       <text>
         <r>
           <rPr>
@@ -562,7 +670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{D8956881-F0C9-4848-9228-EC603B219F1B}">
       <text>
         <r>
           <rPr>
@@ -586,7 +694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{4FBAC0A5-B5E9-489B-BA35-16CC127A2F12}">
       <text>
         <r>
           <rPr>
@@ -610,7 +718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{5CE5F81E-8961-4DF0-9C77-4A9112F7205C}">
       <text>
         <r>
           <rPr>
@@ -634,7 +742,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{E6AD01D7-75FD-456C-B7A9-382930AB949C}">
       <text>
         <r>
           <rPr>
@@ -655,78 +763,6 @@
           </rPr>
           <t xml:space="preserve">
 Date d'obtention</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Age aujourd'hui</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Age au 1er juillet prochain</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Age suivant la règle SGDF : 19 pour les LJ, SG et 21 ans pour les PK</t>
         </r>
       </text>
     </comment>
@@ -735,7 +771,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="201">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -938,9 +974,6 @@
     <t>Stagiaire BAFA potentiel</t>
   </si>
   <si>
-    <t>&lt;jt:if test="${chef.bafapotentiel}"&gt;Oui&lt;/jt:if&gt;</t>
-  </si>
-  <si>
     <t>Code Structure</t>
   </si>
   <si>
@@ -1008,9 +1041,6 @@
   </si>
   <si>
     <t>Titulaire ou stagiaire Dir ou anim</t>
-  </si>
-  <si>
-    <t>${chef.diplome.buchettes4.dateobtention}</t>
   </si>
   <si>
     <t>${chef.qualifs}</t>
@@ -1350,7 +1380,16 @@
     <t>${chef.formation.fif.datefin}</t>
   </si>
   <si>
-    <t>${chef.formation.fcf.datefin}</t>
+    <t>&lt;jt:if test="${chef.bafapotentiel}"&gt;Oui&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${chef.formation.fcf.datefin}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${chef.diplome.buchettes4.dateobtention}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${unites}" var="unite" orderBy="codestructure" where="${unite.nonPrincipal}" &gt;${unite.nom}</t>
   </si>
 </sst>
 </file>
@@ -2513,11 +2552,11 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2531,37 +2570,13 @@
     <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
     <col min="7" max="8" width="10.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="28" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="2.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="2.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="28" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" style="28" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" style="28" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="28" customWidth="1"/>
-    <col min="23" max="23" width="18" style="28" customWidth="1"/>
-    <col min="24" max="25" width="14.28515625" style="28" customWidth="1"/>
-    <col min="26" max="27" width="11.42578125" style="28" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" style="28" customWidth="1"/>
-    <col min="29" max="29" width="11.42578125" style="28" customWidth="1"/>
-    <col min="30" max="30" width="14.140625" style="28" customWidth="1"/>
-    <col min="31" max="32" width="13" style="28" customWidth="1"/>
-    <col min="33" max="37" width="11.42578125" style="28" customWidth="1"/>
-    <col min="38" max="38" width="17.5703125" style="28" customWidth="1"/>
-    <col min="39" max="39" width="15.28515625" style="28" customWidth="1"/>
-    <col min="40" max="40" width="12.5703125" style="28" customWidth="1"/>
-    <col min="41" max="41" width="3.140625" style="2" customWidth="1"/>
-    <col min="42" max="48" width="11.42578125" style="28" customWidth="1"/>
-    <col min="49" max="49" width="4" style="2" customWidth="1"/>
-    <col min="50" max="50" width="12.7109375" style="2" customWidth="1"/>
-    <col min="51" max="51" width="15" style="2" customWidth="1"/>
-    <col min="52" max="52" width="14.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2575,153 +2590,33 @@
         <v>18</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>54</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="U1" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="V1" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="W1" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="X1" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y1" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="Z1" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA1" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB1" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="AC1" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="AD1" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="AE1" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="AF1" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="AG1" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH1" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI1" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ1" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="AK1" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="AL1" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AM1" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN1" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP1" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ1" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="AR1" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="AS1" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="AT1" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="AU1" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV1" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="AW1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="AX1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="AY1" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AZ1" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2733,142 +2628,31 @@
         <v>56</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>64</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="W2" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y2" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="Z2" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC2" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD2" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE2" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF2" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="AG2" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH2" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI2" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ2" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK2" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="AL2" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM2" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="AN2" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ2" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR2" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS2" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT2" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU2" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV2" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>125</v>
+      <c r="I2" s="3"/>
+      <c r="J2" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2880,147 +2664,36 @@
         <v>56</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>64</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="T3" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="U3" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="V3" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="W3" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="X3" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y3" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="Z3" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA3" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB3" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC3" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD3" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE3" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF3" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="AG3" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH3" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI3" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ3" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK3" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="AL3" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM3" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="AN3" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="AO3" s="3"/>
-      <c r="AP3" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ3" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR3" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS3" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT3" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU3" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV3" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW3" s="3"/>
-      <c r="AX3" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AZ3" s="3" t="s">
-        <v>125</v>
+      <c r="I3" s="3"/>
+      <c r="J3" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AZ3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <conditionalFormatting sqref="AZ2:AZ65536">
+  <autoFilter ref="A1:L3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <conditionalFormatting sqref="L2:L65536">
     <cfRule type="cellIs" dxfId="40" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY2:AY65536">
+  <conditionalFormatting sqref="K2:K65536">
     <cfRule type="cellIs" dxfId="39" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -3095,7 +2768,611 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FF42C4-E612-4A2B-8582-F0FFD086172F}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E839BC-6F29-4F14-B58D-1E2088939687}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="9" width="11.42578125" style="28" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="2.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="21"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B21C5B7-5B9C-4DD6-AED7-1EA1BDB21D53}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="28" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="28" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="28" customWidth="1"/>
+    <col min="10" max="10" width="18" style="28" customWidth="1"/>
+    <col min="11" max="12" width="14.28515625" style="28" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" style="28" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="28" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="28" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="28" customWidth="1"/>
+    <col min="18" max="19" width="13" style="28" customWidth="1"/>
+    <col min="20" max="24" width="11.42578125" style="28" customWidth="1"/>
+    <col min="25" max="25" width="17.5703125" style="28" customWidth="1"/>
+    <col min="26" max="26" width="15.28515625" style="28" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y1" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z1" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA1" s="29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y2" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA2" s="28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="W3" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="X3" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y3" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z3" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA3" s="28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AA3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC055CEB-F8BF-4FEF-96B7-58AA4EBF5327}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" style="2" customWidth="1"/>
+    <col min="6" max="12" width="11.42578125" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626E417A-45EE-4D6C-95FD-A71D343FE19B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -3103,10 +3380,10 @@
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,12 +3391,12 @@
     <col min="1" max="1" width="75.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="2"/>
     <col min="6" max="7" width="8.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="2" customWidth="1"/>
     <col min="9" max="10" width="8.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="5" style="2" customWidth="1"/>
     <col min="13" max="13" width="5.5703125" style="2" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" style="2" customWidth="1"/>
@@ -3128,6 +3405,7 @@
     <col min="17" max="17" width="14.85546875" customWidth="1"/>
     <col min="18" max="18" width="17.28515625" customWidth="1"/>
     <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="20" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3135,13 +3413,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>19</v>
@@ -3153,7 +3431,7 @@
         <v>21</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>23</v>
@@ -3162,7 +3440,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L1" s="29" t="s">
         <v>8</v>
@@ -3174,22 +3452,22 @@
         <v>10</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q1" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="S1" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U1" s="19" t="s">
         <v>27</v>
@@ -3212,10 +3490,10 @@
         <v>63</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
@@ -3245,19 +3523,19 @@
         <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="2" t="s">
@@ -3296,7 +3574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86524C9-1323-498D-ABE2-77D2F4C73D5A}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -3307,7 +3585,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,15 +3600,15 @@
     <col min="8" max="8" width="9" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" style="2" customWidth="1"/>
     <col min="13" max="13" width="8.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="6.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="3.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" style="2" customWidth="1"/>
     <col min="16" max="16" width="11" style="2" customWidth="1"/>
     <col min="17" max="17" width="10.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="7.7109375" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" customWidth="1"/>
     <col min="22" max="22" width="8.42578125" customWidth="1"/>
     <col min="24" max="24" width="9" customWidth="1"/>
     <col min="25" max="25" width="15.85546875" customWidth="1"/>
@@ -3343,49 +3621,49 @@
       <c r="C1" s="8"/>
       <c r="E1" s="2"/>
       <c r="F1" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M1" s="48"/>
       <c r="N1" s="49"/>
       <c r="O1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P1" s="47" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="50"/>
       <c r="R1" s="51"/>
       <c r="S1" s="31"/>
       <c r="T1" s="47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="U1" s="50"/>
       <c r="V1" s="51"/>
       <c r="W1" s="50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="X1" s="50"/>
       <c r="Y1" s="51"/>
       <c r="Z1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA1" s="52" t="s">
         <v>42</v>
@@ -3423,33 +3701,33 @@
     </row>
     <row r="3" spans="1:29" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>102</v>
-      </c>
       <c r="K3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L3" s="43" t="s">
         <v>61</v>
@@ -3458,10 +3736,10 @@
         <v>62</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P3" s="43" t="s">
         <v>61</v>
@@ -3470,10 +3748,10 @@
         <v>62</v>
       </c>
       <c r="R3" s="43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T3" s="43" t="s">
         <v>61</v>
@@ -3482,7 +3760,7 @@
         <v>62</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="W3" s="34" t="s">
         <v>61</v>
@@ -3491,10 +3769,10 @@
         <v>62</v>
       </c>
       <c r="Y3" s="32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Z3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA3" s="43" t="s">
         <v>61</v>
@@ -3503,12 +3781,12 @@
         <v>62</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
@@ -3518,67 +3796,67 @@
         <v>57</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2">
         <v>1</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
@@ -3645,7 +3923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64634AA-9071-4111-8E53-9AF735BF36D3}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -3666,29 +3944,29 @@
     <col min="3" max="3" width="17.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" style="2" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="35" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.42578125" style="35" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" style="2" customWidth="1"/>
     <col min="19" max="19" width="7.85546875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" customWidth="1"/>
     <col min="21" max="21" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.140625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="4.85546875" customWidth="1"/>
+    <col min="24" max="24" width="2.85546875" customWidth="1"/>
     <col min="25" max="25" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.5703125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" customWidth="1"/>
+    <col min="28" max="28" width="2.85546875" customWidth="1"/>
     <col min="29" max="29" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -3701,22 +3979,22 @@
       <c r="D1" s="54"/>
       <c r="E1" s="55"/>
       <c r="G1" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>155</v>
-      </c>
       <c r="I1" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>27</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M1" s="52" t="s">
         <v>58</v>
@@ -3724,27 +4002,27 @@
       <c r="N1" s="48"/>
       <c r="O1" s="49"/>
       <c r="P1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R1" s="50"/>
       <c r="S1" s="51"/>
       <c r="T1" s="31"/>
       <c r="U1" s="47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="V1" s="50"/>
       <c r="W1" s="51"/>
       <c r="X1" s="44"/>
       <c r="Y1" s="47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Z1" s="50"/>
       <c r="AA1" s="51"/>
       <c r="AB1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC1" s="52" t="s">
         <v>42</v>
@@ -3789,10 +4067,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>19</v>
@@ -3801,25 +4079,25 @@
         <v>20</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="J3" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="K3" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="K3" s="46" t="s">
-        <v>102</v>
-      </c>
       <c r="L3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>61</v>
@@ -3828,10 +4106,10 @@
         <v>62</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="22" t="s">
         <v>61</v>
@@ -3840,10 +4118,10 @@
         <v>62</v>
       </c>
       <c r="S3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="T3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U3" s="22" t="s">
         <v>61</v>
@@ -3852,10 +4130,10 @@
         <v>62</v>
       </c>
       <c r="W3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y3" s="22" t="s">
         <v>61</v>
@@ -3864,10 +4142,10 @@
         <v>62</v>
       </c>
       <c r="AA3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AB3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC3" s="22" t="s">
         <v>61</v>
@@ -3876,18 +4154,18 @@
         <v>62</v>
       </c>
       <c r="AE3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>200</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
@@ -3896,65 +4174,65 @@
         <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N4" s="35" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="R4" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="Z4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AC4" s="2">
         <v>1</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4022,7 +4300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9364C085-89A2-4191-BD71-23274096DEBB}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4036,10 +4314,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="6"/>
     </row>
@@ -4057,14 +4335,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AFD6E7-296C-4D2D-8BB3-DCE2EA8A2647}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4077,7 +4357,8 @@
         <v>37</v>
       </c>
       <c r="B1" s="25">
-        <v>43502</v>
+        <f ca="1">TODAY()</f>
+        <v>43587</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4090,33 +4371,13 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
         <v>86</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FF42C4-E612-4A2B-8582-F0FFD086172F}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Filtrage du unité "non-jeune" dans les quotas de camp
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1379AB5D-05A9-4414-8DDC-D9CEA5CDC883}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E15DB37-F36F-4973-A6EA-1F865DECA3A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="690" windowWidth="21810" windowHeight="13680" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
-    <sheet name="Synthèse par unité" sheetId="3" r:id="rId2"/>
-    <sheet name="Quotas Année" sheetId="8" r:id="rId3"/>
-    <sheet name="Quotas Camps" sheetId="2" r:id="rId4"/>
-    <sheet name="Global" sheetId="9" r:id="rId5"/>
-    <sheet name="Général" sheetId="10" r:id="rId6"/>
-    <sheet name="Aide" sheetId="4" r:id="rId7"/>
+    <sheet name="Qualifications" sheetId="12" r:id="rId2"/>
+    <sheet name="Formations" sheetId="13" r:id="rId3"/>
+    <sheet name="Diplômes" sheetId="11" r:id="rId4"/>
+    <sheet name="Synthèse par unité" sheetId="3" r:id="rId5"/>
+    <sheet name="Quotas Année" sheetId="8" r:id="rId6"/>
+    <sheet name="Quotas Camps" sheetId="2" r:id="rId7"/>
+    <sheet name="Global" sheetId="9" r:id="rId8"/>
+    <sheet name="Général" sheetId="10" r:id="rId9"/>
+    <sheet name="Aide" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Quotas Année'!$A$3:$AC$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Quotas Camps'!$A$3:$AE$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$AZ$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Synthèse par unité'!$A$1:$AE$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Diplômes!$A$1:$L$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Formations!$A$1:$AA$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Qualifications!$A$1:$N$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Quotas Année'!$A$3:$AC$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quotas Camps'!$A$3:$AE$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$L$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Synthèse par unité'!$A$1:$AE$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +54,89 @@
     <author>Sébastien</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{46CD7ABF-224E-46F0-A443-9BFA12BC8FFF}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Age aujourd'hui</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Age au 1er juillet prochain</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sébastien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Age suivant la règle SGDF : 19 pour les LJ, SG et 21 ans pour les PK</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sébastien</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{905C7348-F4B2-4963-9D43-F692C6BCB07E}">
       <text>
         <r>
           <rPr>
@@ -72,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{E1578AE2-3E3D-4BF6-BDA1-0E6F28CF9A3F}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{A3B3A2F3-DC17-4DC7-94F8-B179C2728450}">
       <text>
         <r>
           <rPr>
@@ -96,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{85A87D93-DCFF-4024-A69F-EC8165F611A2}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{8B58F3BB-A36A-4A98-A40C-91AA8FD2F679}">
       <text>
         <r>
           <rPr>
@@ -120,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{C1BA196E-6BE0-448D-B5DF-539830267ED2}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{C24EDFC6-6157-43E5-833C-76817656A6CF}">
       <text>
         <r>
           <rPr>
@@ -144,7 +232,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{E61AC8E6-5369-486E-BB2A-CFC3F3BBFC62}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sébastien</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{60E4E0F6-7DF8-4A49-8516-9CA0D5538197}">
       <text>
         <r>
           <rPr>
@@ -168,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{BD73F079-BD47-4A9B-9DB9-888F403257F2}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{44FEFEDC-A3B6-4440-A607-CA059DB1D796}">
       <text>
         <r>
           <rPr>
@@ -192,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{4EEDDAC8-2343-467D-9346-63590EC6F6AE}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{1B3E1A7C-0680-43B6-A451-B9AD30B871AA}">
       <text>
         <r>
           <rPr>
@@ -216,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{6A99CB9E-35A8-4FA1-BC9B-4D96C495F872}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9CEDF5E2-D139-4510-A103-13F24DE204C2}">
       <text>
         <r>
           <rPr>
@@ -240,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{86FD4D1A-31E9-4CF5-B839-4DB3C6578C7B}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{2A55408E-B129-432E-95A2-3D62178E53C8}">
       <text>
         <r>
           <rPr>
@@ -264,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{D4CB2E41-2D86-492F-A896-A7F2621165D9}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{0DD2F092-25CF-43A2-8C2E-3982770EFBCF}">
       <text>
         <r>
           <rPr>
@@ -288,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{55CC420A-73E2-4858-9D36-083E75638385}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{AC82776C-F530-4190-B75F-397D22581B23}">
       <text>
         <r>
           <rPr>
@@ -312,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{E842F17D-4EA4-46A7-8AA9-D11373D8D411}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{EEC66E3F-8B4A-467C-8A5C-B64083AA3370}">
       <text>
         <r>
           <rPr>
@@ -336,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{83C77407-EDE7-4503-93FD-393628AE54E4}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{2D4538CE-D3F1-4FF9-ACD5-AAC67EC52826}">
       <text>
         <r>
           <rPr>
@@ -360,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{83CCAF6B-404B-4C1D-92E5-BE497427DD7D}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{E2F6D111-FFD2-44BA-9F41-49F796F2947E}">
       <text>
         <r>
           <rPr>
@@ -384,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{156BCBB7-1FAF-413C-8ECC-A4A9CA20E3FD}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{77306F0C-F710-4452-BAF6-5C1D346D28EC}">
       <text>
         <r>
           <rPr>
@@ -418,7 +516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{2C5F74EA-D518-4557-AC0F-8BFFC404907C}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{4466B097-0290-42E9-B624-B1A0AD9D1C42}">
       <text>
         <r>
           <rPr>
@@ -442,7 +540,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{6045E9B0-AA1D-41B4-9C3C-BC746D9BC589}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{957A0E74-9F8C-4A5B-9184-FE95E02D667F}">
       <text>
         <r>
           <rPr>
@@ -466,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{1F3E1ACB-E2A6-4A98-A36E-7ABE327D55F6}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{A20B21DD-1881-441A-A5A4-C77419ED7E93}">
       <text>
         <r>
           <rPr>
@@ -490,7 +588,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sébastien</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E72231DA-93D3-4418-B8D7-76AE634C1E08}">
       <text>
         <r>
           <rPr>
@@ -514,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{D775B390-A3E7-4B49-97AA-2086091F8E1A}">
       <text>
         <r>
           <rPr>
@@ -538,7 +646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{2F31B678-BEA5-4DB4-AC1D-AC1EC879D750}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{62B9A651-BDE7-475F-9529-41A0A2DFFE4C}">
       <text>
         <r>
           <rPr>
@@ -562,7 +670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{C8A48C2F-9EB4-4B10-8DBC-DE0A2B010CD5}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{D8956881-F0C9-4848-9228-EC603B219F1B}">
       <text>
         <r>
           <rPr>
@@ -586,7 +694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{CE08BEFE-EAC8-4844-983C-8BADEFBFE2C5}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{4FBAC0A5-B5E9-489B-BA35-16CC127A2F12}">
       <text>
         <r>
           <rPr>
@@ -610,7 +718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{28DEFE86-2BEB-4C19-99F9-9FC3C46725F3}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{5CE5F81E-8961-4DF0-9C77-4A9112F7205C}">
       <text>
         <r>
           <rPr>
@@ -634,7 +742,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{9189F978-0462-4031-826A-0220C3A0FBE8}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{E6AD01D7-75FD-456C-B7A9-382930AB949C}">
       <text>
         <r>
           <rPr>
@@ -655,78 +763,6 @@
           </rPr>
           <t xml:space="preserve">
 Date d'obtention</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Age aujourd'hui</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Age au 1er juillet prochain</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sébastien:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Age suivant la règle SGDF : 19 pour les LJ, SG et 21 ans pour les PK</t>
         </r>
       </text>
     </comment>
@@ -735,7 +771,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="201">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -938,9 +974,6 @@
     <t>Stagiaire BAFA potentiel</t>
   </si>
   <si>
-    <t>&lt;jt:if test="${chef.bafapotentiel}"&gt;Oui&lt;/jt:if&gt;</t>
-  </si>
-  <si>
     <t>Code Structure</t>
   </si>
   <si>
@@ -1008,9 +1041,6 @@
   </si>
   <si>
     <t>Titulaire ou stagiaire Dir ou anim</t>
-  </si>
-  <si>
-    <t>${chef.diplome.buchettes4.dateobtention}</t>
   </si>
   <si>
     <t>${chef.qualifs}</t>
@@ -1350,7 +1380,16 @@
     <t>${chef.formation.fif.datefin}</t>
   </si>
   <si>
-    <t>${chef.formation.fcf.datefin}</t>
+    <t>&lt;jt:if test="${chef.bafapotentiel}"&gt;Oui&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${chef.formation.fcf.datefin}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${chef.diplome.buchettes4.dateobtention}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${unites}" var="unite" orderBy="codestructure" where="${unite.nonPrincipal}" &gt;${unite.nom}</t>
   </si>
 </sst>
 </file>
@@ -2513,11 +2552,11 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2531,37 +2570,13 @@
     <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
     <col min="7" max="8" width="10.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="28" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="2.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="2.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="28" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" style="28" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" style="28" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="28" customWidth="1"/>
-    <col min="23" max="23" width="18" style="28" customWidth="1"/>
-    <col min="24" max="25" width="14.28515625" style="28" customWidth="1"/>
-    <col min="26" max="27" width="11.42578125" style="28" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" style="28" customWidth="1"/>
-    <col min="29" max="29" width="11.42578125" style="28" customWidth="1"/>
-    <col min="30" max="30" width="14.140625" style="28" customWidth="1"/>
-    <col min="31" max="32" width="13" style="28" customWidth="1"/>
-    <col min="33" max="37" width="11.42578125" style="28" customWidth="1"/>
-    <col min="38" max="38" width="17.5703125" style="28" customWidth="1"/>
-    <col min="39" max="39" width="15.28515625" style="28" customWidth="1"/>
-    <col min="40" max="40" width="12.5703125" style="28" customWidth="1"/>
-    <col min="41" max="41" width="3.140625" style="2" customWidth="1"/>
-    <col min="42" max="48" width="11.42578125" style="28" customWidth="1"/>
-    <col min="49" max="49" width="4" style="2" customWidth="1"/>
-    <col min="50" max="50" width="12.7109375" style="2" customWidth="1"/>
-    <col min="51" max="51" width="15" style="2" customWidth="1"/>
-    <col min="52" max="52" width="14.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2575,153 +2590,33 @@
         <v>18</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>54</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="U1" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="V1" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="W1" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="X1" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y1" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="Z1" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA1" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB1" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="AC1" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="AD1" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="AE1" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="AF1" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="AG1" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH1" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI1" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ1" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="AK1" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="AL1" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AM1" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN1" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP1" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ1" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="AR1" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="AS1" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="AT1" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="AU1" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV1" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="AW1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="AX1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="AY1" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AZ1" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2733,142 +2628,31 @@
         <v>56</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>64</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="W2" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y2" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="Z2" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC2" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD2" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE2" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF2" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="AG2" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH2" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI2" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ2" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK2" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="AL2" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM2" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="AN2" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ2" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR2" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS2" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT2" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU2" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV2" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>125</v>
+      <c r="I2" s="3"/>
+      <c r="J2" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2880,147 +2664,36 @@
         <v>56</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>64</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="T3" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="U3" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="V3" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="W3" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="X3" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y3" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="Z3" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA3" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB3" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC3" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD3" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE3" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF3" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="AG3" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH3" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI3" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ3" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK3" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="AL3" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM3" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="AN3" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="AO3" s="3"/>
-      <c r="AP3" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ3" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR3" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS3" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT3" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU3" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV3" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW3" s="3"/>
-      <c r="AX3" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AZ3" s="3" t="s">
-        <v>125</v>
+      <c r="I3" s="3"/>
+      <c r="J3" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AZ3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <conditionalFormatting sqref="AZ2:AZ65536">
+  <autoFilter ref="A1:L3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <conditionalFormatting sqref="L2:L65536">
     <cfRule type="cellIs" dxfId="40" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY2:AY65536">
+  <conditionalFormatting sqref="K2:K65536">
     <cfRule type="cellIs" dxfId="39" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -3095,7 +2768,611 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FF42C4-E612-4A2B-8582-F0FFD086172F}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E839BC-6F29-4F14-B58D-1E2088939687}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="9" width="11.42578125" style="28" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="2.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="21"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B21C5B7-5B9C-4DD6-AED7-1EA1BDB21D53}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="28" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="28" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="28" customWidth="1"/>
+    <col min="10" max="10" width="18" style="28" customWidth="1"/>
+    <col min="11" max="12" width="14.28515625" style="28" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" style="28" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="28" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="28" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="28" customWidth="1"/>
+    <col min="18" max="19" width="13" style="28" customWidth="1"/>
+    <col min="20" max="24" width="11.42578125" style="28" customWidth="1"/>
+    <col min="25" max="25" width="17.5703125" style="28" customWidth="1"/>
+    <col min="26" max="26" width="15.28515625" style="28" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y1" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z1" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA1" s="29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y2" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA2" s="28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="W3" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="X3" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y3" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z3" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA3" s="28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AA3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC055CEB-F8BF-4FEF-96B7-58AA4EBF5327}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" style="2" customWidth="1"/>
+    <col min="6" max="12" width="11.42578125" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626E417A-45EE-4D6C-95FD-A71D343FE19B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -3103,10 +3380,10 @@
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,12 +3391,12 @@
     <col min="1" max="1" width="75.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="2"/>
     <col min="6" max="7" width="8.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="2" customWidth="1"/>
     <col min="9" max="10" width="8.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="5" style="2" customWidth="1"/>
     <col min="13" max="13" width="5.5703125" style="2" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" style="2" customWidth="1"/>
@@ -3128,6 +3405,7 @@
     <col min="17" max="17" width="14.85546875" customWidth="1"/>
     <col min="18" max="18" width="17.28515625" customWidth="1"/>
     <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="20" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3135,13 +3413,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>19</v>
@@ -3153,7 +3431,7 @@
         <v>21</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>23</v>
@@ -3162,7 +3440,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L1" s="29" t="s">
         <v>8</v>
@@ -3174,22 +3452,22 @@
         <v>10</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q1" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="S1" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U1" s="19" t="s">
         <v>27</v>
@@ -3212,10 +3490,10 @@
         <v>63</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
@@ -3245,19 +3523,19 @@
         <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="2" t="s">
@@ -3296,7 +3574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86524C9-1323-498D-ABE2-77D2F4C73D5A}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -3307,7 +3585,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,15 +3600,15 @@
     <col min="8" max="8" width="9" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" style="2" customWidth="1"/>
     <col min="13" max="13" width="8.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="6.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="3.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" style="2" customWidth="1"/>
     <col min="16" max="16" width="11" style="2" customWidth="1"/>
     <col min="17" max="17" width="10.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="7.7109375" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" customWidth="1"/>
     <col min="22" max="22" width="8.42578125" customWidth="1"/>
     <col min="24" max="24" width="9" customWidth="1"/>
     <col min="25" max="25" width="15.85546875" customWidth="1"/>
@@ -3343,49 +3621,49 @@
       <c r="C1" s="8"/>
       <c r="E1" s="2"/>
       <c r="F1" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M1" s="48"/>
       <c r="N1" s="49"/>
       <c r="O1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P1" s="47" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="50"/>
       <c r="R1" s="51"/>
       <c r="S1" s="31"/>
       <c r="T1" s="47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="U1" s="50"/>
       <c r="V1" s="51"/>
       <c r="W1" s="50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="X1" s="50"/>
       <c r="Y1" s="51"/>
       <c r="Z1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA1" s="52" t="s">
         <v>42</v>
@@ -3423,33 +3701,33 @@
     </row>
     <row r="3" spans="1:29" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>102</v>
-      </c>
       <c r="K3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L3" s="43" t="s">
         <v>61</v>
@@ -3458,10 +3736,10 @@
         <v>62</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P3" s="43" t="s">
         <v>61</v>
@@ -3470,10 +3748,10 @@
         <v>62</v>
       </c>
       <c r="R3" s="43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T3" s="43" t="s">
         <v>61</v>
@@ -3482,7 +3760,7 @@
         <v>62</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="W3" s="34" t="s">
         <v>61</v>
@@ -3491,10 +3769,10 @@
         <v>62</v>
       </c>
       <c r="Y3" s="32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Z3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA3" s="43" t="s">
         <v>61</v>
@@ -3503,12 +3781,12 @@
         <v>62</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
@@ -3518,67 +3796,67 @@
         <v>57</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2">
         <v>1</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
@@ -3645,7 +3923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64634AA-9071-4111-8E53-9AF735BF36D3}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -3666,29 +3944,29 @@
     <col min="3" max="3" width="17.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" style="2" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="35" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.42578125" style="35" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" style="2" customWidth="1"/>
     <col min="19" max="19" width="7.85546875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" customWidth="1"/>
     <col min="21" max="21" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.140625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="4.85546875" customWidth="1"/>
+    <col min="24" max="24" width="2.85546875" customWidth="1"/>
     <col min="25" max="25" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.5703125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" customWidth="1"/>
+    <col min="28" max="28" width="2.85546875" customWidth="1"/>
     <col min="29" max="29" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -3701,22 +3979,22 @@
       <c r="D1" s="54"/>
       <c r="E1" s="55"/>
       <c r="G1" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>155</v>
-      </c>
       <c r="I1" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>27</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M1" s="52" t="s">
         <v>58</v>
@@ -3724,27 +4002,27 @@
       <c r="N1" s="48"/>
       <c r="O1" s="49"/>
       <c r="P1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R1" s="50"/>
       <c r="S1" s="51"/>
       <c r="T1" s="31"/>
       <c r="U1" s="47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="V1" s="50"/>
       <c r="W1" s="51"/>
       <c r="X1" s="44"/>
       <c r="Y1" s="47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Z1" s="50"/>
       <c r="AA1" s="51"/>
       <c r="AB1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC1" s="52" t="s">
         <v>42</v>
@@ -3789,10 +4067,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>19</v>
@@ -3801,25 +4079,25 @@
         <v>20</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="J3" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="K3" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="K3" s="46" t="s">
-        <v>102</v>
-      </c>
       <c r="L3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>61</v>
@@ -3828,10 +4106,10 @@
         <v>62</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="22" t="s">
         <v>61</v>
@@ -3840,10 +4118,10 @@
         <v>62</v>
       </c>
       <c r="S3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="T3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U3" s="22" t="s">
         <v>61</v>
@@ -3852,10 +4130,10 @@
         <v>62</v>
       </c>
       <c r="W3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="X3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y3" s="22" t="s">
         <v>61</v>
@@ -3864,10 +4142,10 @@
         <v>62</v>
       </c>
       <c r="AA3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AB3" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC3" s="22" t="s">
         <v>61</v>
@@ -3876,18 +4154,18 @@
         <v>62</v>
       </c>
       <c r="AE3" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>200</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
@@ -3896,65 +4174,65 @@
         <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N4" s="35" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="R4" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="Z4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AC4" s="2">
         <v>1</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4022,7 +4300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9364C085-89A2-4191-BD71-23274096DEBB}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4036,10 +4314,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="6"/>
     </row>
@@ -4057,14 +4335,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AFD6E7-296C-4D2D-8BB3-DCE2EA8A2647}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4077,7 +4357,8 @@
         <v>37</v>
       </c>
       <c r="B1" s="25">
-        <v>43502</v>
+        <f ca="1">TODAY()</f>
+        <v>43587</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4090,33 +4371,13 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
         <v>86</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FF42C4-E612-4A2B-8582-F0FFD086172F}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout d'une colonne Code de branche pour faciliter le filtrage
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337777E5-C3F3-4726-A360-0E7C17D1CA11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF2F5D3-69C6-4C55-9994-10212268C51A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
@@ -29,11 +29,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Formations!$A$1:$AA$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Qualifications!$A$1:$N$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Quotas Année'!$A$3:$AC$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quotas Camps'!$A$3:$AE$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quotas Camps'!$A$3:$AF$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Responsables!$A$1:$L$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Synthèse par unité'!$A$1:$AE$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,6 +41,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -770,7 +771,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="203">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -1074,12 +1075,6 @@
   </si>
   <si>
     <t>Delta5</t>
-  </si>
-  <si>
-    <t>$[Z4-Y4]</t>
-  </si>
-  <si>
-    <t>$[R4-Q4]</t>
   </si>
   <si>
     <t>$[E4]</t>
@@ -1178,12 +1173,6 @@
   </si>
   <si>
     <t>Delta1</t>
-  </si>
-  <si>
-    <t>$[N4-M4]</t>
-  </si>
-  <si>
-    <t>$[AD4-AC4]&lt;/jt:forEach&gt;</t>
   </si>
   <si>
     <t>Y a-t-il un directeur titulaire ou stagiaire ?</t>
@@ -1206,21 +1195,6 @@
 1 dir titulaire ou stagiaire hors compagnons</t>
   </si>
   <si>
-    <t>$[O4]</t>
-  </si>
-  <si>
-    <t>$[S4]</t>
-  </si>
-  <si>
-    <t>$[W4]</t>
-  </si>
-  <si>
-    <t>$[AA4]</t>
-  </si>
-  <si>
-    <t>$[AE4]</t>
-  </si>
-  <si>
     <t>$[IF($B4=$C4,0,IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=4,0,1))]</t>
   </si>
   <si>
@@ -1234,20 +1208,6 @@
   </si>
   <si>
     <t>Y a-t-il un directeur titulaire ?</t>
-  </si>
-  <si>
-    <t>Nb  titulaires ou stagiaires et 1 dir (sauf rouge)</t>
-  </si>
-  <si>
-    <t>Nb animateurs et 1 dir (sauf rouge)</t>
-  </si>
-  <si>
-    <t>Nb titulaires et 1 dir (sauf rouge)</t>
-  </si>
-  <si>
-    <t>Encadrement 2ème étape
-par rapport au minimum de animateurs : 
-50% titulaire + 1 dir titulaire (sauf rouge)</t>
   </si>
   <si>
     <t>Encadrement 1ère étape
@@ -1256,139 +1216,186 @@
 (sauf unité rouge)</t>
   </si>
   <si>
+    <t xml:space="preserve">APPRO ANIM </t>
+  </si>
+  <si>
+    <t>${chef.formation.appro_anim.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.appro_accueil.datefin}</t>
+  </si>
+  <si>
+    <t>APPRO ANIM</t>
+  </si>
+  <si>
+    <t>${unite.appro_anim}</t>
+  </si>
+  <si>
+    <t>${unite.appro_accueil}</t>
+  </si>
+  <si>
+    <t>${chef.formation.module_appro_accueil_scoutisme.datefin}</t>
+  </si>
+  <si>
+    <t>MODULE APPRO ACCUEIL DE SCOUTISME</t>
+  </si>
+  <si>
+    <t>${chef.formation.module_animateur_scoutisme_campisme.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.module_appro_surveillant_baignade.datefin}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MODULE ANIMATEUR DE SCOUTISME ET CAMPISME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPRO SURVEILLANT DE BAIGNADE </t>
+  </si>
+  <si>
+    <t>${unite.module_appro_accueil_scoutisme}</t>
+  </si>
+  <si>
+    <t>${unite.module_animateur_scoutisme_campisme}</t>
+  </si>
+  <si>
+    <t>${unite.module_appro_surveillant_baignade}</t>
+  </si>
+  <si>
+    <t>APPRO ACCUEIL DE SCOUTISME</t>
+  </si>
+  <si>
+    <t>BAFA FORMATION GÉNÉRALE</t>
+  </si>
+  <si>
+    <t>BAFD FORMATION GÉNÉRALE</t>
+  </si>
+  <si>
+    <t>APF CHEFS-CHEFTAINES</t>
+  </si>
+  <si>
+    <t>APF RESPONSABLES de GROUPE</t>
+  </si>
+  <si>
+    <t>AIDE A LA PRISE DE FONCTION</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_chefs.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_rg.datefin}</t>
+  </si>
+  <si>
+    <t>APF SECRETAIRE TRESORIER</t>
+  </si>
+  <si>
+    <t>APF AUMONIER ET AVSC</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_sp.datefin}</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_aavsc.datefin}</t>
+  </si>
+  <si>
+    <t>APF RESPONSABLE LOCAL DEVELOPPEMENT ET RESEAUX</t>
+  </si>
+  <si>
+    <t>${chef.formation.apf_rldr.datefin}</t>
+  </si>
+  <si>
+    <t>FORMATION ACCUEIL DE SCOUTISME RG</t>
+  </si>
+  <si>
+    <t>${chef.formation.accueil_scoutisme_rg.datefin}</t>
+  </si>
+  <si>
+    <t>Fonction secondaire</t>
+  </si>
+  <si>
+    <t>${chef.fonctionsecondairecomplet}</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${chef.qualif.dirsf.aetaetetitulaire}" onProcessed="org.leplan73.outilssgdf.outils.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>FORMATION INITIALE DE FORMATEURS</t>
+  </si>
+  <si>
+    <t>FORMATION CONTINUE DE FORMATEURS</t>
+  </si>
+  <si>
+    <t>${chef.formation.fif.datefin}</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${chef.bafapotentiel}"&gt;Oui&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${chef.formation.fcf.datefin}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${chef.diplome.buchettes4.dateobtention}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${unites}" var="unite" orderBy="codestructure" where="${unite.nonPrincipal}" &gt;${unite.nom}</t>
+  </si>
+  <si>
+    <t>Code Branche</t>
+  </si>
+  <si>
+    <t>${unite.codebranche}</t>
+  </si>
+  <si>
+    <t>$[P4]</t>
+  </si>
+  <si>
+    <t>$[T4]</t>
+  </si>
+  <si>
+    <t>$[X4]</t>
+  </si>
+  <si>
+    <t>$[AB4]</t>
+  </si>
+  <si>
+    <t>$[AF4]</t>
+  </si>
+  <si>
+    <t>$[O4-N4]</t>
+  </si>
+  <si>
+    <t>$[S4-R4]</t>
+  </si>
+  <si>
+    <t>$[W4-V4]</t>
+  </si>
+  <si>
+    <t>$[AA4-Z4]</t>
+  </si>
+  <si>
+    <t>$[AE4-AD4]&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>Nb animateurs et 1 dir (sauf unité rouge)</t>
+  </si>
+  <si>
+    <t>Nb titulaires et 1 dir (sauf unité rouge)</t>
+  </si>
+  <si>
+    <t>Nb  titulaires ou stagiaires et 1 dir (sauf unité rouge)</t>
+  </si>
+  <si>
+    <t>Encadrement 2ème étape
+par rapport au minimum de animateurs : 
+50% titulaire + 1 dir titulaire (sauf unité rouge)</t>
+  </si>
+  <si>
     <t>Encadrement 2ème étape
 par rapport au minimum d'animateurs : 
 80% titulaire ou stagiaire +
-1 dir titulaire (sauf rouge)</t>
-  </si>
-  <si>
-    <t>$[V4-U4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPRO ANIM </t>
-  </si>
-  <si>
-    <t>${chef.formation.appro_anim.datefin}</t>
-  </si>
-  <si>
-    <t>${chef.formation.appro_accueil.datefin}</t>
-  </si>
-  <si>
-    <t>APPRO ANIM</t>
-  </si>
-  <si>
-    <t>${unite.appro_anim}</t>
-  </si>
-  <si>
-    <t>${unite.appro_accueil}</t>
-  </si>
-  <si>
-    <t>${chef.formation.module_appro_accueil_scoutisme.datefin}</t>
-  </si>
-  <si>
-    <t>MODULE APPRO ACCUEIL DE SCOUTISME</t>
-  </si>
-  <si>
-    <t>${chef.formation.module_animateur_scoutisme_campisme.datefin}</t>
-  </si>
-  <si>
-    <t>${chef.formation.module_appro_surveillant_baignade.datefin}</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MODULE ANIMATEUR DE SCOUTISME ET CAMPISME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPRO SURVEILLANT DE BAIGNADE </t>
-  </si>
-  <si>
-    <t>${unite.module_appro_accueil_scoutisme}</t>
-  </si>
-  <si>
-    <t>${unite.module_animateur_scoutisme_campisme}</t>
-  </si>
-  <si>
-    <t>${unite.module_appro_surveillant_baignade}</t>
-  </si>
-  <si>
-    <t>APPRO ACCUEIL DE SCOUTISME</t>
-  </si>
-  <si>
-    <t>BAFA FORMATION GÉNÉRALE</t>
-  </si>
-  <si>
-    <t>BAFD FORMATION GÉNÉRALE</t>
-  </si>
-  <si>
-    <t>APF CHEFS-CHEFTAINES</t>
-  </si>
-  <si>
-    <t>APF RESPONSABLES de GROUPE</t>
-  </si>
-  <si>
-    <t>AIDE A LA PRISE DE FONCTION</t>
-  </si>
-  <si>
-    <t>${chef.formation.apf.datefin}</t>
-  </si>
-  <si>
-    <t>${chef.formation.apf_chefs.datefin}</t>
-  </si>
-  <si>
-    <t>${chef.formation.apf_rg.datefin}</t>
-  </si>
-  <si>
-    <t>APF SECRETAIRE TRESORIER</t>
-  </si>
-  <si>
-    <t>APF AUMONIER ET AVSC</t>
-  </si>
-  <si>
-    <t>${chef.formation.apf_sp.datefin}</t>
-  </si>
-  <si>
-    <t>${chef.formation.apf_aavsc.datefin}</t>
-  </si>
-  <si>
-    <t>APF RESPONSABLE LOCAL DEVELOPPEMENT ET RESEAUX</t>
-  </si>
-  <si>
-    <t>${chef.formation.apf_rldr.datefin}</t>
-  </si>
-  <si>
-    <t>FORMATION ACCUEIL DE SCOUTISME RG</t>
-  </si>
-  <si>
-    <t>${chef.formation.accueil_scoutisme_rg.datefin}</t>
-  </si>
-  <si>
-    <t>Fonction secondaire</t>
-  </si>
-  <si>
-    <t>${chef.fonctionsecondairecomplet}</t>
-  </si>
-  <si>
-    <t>&lt;jt:if test="${chef.qualif.dirsf.aetaetetitulaire}" onProcessed="org.leplan73.outilssgdf.outils.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
-  </si>
-  <si>
-    <t>FORMATION INITIALE DE FORMATEURS</t>
-  </si>
-  <si>
-    <t>FORMATION CONTINUE DE FORMATEURS</t>
-  </si>
-  <si>
-    <t>${chef.formation.fif.datefin}</t>
-  </si>
-  <si>
-    <t>&lt;jt:if test="${chef.bafapotentiel}"&gt;Oui&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
-    <t>${chef.formation.fcf.datefin}&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
-    <t>${chef.diplome.buchettes4.dateobtention}&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
-    <t>&lt;jt:forEach items="${unites}" var="unite" orderBy="codestructure" where="${unite.nonPrincipal}" &gt;${unite.nom}</t>
+1 dir titulaire (sauf unité rouge)</t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1641,6 +1648,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1649,7 +1700,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1714,9 +1765,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1783,6 +1831,30 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1800,15 +1872,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2245,12 +2308,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Sébastien Bouchex" id="{D2D877DA-17D9-4BDD-B14D-4E2D1B208222}" userId="S::sbouchex@infovista.com::4b272613-d5ab-4e32-92d1-b65864253ecd" providerId="AD"/>
-</personList>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -2558,22 +2615,22 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.26953125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="2.81640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="15" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2596,7 +2653,7 @@
         <v>54</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="I1" s="21" t="s">
         <v>75</v>
@@ -2611,7 +2668,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>80</v>
       </c>
@@ -2634,20 +2691,20 @@
         <v>64</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>73</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>87</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
@@ -2670,17 +2727,17 @@
         <v>64</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="25" t="s">
         <v>73</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>87</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2774,10 +2831,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.453125" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2796,25 +2853,25 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" customWidth="1"/>
-    <col min="6" max="9" width="11.453125" style="28" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="17.7265625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="2.54296875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14.7265625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="2.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="9" width="11.42578125" style="27" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="2.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2830,16 +2887,16 @@
       <c r="E1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="26" t="s">
         <v>79</v>
       </c>
       <c r="J1" s="16" t="s">
@@ -2856,7 +2913,7 @@
       </c>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>80</v>
       </c>
@@ -2869,16 +2926,16 @@
       <c r="D2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>60</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -2889,11 +2946,11 @@
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
@@ -2906,16 +2963,16 @@
       <c r="D3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="G3" s="28" t="s">
+      <c r="F3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="27" t="s">
         <v>60</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -2926,7 +2983,7 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="N3" s="3"/>
     </row>
@@ -2952,31 +3009,31 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="28" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" style="28" customWidth="1"/>
-    <col min="8" max="8" width="14.26953125" style="28" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="28" customWidth="1"/>
-    <col min="10" max="10" width="18" style="28" customWidth="1"/>
-    <col min="11" max="12" width="14.26953125" style="28" customWidth="1"/>
-    <col min="13" max="14" width="11.453125" style="28" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" style="28" customWidth="1"/>
-    <col min="16" max="16" width="11.453125" style="28" customWidth="1"/>
-    <col min="17" max="17" width="14.1796875" style="28" customWidth="1"/>
-    <col min="18" max="19" width="13" style="28" customWidth="1"/>
-    <col min="20" max="24" width="11.453125" style="28" customWidth="1"/>
-    <col min="25" max="25" width="18.1796875" style="28" customWidth="1"/>
-    <col min="26" max="26" width="15.26953125" style="28" customWidth="1"/>
-    <col min="27" max="27" width="12.54296875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="27" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="27" customWidth="1"/>
+    <col min="10" max="10" width="18" style="27" customWidth="1"/>
+    <col min="11" max="12" width="14.28515625" style="27" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" style="27" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="27" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="27" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="27" customWidth="1"/>
+    <col min="18" max="19" width="13" style="27" customWidth="1"/>
+    <col min="20" max="24" width="11.42578125" style="27" customWidth="1"/>
+    <col min="25" max="25" width="18.140625" style="27" customWidth="1"/>
+    <col min="26" max="26" width="15.28515625" style="27" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="20" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" s="20" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2992,74 +3049,74 @@
       <c r="E1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z1" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>187</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="P1" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="W1" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="X1" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="Y1" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z1" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="AA1" s="29" t="s">
-        <v>195</v>
+      <c r="AA1" s="28" t="s">
+        <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>80</v>
       </c>
@@ -3072,74 +3129,74 @@
       <c r="D2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="S2" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="T2" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="W2" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="X2" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y2" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z2" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="P2" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q2" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="R2" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="S2" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="W2" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y2" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z2" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA2" s="28" t="s">
-        <v>198</v>
+      <c r="AA2" s="27" t="s">
+        <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
@@ -3152,71 +3209,71 @@
       <c r="D3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="G3" s="28" t="s">
+      <c r="F3" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="P3" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q3" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="R3" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="S3" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="T3" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="W3" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="X3" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y3" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z3" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="I3" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="L3" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="M3" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="P3" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q3" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="R3" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="S3" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="T3" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="U3" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="W3" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="X3" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y3" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z3" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA3" s="28" t="s">
-        <v>198</v>
+      <c r="AA3" s="27" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3241,17 +3298,17 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" style="2" customWidth="1"/>
-    <col min="6" max="12" width="11.453125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" style="2" customWidth="1"/>
+    <col min="6" max="12" width="11.42578125" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -3267,29 +3324,29 @@
       <c r="E1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>80</v>
       </c>
@@ -3303,29 +3360,29 @@
         <v>56</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="28" t="s">
-        <v>199</v>
+      <c r="L2" s="27" t="s">
+        <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
@@ -3339,26 +3396,26 @@
         <v>56</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="28" t="s">
-        <v>199</v>
+      <c r="L3" s="27" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3383,29 +3440,29 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.26953125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="2.81640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="2"/>
-    <col min="6" max="7" width="8.81640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.81640625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="8.81640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="2.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="75.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2"/>
+    <col min="6" max="7" width="8.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="5.54296875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.81640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.453125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" customWidth="1"/>
-    <col min="18" max="18" width="17.26953125" customWidth="1"/>
-    <col min="19" max="19" width="12.7265625" customWidth="1"/>
-    <col min="20" max="20" width="2.81640625" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="20" customFormat="1" ht="46.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" s="20" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
@@ -3439,7 +3496,7 @@
       <c r="K1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="28" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="18" t="s">
@@ -3449,19 +3506,19 @@
         <v>10</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>170</v>
+        <v>147</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>155</v>
       </c>
       <c r="T1" s="21" t="s">
         <v>75</v>
@@ -3482,7 +3539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>63</v>
       </c>
@@ -3520,19 +3577,19 @@
         <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="2" t="s">
@@ -3557,11 +3614,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="R4" s="1"/>
     </row>
   </sheetData>
@@ -3585,49 +3642,49 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.26953125" customWidth="1"/>
-    <col min="2" max="2" width="3.453125" customWidth="1"/>
+    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
     <col min="3" max="3" width="3" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="11" style="2" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.26953125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="2.81640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.1796875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.81640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="2.81640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" style="2" customWidth="1"/>
     <col min="16" max="16" width="11" style="2" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="7.7265625" customWidth="1"/>
-    <col min="19" max="19" width="2.81640625" customWidth="1"/>
-    <col min="22" max="22" width="8.453125" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" customWidth="1"/>
     <col min="24" max="24" width="9" customWidth="1"/>
-    <col min="25" max="25" width="15.81640625" customWidth="1"/>
-    <col min="26" max="26" width="3.1796875" customWidth="1"/>
-    <col min="28" max="28" width="10.1796875" customWidth="1"/>
-    <col min="29" max="29" width="9.26953125" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" customWidth="1"/>
+    <col min="26" max="26" width="3.140625" customWidth="1"/>
+    <col min="28" max="28" width="10.140625" customWidth="1"/>
+    <col min="29" max="29" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="8"/>
       <c r="E1" s="2"/>
       <c r="F1" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>27</v>
@@ -3635,68 +3692,68 @@
       <c r="K1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="48"/>
-      <c r="N1" s="49"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="56"/>
       <c r="O1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="U1" s="50"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="50" t="s">
-        <v>141</v>
-      </c>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="51"/>
+      <c r="P1" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="U1" s="57"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="58"/>
       <c r="Z1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="52" t="s">
+      <c r="AA1" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="49"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="56"/>
     </row>
-    <row r="2" spans="1:29" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:29" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="8"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="42"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="41"/>
       <c r="K2" s="21"/>
-      <c r="L2" s="37"/>
+      <c r="L2" s="36"/>
       <c r="M2" s="10"/>
-      <c r="N2" s="40"/>
+      <c r="N2" s="39"/>
       <c r="O2" s="21"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="38"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="21"/>
-      <c r="AA2" s="39"/>
+      <c r="AA2" s="38"/>
       <c r="AB2" s="10"/>
-      <c r="AC2" s="40"/>
+      <c r="AC2" s="39"/>
     </row>
-    <row r="3" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:29" s="32" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>72</v>
       </c>
@@ -3709,7 +3766,7 @@
         <v>95</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>97</v>
@@ -3726,64 +3783,64 @@
       <c r="K3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="42" t="s">
         <v>96</v>
       </c>
       <c r="O3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="R3" s="43" t="s">
+      <c r="R3" s="42" t="s">
         <v>96</v>
       </c>
       <c r="S3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="T3" s="43" t="s">
+      <c r="T3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="U3" s="43" t="s">
+      <c r="U3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="V3" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="W3" s="34" t="s">
+      <c r="W3" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="X3" s="43" t="s">
+      <c r="X3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="Y3" s="32" t="s">
+      <c r="Y3" s="31" t="s">
         <v>96</v>
       </c>
       <c r="Z3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="AA3" s="43" t="s">
+      <c r="AA3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="AB3" s="43" t="s">
+      <c r="AB3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="AC3" s="43" t="s">
+      <c r="AC3" s="42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
@@ -3793,70 +3850,70 @@
         <v>57</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2">
         <v>1</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C5" s="8"/>
       <c r="E5" s="2"/>
       <c r="F5"/>
@@ -3925,238 +3982,247 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:E1"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="2.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="7.54296875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="2.81640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="35" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.81640625" customWidth="1"/>
-    <col min="17" max="17" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" style="2" customWidth="1"/>
-    <col min="19" max="19" width="7.81640625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="2.81640625" customWidth="1"/>
-    <col min="21" max="21" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.1796875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="2.81640625" customWidth="1"/>
-    <col min="25" max="25" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.54296875" style="2" customWidth="1"/>
-    <col min="28" max="28" width="2.81640625" customWidth="1"/>
-    <col min="29" max="29" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" style="2" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="2.85546875" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="2.85546875" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="2.85546875" customWidth="1"/>
+    <col min="30" max="30" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="53"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55"/>
-      <c r="G1" s="15" t="s">
-        <v>151</v>
+    <row r="1" spans="1:32" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="N1" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="48"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="21" t="s">
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="R1" s="50"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="V1" s="50"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="21" t="s">
+      <c r="R1" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" s="57"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="W1" s="57"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="54" t="s">
+        <v>202</v>
+      </c>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="AC1" s="52" t="s">
+      <c r="AD1" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="49"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="56"/>
     </row>
-    <row r="2" spans="1:31" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="41"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="42"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="40"/>
+    <row r="2" spans="1:32" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="39"/>
     </row>
-    <row r="3" spans="1:31" s="20" customFormat="1" ht="12.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:32" s="20" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="47" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="G3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="H3" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="I3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="J3" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="K3" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="L3" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="M3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="N3" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="O3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="P3" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="P3" s="45" t="s">
+      <c r="Q3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="R3" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="S3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="S3" s="22" t="s">
+      <c r="T3" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="T3" s="45" t="s">
+      <c r="U3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="V3" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="W3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="W3" s="22" t="s">
+      <c r="X3" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="X3" s="45" t="s">
+      <c r="Y3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="Y3" s="22" t="s">
+      <c r="Z3" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="Z3" s="22" t="s">
+      <c r="AA3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="22" t="s">
+      <c r="AB3" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="AB3" s="45" t="s">
+      <c r="AC3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AC3" s="22" t="s">
+      <c r="AD3" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AD3" s="22" t="s">
+      <c r="AE3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AE3" s="22" t="s">
+      <c r="AF3" s="22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>83</v>
@@ -4165,129 +4231,131 @@
         <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="N4" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="O4" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="R4" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>149</v>
+      <c r="P4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="S4" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>150</v>
+        <v>116</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC4" s="2">
+        <v>117</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD4" s="2">
         <v>1</v>
       </c>
-      <c r="AD4" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="AE4" s="2" t="s">
-        <v>136</v>
+        <v>105</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AE3" xr:uid="{F1DE6F8D-B184-4B95-A70D-9A818A97D85F}"/>
-  <mergeCells count="6">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="Q1:S1"/>
+  <autoFilter ref="A3:AF3" xr:uid="{F1DE6F8D-B184-4B95-A70D-9A818A97D85F}"/>
+  <mergeCells count="5">
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="R1:T1"/>
   </mergeCells>
-  <conditionalFormatting sqref="O4:O65537">
+  <conditionalFormatting sqref="P4:P65537">
     <cfRule type="cellIs" dxfId="9" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4:S65537">
+  <conditionalFormatting sqref="T4:T65537">
     <cfRule type="cellIs" dxfId="8" priority="13" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W4:W65537">
+  <conditionalFormatting sqref="X4:X65537">
     <cfRule type="cellIs" dxfId="7" priority="12" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA4:AA65537">
+  <conditionalFormatting sqref="AB4:AB65537">
     <cfRule type="cellIs" dxfId="6" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE4:AE65537">
+  <conditionalFormatting sqref="AF4:AF65537">
     <cfRule type="cellIs" dxfId="5" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G65537">
+  <conditionalFormatting sqref="H4:H65537">
     <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H65537">
+  <conditionalFormatting sqref="I4:I65537">
     <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I65537">
+  <conditionalFormatting sqref="J4:J65537">
     <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4:J65537">
+  <conditionalFormatting sqref="K4:K65537">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K65537">
+  <conditionalFormatting sqref="L4:L65537">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4303,13 +4371,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>72</v>
       </c>
@@ -4318,7 +4386,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>40</v>
       </c>
@@ -4343,22 +4411,22 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="24">
         <f ca="1">TODAY()</f>
-        <v>43594</v>
+        <v>43604</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
@@ -4366,7 +4434,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
bug sur le quota à l'année
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D67BA9-DB9E-4FCC-AB59-295AF9CE7B3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F9EA73-6F1D-4AF9-B274-3AF452161B2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="630" windowWidth="25410" windowHeight="14790" tabRatio="677" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="990" yWindow="1245" windowWidth="27150" windowHeight="14160" tabRatio="677" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Synthèse par unité'!$A$1:$Y$1</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1382,7 +1383,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="215">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -1759,9 +1760,6 @@
     <t>$[X4-W4]</t>
   </si>
   <si>
-    <t>$[AB4-AA4]&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
-  </si>
-  <si>
     <t>$[N4]</t>
   </si>
   <si>
@@ -1781,12 +1779,6 @@
   </si>
   <si>
     <t>Y a-t-il un directeur titulaire ou stagiaire ?</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${unites}" aggs="Sum(jeunes);Sum(chefs);Sum(qualifieannee);Sum(stagiairesf);Sum(psc1afps);Sum(toutsf)" valuesVar="results" groupBy="codegroupe"&gt;&lt;jt:forEach items="${results}" var="unite"&gt;${unite.object.nom}</t>
-  </si>
-  <si>
-    <t>${unite.object.dirsfqnonq}</t>
   </si>
   <si>
     <t>Encadrement 2ème étape
@@ -2037,6 +2029,21 @@
   </si>
   <si>
     <t>${chef.formation.fc2.datefin}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${unites}" aggs="Sum(jeunes);Sum(chefs);Sum(qualifieannee);Sum(stagiairesf);Sum(psc1afps);Sum(toutsf);Sum(dirsfqnonq)" valuesVar="results" groupBy="codegroupe"&gt;&lt;jt:forEach items="${results}" var="unite"&gt;${unite.object.nom}</t>
+  </si>
+  <si>
+    <t>${unite.getAggregateValue(aggs[6])}</t>
+  </si>
+  <si>
+    <t>$[AB4-AA4]</t>
+  </si>
+  <si>
+    <t>&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
+  </si>
+  <si>
+    <t>$[MIN(AE4,1)]</t>
   </si>
 </sst>
 </file>
@@ -2512,32 +2519,32 @@
     <xf numFmtId="14" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="14" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3341,16 +3348,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="63"/>
+      <c r="A1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="61"/>
       <c r="J1" s="54" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K1" s="55"/>
       <c r="L1" s="55"/>
@@ -3358,44 +3365,44 @@
       <c r="N1" s="55"/>
       <c r="O1" s="56"/>
       <c r="Q1" s="17"/>
-      <c r="S1" s="57" t="s">
-        <v>203</v>
-      </c>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="58"/>
-      <c r="AE1" s="58"/>
-      <c r="AF1" s="58"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="58"/>
-      <c r="AI1" s="58"/>
-      <c r="AJ1" s="58"/>
-      <c r="AK1" s="58"/>
-      <c r="AL1" s="58"/>
-      <c r="AM1" s="58"/>
-      <c r="AN1" s="58"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="58"/>
-      <c r="AR1" s="59" t="s">
-        <v>204</v>
-      </c>
-      <c r="AS1" s="60"/>
-      <c r="AT1" s="60"/>
-      <c r="AU1" s="60"/>
-      <c r="AV1" s="60"/>
-      <c r="AW1" s="60"/>
-      <c r="AX1" s="60"/>
-      <c r="AZ1" s="64"/>
-      <c r="BA1" s="65"/>
-      <c r="BB1" s="65"/>
+      <c r="S1" s="64" t="s">
+        <v>200</v>
+      </c>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AR1" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS1" s="58"/>
+      <c r="AT1" s="58"/>
+      <c r="AU1" s="58"/>
+      <c r="AV1" s="58"/>
+      <c r="AW1" s="58"/>
+      <c r="AX1" s="58"/>
+      <c r="AZ1" s="62"/>
+      <c r="BA1" s="63"/>
+      <c r="BB1" s="63"/>
     </row>
     <row r="2" spans="1:54" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -3420,7 +3427,7 @@
         <v>52</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>73</v>
@@ -3453,25 +3460,25 @@
         <v>73</v>
       </c>
       <c r="S2" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="T2" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="U2" s="28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="V2" s="28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="W2" s="28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="X2" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Y2" s="28" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="Z2" s="28" t="s">
         <v>8</v>
@@ -3480,19 +3487,19 @@
         <v>9</v>
       </c>
       <c r="AB2" s="28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AC2" s="28" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AD2" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE2" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="AE2" s="28" t="s">
-        <v>149</v>
-      </c>
       <c r="AF2" s="28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AG2" s="28" t="s">
         <v>10</v>
@@ -3504,25 +3511,25 @@
         <v>108</v>
       </c>
       <c r="AJ2" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AK2" s="28" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AL2" s="28" t="s">
         <v>109</v>
       </c>
       <c r="AM2" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AN2" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AO2" s="28" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AP2" s="28" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AQ2" s="21" t="s">
         <v>73</v>
@@ -3584,11 +3591,11 @@
         <v>62</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K3" s="27" t="s">
         <v>68</v>
@@ -3607,28 +3614,28 @@
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="S3" s="27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="T3" s="27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="U3" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="V3" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="V3" s="27" t="s">
+      <c r="W3" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="W3" s="27" t="s">
-        <v>168</v>
-      </c>
       <c r="X3" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="Y3" s="27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="Z3" s="27" t="s">
         <v>42</v>
@@ -3637,19 +3644,19 @@
         <v>43</v>
       </c>
       <c r="AB3" s="27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AC3" s="27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AD3" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE3" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF3" s="27" t="s">
         <v>145</v>
-      </c>
-      <c r="AE3" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="AF3" s="27" t="s">
-        <v>148</v>
       </c>
       <c r="AG3" s="27" t="s">
         <v>44</v>
@@ -3670,16 +3677,16 @@
         <v>113</v>
       </c>
       <c r="AM3" s="27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN3" s="27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AO3" s="27" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AP3" s="27" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AQ3" s="3"/>
       <c r="AR3" s="27" t="s">
@@ -3701,7 +3708,7 @@
         <v>50</v>
       </c>
       <c r="AX3" s="27" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AY3" s="3"/>
       <c r="AZ3" s="25" t="s">
@@ -3737,11 +3744,11 @@
         <v>62</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K4" s="27" t="s">
         <v>68</v>
@@ -3760,28 +3767,28 @@
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="S4" s="27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="T4" s="27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="U4" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="V4" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="V4" s="27" t="s">
+      <c r="W4" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="W4" s="27" t="s">
-        <v>168</v>
-      </c>
       <c r="X4" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="Y4" s="27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="Z4" s="27" t="s">
         <v>42</v>
@@ -3790,19 +3797,19 @@
         <v>43</v>
       </c>
       <c r="AB4" s="27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AC4" s="27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AD4" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE4" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF4" s="27" t="s">
         <v>145</v>
-      </c>
-      <c r="AE4" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="AF4" s="27" t="s">
-        <v>148</v>
       </c>
       <c r="AG4" s="27" t="s">
         <v>44</v>
@@ -3823,16 +3830,16 @@
         <v>113</v>
       </c>
       <c r="AM4" s="27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN4" s="27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AO4" s="27" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AP4" s="27" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AQ4" s="3"/>
       <c r="AR4" s="27" t="s">
@@ -3854,7 +3861,7 @@
         <v>50</v>
       </c>
       <c r="AX4" s="27" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AY4" s="3"/>
       <c r="AZ4" s="25" t="s">
@@ -4059,7 +4066,7 @@
         <v>54</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G2" s="27" t="s">
         <v>68</v>
@@ -4078,7 +4085,7 @@
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4095,7 +4102,7 @@
         <v>54</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>68</v>
@@ -4114,7 +4121,7 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -4180,25 +4187,25 @@
         <v>73</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M1" s="28" t="s">
         <v>8</v>
@@ -4207,19 +4214,19 @@
         <v>9</v>
       </c>
       <c r="O1" s="28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="P1" s="28" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="Q1" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="R1" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="28" t="s">
-        <v>149</v>
-      </c>
       <c r="S1" s="28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>10</v>
@@ -4231,19 +4238,19 @@
         <v>108</v>
       </c>
       <c r="W1" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="X1" s="28" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Y1" s="28" t="s">
         <v>109</v>
       </c>
       <c r="Z1" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AA1" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -4260,25 +4267,25 @@
         <v>54</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H2" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="27" t="s">
-        <v>168</v>
-      </c>
       <c r="K2" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M2" s="27" t="s">
         <v>42</v>
@@ -4287,19 +4294,19 @@
         <v>43</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="Q2" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="S2" s="27" t="s">
         <v>145</v>
-      </c>
-      <c r="R2" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="S2" s="27" t="s">
-        <v>148</v>
       </c>
       <c r="T2" s="27" t="s">
         <v>44</v>
@@ -4320,10 +4327,10 @@
         <v>113</v>
       </c>
       <c r="Z2" s="27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AA2" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -4340,25 +4347,25 @@
         <v>54</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H3" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="J3" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="J3" s="27" t="s">
-        <v>168</v>
-      </c>
       <c r="K3" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M3" s="27" t="s">
         <v>42</v>
@@ -4367,19 +4374,19 @@
         <v>43</v>
       </c>
       <c r="O3" s="27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P3" s="27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="Q3" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="R3" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="S3" s="27" t="s">
         <v>145</v>
-      </c>
-      <c r="R3" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="S3" s="27" t="s">
-        <v>148</v>
       </c>
       <c r="T3" s="27" t="s">
         <v>44</v>
@@ -4400,10 +4407,10 @@
         <v>113</v>
       </c>
       <c r="Z3" s="27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AA3" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -4509,7 +4516,7 @@
         <v>50</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4545,7 +4552,7 @@
         <v>50</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -4636,19 +4643,19 @@
         <v>9</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="R1" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="28" t="s">
-        <v>149</v>
-      </c>
       <c r="S1" s="28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="T1" s="21" t="s">
         <v>73</v>
@@ -4707,19 +4714,19 @@
         <v>29</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="2" t="s">
@@ -4735,7 +4742,7 @@
         <v>34</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4757,7 +4764,7 @@
   <sheetPr codeName="Feuil6">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
@@ -4793,13 +4800,14 @@
     <col min="26" max="26" width="3.140625" customWidth="1"/>
     <col min="28" max="28" width="10.140625" customWidth="1"/>
     <col min="29" max="29" width="9.28515625" customWidth="1"/>
+    <col min="31" max="31" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="8"/>
       <c r="E1" s="2"/>
       <c r="F1" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>107</v>
@@ -4831,12 +4839,12 @@
       <c r="R1" s="70"/>
       <c r="S1" s="30"/>
       <c r="T1" s="66" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U1" s="69"/>
       <c r="V1" s="70"/>
       <c r="W1" s="69" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="X1" s="69"/>
       <c r="Y1" s="70"/>
@@ -4849,7 +4857,7 @@
       <c r="AB1" s="67"/>
       <c r="AC1" s="68"/>
     </row>
-    <row r="2" spans="1:29" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="8"/>
       <c r="E2" s="2"/>
       <c r="F2" s="40"/>
@@ -4877,7 +4885,7 @@
       <c r="AB2" s="10"/>
       <c r="AC2" s="39"/>
     </row>
-    <row r="3" spans="1:29" s="32" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" s="32" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>70</v>
       </c>
@@ -4890,7 +4898,7 @@
         <v>93</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>95</v>
@@ -4962,9 +4970,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>210</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
@@ -4974,26 +4982,26 @@
         <v>55</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>133</v>
+        <v>214</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>120</v>
@@ -5034,10 +5042,16 @@
         <v>100</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>124</v>
+        <v>212</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C5" s="8"/>
       <c r="E5" s="2"/>
       <c r="F5"/>
@@ -5112,7 +5126,7 @@
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5162,16 +5176,16 @@
         <v>73</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="L1" s="15" t="s">
         <v>26</v>
@@ -5188,19 +5202,19 @@
         <v>73</v>
       </c>
       <c r="R1" s="66" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="S1" s="69"/>
       <c r="T1" s="70"/>
       <c r="U1" s="30"/>
       <c r="V1" s="66" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="W1" s="69"/>
       <c r="X1" s="70"/>
       <c r="Y1" s="43"/>
       <c r="Z1" s="66" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AA1" s="69"/>
       <c r="AB1" s="70"/>
@@ -5257,7 +5271,7 @@
         <v>65</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>18</v>
@@ -5346,7 +5360,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>81</v>
@@ -5355,7 +5369,7 @@
         <v>67</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>25</v>
@@ -5364,56 +5378,56 @@
         <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="34" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="O4" s="34" t="s">
         <v>32</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S4" s="34" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>114</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AA4" s="2" t="s">
         <v>115</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AD4" s="2">
         <v>1</v>
@@ -5422,7 +5436,7 @@
         <v>103</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de l'expiration des qualif directeur SF temporaires
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E30158-DA51-4F66-A1BD-DB91125E1B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5DA5C7-22FA-4EB3-A155-DD7EB23FC2B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="643" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1320" yWindow="360" windowWidth="24900" windowHeight="13950" tabRatio="643" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="259">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -843,6 +843,9 @@
   </si>
   <si>
     <t>Alerte</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${chef.qualif.dirsf.aetaetestagiaire}" onProcessed="org.leplan73.outilssgdf.outils.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2707,7 @@
         <v>169</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>68</v>
+        <v>258</v>
       </c>
       <c r="L3" s="26" t="s">
         <v>57</v>
@@ -2866,7 +2869,7 @@
         <v>169</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>68</v>
+        <v>258</v>
       </c>
       <c r="L4" s="26" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Ajout du noeud de tisserand #13
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5DA5C7-22FA-4EB3-A155-DD7EB23FC2B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322E385A-7BCA-4D65-9263-81508E35B9D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="360" windowWidth="24900" windowHeight="13950" tabRatio="643" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Qualifications!$A$1:$O$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Quota année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Quota unités'!$A$3:$AF$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BF$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BG$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Synthèse par unité'!$A$1:$Y$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="261">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -846,6 +846,12 @@
   </si>
   <si>
     <t>&lt;jt:if test="${chef.qualif.dirsf.aetaetestagiaire}" onProcessed="org.leplan73.outilssgdf.outils.QualifDirSfListener"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>Nœud de tisserand</t>
+  </si>
+  <si>
+    <t>${chef.diplome.noeuddetisserand.dateobtention}</t>
   </si>
 </sst>
 </file>
@@ -1350,12 +1356,6 @@
     <xf numFmtId="14" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1397,6 +1397,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2385,7 +2391,7 @@
   <sheetPr codeName="Feuil1">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:BF4"/>
+  <dimension ref="A1:BG4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -2426,26 +2432,26 @@
     <col min="39" max="39" width="15.28515625" style="26" customWidth="1"/>
     <col min="40" max="42" width="12.5703125" style="26" customWidth="1"/>
     <col min="43" max="43" width="2.85546875" style="2" customWidth="1"/>
-    <col min="44" max="50" width="11.42578125" style="26" customWidth="1"/>
-    <col min="51" max="51" width="2.85546875" style="2" customWidth="1"/>
-    <col min="52" max="52" width="12.7109375" style="2" customWidth="1"/>
-    <col min="53" max="53" width="15" style="2" customWidth="1"/>
-    <col min="54" max="54" width="14.140625" style="2" customWidth="1"/>
-    <col min="55" max="55" width="2.85546875" customWidth="1"/>
-    <col min="56" max="56" width="18.5703125" style="2" customWidth="1"/>
-    <col min="57" max="57" width="16.42578125" style="2" customWidth="1"/>
-    <col min="58" max="58" width="28.5703125" style="2" customWidth="1"/>
+    <col min="44" max="51" width="11.42578125" style="26" customWidth="1"/>
+    <col min="52" max="52" width="2.85546875" style="2" customWidth="1"/>
+    <col min="53" max="53" width="12.7109375" style="2" customWidth="1"/>
+    <col min="54" max="54" width="15" style="2" customWidth="1"/>
+    <col min="55" max="55" width="14.140625" style="2" customWidth="1"/>
+    <col min="56" max="56" width="2.85546875" customWidth="1"/>
+    <col min="57" max="57" width="18.5703125" style="2" customWidth="1"/>
+    <col min="58" max="58" width="16.42578125" style="2" customWidth="1"/>
+    <col min="59" max="59" width="28.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66"/>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
+    <row r="1" spans="1:59" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="66"/>
       <c r="J1" s="61" t="s">
         <v>198</v>
       </c>
@@ -2455,53 +2461,54 @@
       <c r="N1" s="62"/>
       <c r="O1" s="63"/>
       <c r="Q1" s="17"/>
-      <c r="S1" s="72" t="s">
+      <c r="S1" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
-      <c r="AB1" s="73"/>
-      <c r="AC1" s="73"/>
-      <c r="AD1" s="73"/>
-      <c r="AE1" s="73"/>
-      <c r="AF1" s="73"/>
-      <c r="AG1" s="73"/>
-      <c r="AH1" s="73"/>
-      <c r="AI1" s="73"/>
-      <c r="AJ1" s="73"/>
-      <c r="AK1" s="73"/>
-      <c r="AL1" s="73"/>
-      <c r="AM1" s="73"/>
-      <c r="AN1" s="73"/>
-      <c r="AO1" s="73"/>
-      <c r="AP1" s="73"/>
-      <c r="AR1" s="64" t="s">
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="71"/>
+      <c r="AD1" s="71"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="71"/>
+      <c r="AG1" s="71"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="71"/>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="71"/>
+      <c r="AM1" s="71"/>
+      <c r="AN1" s="71"/>
+      <c r="AO1" s="71"/>
+      <c r="AP1" s="71"/>
+      <c r="AR1" s="78" t="s">
         <v>200</v>
       </c>
-      <c r="AS1" s="65"/>
-      <c r="AT1" s="65"/>
-      <c r="AU1" s="65"/>
-      <c r="AV1" s="65"/>
-      <c r="AW1" s="65"/>
-      <c r="AX1" s="65"/>
-      <c r="AZ1" s="69" t="s">
+      <c r="AS1" s="79"/>
+      <c r="AT1" s="79"/>
+      <c r="AU1" s="79"/>
+      <c r="AV1" s="79"/>
+      <c r="AW1" s="79"/>
+      <c r="AX1" s="79"/>
+      <c r="AY1" s="79"/>
+      <c r="BA1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="BA1" s="70"/>
-      <c r="BB1" s="71"/>
-      <c r="BD1" s="58" t="s">
+      <c r="BB1" s="68"/>
+      <c r="BC1" s="69"/>
+      <c r="BE1" s="58" t="s">
         <v>250</v>
       </c>
-      <c r="BE1" s="59"/>
-      <c r="BF1" s="60"/>
-    </row>
-    <row r="2" spans="1:58" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BF1" s="59"/>
+      <c r="BG1" s="60"/>
+    </row>
+    <row r="2" spans="1:59" s="20" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2652,32 +2659,35 @@
       <c r="AX2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="AY2" s="21" t="s">
+      <c r="AY2" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="AZ2" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AZ2" s="12" t="s">
+      <c r="BA2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="BA2" s="15" t="s">
+      <c r="BB2" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="BB2" s="15" t="s">
+      <c r="BC2" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="BC2" s="21" t="s">
+      <c r="BD2" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="BD2" s="17" t="s">
+      <c r="BE2" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="BE2" s="17" t="s">
+      <c r="BF2" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="BF2" s="17" t="s">
+      <c r="BG2" s="17" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>78</v>
       </c>
@@ -2819,27 +2829,30 @@
       <c r="AX3" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="AY3" s="3"/>
-      <c r="AZ3" s="57" t="s">
+      <c r="AY3" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="AZ3" s="3"/>
+      <c r="BA3" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="BA3" s="3" t="s">
+      <c r="BB3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="BB3" s="3" t="s">
+      <c r="BC3" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="BD3" s="2" t="s">
+      <c r="BE3" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="BE3" s="2" t="s">
+      <c r="BF3" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="BF3" s="2" t="s">
+      <c r="BG3" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>82</v>
       </c>
@@ -2981,42 +2994,45 @@
       <c r="AX4" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="AY4" s="3"/>
-      <c r="AZ4" s="57" t="s">
+      <c r="AY4" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="AZ4" s="3"/>
+      <c r="BA4" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="BA4" s="3" t="s">
+      <c r="BB4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="BB4" s="3" t="s">
+      <c r="BC4" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="BD4" s="2" t="s">
+      <c r="BE4" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="BE4" s="2" t="s">
+      <c r="BF4" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="BF4" s="2" t="s">
+      <c r="BG4" s="2" t="s">
         <v>254</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:BF4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
+  <autoFilter ref="A2:BG4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
   <mergeCells count="6">
-    <mergeCell ref="BD1:BF1"/>
+    <mergeCell ref="BE1:BG1"/>
     <mergeCell ref="J1:O1"/>
-    <mergeCell ref="AR1:AX1"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="AZ1:BB1"/>
+    <mergeCell ref="BA1:BC1"/>
     <mergeCell ref="S1:AP1"/>
+    <mergeCell ref="AR1:AY1"/>
   </mergeCells>
-  <conditionalFormatting sqref="BB3:BB65537">
+  <conditionalFormatting sqref="BC3:BC65537">
     <cfRule type="cellIs" dxfId="43" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BA3:BA65537">
+  <conditionalFormatting sqref="BB3:BB65537">
     <cfRule type="cellIs" dxfId="42" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -4095,38 +4111,38 @@
       <c r="K1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="M1" s="75"/>
-      <c r="N1" s="76"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="74"/>
       <c r="O1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="74" t="s">
+      <c r="P1" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="78"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="76"/>
       <c r="S1" s="29"/>
-      <c r="T1" s="74" t="s">
+      <c r="T1" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="U1" s="77"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="77" t="s">
+      <c r="U1" s="75"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="78"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="76"/>
       <c r="Z1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA1" s="79" t="s">
+      <c r="AA1" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="76"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="74"/>
     </row>
     <row r="2" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="8"/>
@@ -4469,39 +4485,39 @@
       <c r="M1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="79" t="s">
+      <c r="N1" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="76"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="74"/>
       <c r="Q1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="74" t="s">
+      <c r="R1" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="S1" s="77"/>
-      <c r="T1" s="78"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="76"/>
       <c r="U1" s="29"/>
-      <c r="V1" s="74" t="s">
+      <c r="V1" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="W1" s="77"/>
-      <c r="X1" s="78"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="76"/>
       <c r="Y1" s="42"/>
-      <c r="Z1" s="74" t="s">
+      <c r="Z1" s="72" t="s">
         <v>193</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="78"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="76"/>
       <c r="AC1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="79" t="s">
+      <c r="AD1" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="76"/>
+      <c r="AE1" s="73"/>
+      <c r="AF1" s="74"/>
     </row>
     <row r="2" spans="1:32" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47"/>

</xml_diff>

<commit_message>
Ajout de la formation "responsable farfadets" #14
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EA0AB2-94E8-4578-89CB-023DD0A2724A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A08B29-22D1-4531-BFB4-39962BC974DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" tabRatio="643" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="780" yWindow="570" windowWidth="21945" windowHeight="14865" tabRatio="682" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Qualifications!$A$1:$O$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Quota année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Quota unités'!$A$3:$AF$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BG$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BH$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Synthèse par unité'!$A$1:$Y$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="263">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -850,6 +850,12 @@
   </si>
   <si>
     <t>Nb titulaires ou stagiaires et 1 dir</t>
+  </si>
+  <si>
+    <t>RESPONSABLE FARFADETS</t>
+  </si>
+  <si>
+    <t>${chef.formation.responsable_farfadets.datefin}</t>
   </si>
 </sst>
 </file>
@@ -2210,129 +2216,129 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="155" style="52" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" style="52" customWidth="1"/>
-    <col min="3" max="16384" width="11.453125" style="52"/>
+    <col min="2" max="2" width="17.5703125" style="52" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="51" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="52" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="51" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="51" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
         <v>237</v>
       </c>
@@ -2350,13 +2356,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>70</v>
       </c>
@@ -2365,7 +2371,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -2386,23 +2392,25 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="23">
-        <v>43744</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>43766</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>36</v>
       </c>
@@ -2410,7 +2418,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>83</v>
       </c>
@@ -2428,7 +2436,7 @@
   <sheetPr codeName="Feuil1">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:BG4"/>
+  <dimension ref="A1:BH4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -2437,52 +2445,53 @@
       <selection pane="bottomRight" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" customWidth="1"/>
-    <col min="3" max="3" width="24.7265625" customWidth="1"/>
-    <col min="4" max="4" width="51.81640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
     <col min="7" max="8" width="10" style="2" customWidth="1"/>
-    <col min="9" max="9" width="2.81640625" style="2" customWidth="1"/>
-    <col min="10" max="13" width="11.453125" style="25" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="13.54296875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="2.54296875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="2.81640625" customWidth="1"/>
-    <col min="19" max="19" width="11.453125" style="25" customWidth="1"/>
-    <col min="20" max="20" width="11.1796875" style="25" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" style="25" customWidth="1"/>
-    <col min="22" max="22" width="11.453125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="2" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="25" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="2.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="2.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" style="25" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" style="25" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" style="25" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="25" customWidth="1"/>
     <col min="23" max="23" width="18" style="25" customWidth="1"/>
-    <col min="24" max="25" width="14.26953125" style="25" customWidth="1"/>
-    <col min="26" max="27" width="11.453125" style="25" customWidth="1"/>
-    <col min="28" max="28" width="12.453125" style="25" customWidth="1"/>
-    <col min="29" max="29" width="11.453125" style="25" customWidth="1"/>
-    <col min="30" max="30" width="14.1796875" style="25" customWidth="1"/>
-    <col min="31" max="31" width="14.36328125" style="25" customWidth="1"/>
-    <col min="32" max="32" width="13" style="25" customWidth="1"/>
-    <col min="33" max="37" width="11.453125" style="25" customWidth="1"/>
-    <col min="38" max="38" width="18.1796875" style="25" customWidth="1"/>
-    <col min="39" max="39" width="15.26953125" style="25" customWidth="1"/>
-    <col min="40" max="42" width="12.54296875" style="25" customWidth="1"/>
-    <col min="43" max="43" width="2.81640625" style="2" customWidth="1"/>
-    <col min="44" max="45" width="11.453125" style="25" customWidth="1"/>
-    <col min="46" max="51" width="10.81640625" style="25" customWidth="1"/>
-    <col min="52" max="52" width="2.81640625" style="2" customWidth="1"/>
-    <col min="53" max="53" width="8.54296875" style="2" customWidth="1"/>
-    <col min="54" max="54" width="11.26953125" style="2" customWidth="1"/>
-    <col min="55" max="55" width="10.453125" style="2" customWidth="1"/>
-    <col min="56" max="56" width="2.81640625" customWidth="1"/>
-    <col min="57" max="57" width="12.1796875" style="2" customWidth="1"/>
-    <col min="58" max="58" width="17.54296875" style="2" customWidth="1"/>
-    <col min="59" max="59" width="24.90625" style="2" customWidth="1"/>
+    <col min="24" max="25" width="14.28515625" style="25" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" style="25" customWidth="1"/>
+    <col min="27" max="28" width="11.42578125" style="25" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" style="25" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" style="25" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" style="25" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="25" customWidth="1"/>
+    <col min="33" max="33" width="13" style="25" customWidth="1"/>
+    <col min="34" max="38" width="11.42578125" style="25" customWidth="1"/>
+    <col min="39" max="39" width="18.140625" style="25" customWidth="1"/>
+    <col min="40" max="40" width="15.28515625" style="25" customWidth="1"/>
+    <col min="41" max="43" width="12.5703125" style="25" customWidth="1"/>
+    <col min="44" max="44" width="2.85546875" style="2" customWidth="1"/>
+    <col min="45" max="46" width="11.42578125" style="25" customWidth="1"/>
+    <col min="47" max="52" width="10.85546875" style="25" customWidth="1"/>
+    <col min="53" max="53" width="2.85546875" style="2" customWidth="1"/>
+    <col min="54" max="54" width="8.5703125" style="2" customWidth="1"/>
+    <col min="55" max="55" width="11.28515625" style="2" customWidth="1"/>
+    <col min="56" max="56" width="10.42578125" style="2" customWidth="1"/>
+    <col min="57" max="57" width="2.85546875" customWidth="1"/>
+    <col min="58" max="58" width="12.140625" style="2" customWidth="1"/>
+    <col min="59" max="59" width="17.5703125" style="2" customWidth="1"/>
+    <col min="60" max="60" width="24.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:60" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77"/>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
@@ -2526,28 +2535,29 @@
       <c r="AN1" s="84"/>
       <c r="AO1" s="84"/>
       <c r="AP1" s="84"/>
-      <c r="AR1" s="85" t="s">
+      <c r="AQ1" s="84"/>
+      <c r="AS1" s="85" t="s">
         <v>199</v>
       </c>
-      <c r="AS1" s="86"/>
       <c r="AT1" s="86"/>
       <c r="AU1" s="86"/>
       <c r="AV1" s="86"/>
       <c r="AW1" s="86"/>
       <c r="AX1" s="86"/>
       <c r="AY1" s="86"/>
-      <c r="BA1" s="80" t="s">
+      <c r="AZ1" s="86"/>
+      <c r="BB1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="BB1" s="81"/>
-      <c r="BC1" s="82"/>
-      <c r="BE1" s="71" t="s">
+      <c r="BC1" s="81"/>
+      <c r="BD1" s="82"/>
+      <c r="BF1" s="71" t="s">
         <v>249</v>
       </c>
-      <c r="BF1" s="72"/>
-      <c r="BG1" s="73"/>
-    </row>
-    <row r="2" spans="1:59" s="65" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BG1" s="72"/>
+      <c r="BH1" s="73"/>
+    </row>
+    <row r="2" spans="1:60" s="65" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
         <v>2</v>
       </c>
@@ -2624,109 +2634,112 @@
         <v>164</v>
       </c>
       <c r="Z2" s="64" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA2" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="64" t="s">
+      <c r="AB2" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="AB2" s="64" t="s">
+      <c r="AC2" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="AC2" s="64" t="s">
+      <c r="AD2" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="AD2" s="64" t="s">
+      <c r="AE2" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="AE2" s="64" t="s">
+      <c r="AF2" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="AF2" s="64" t="s">
+      <c r="AG2" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="AG2" s="64" t="s">
+      <c r="AH2" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="AH2" s="64" t="s">
+      <c r="AI2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="64" t="s">
+      <c r="AJ2" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="AJ2" s="64" t="s">
+      <c r="AK2" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="AK2" s="64" t="s">
+      <c r="AL2" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="AL2" s="64" t="s">
+      <c r="AM2" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="AM2" s="64" t="s">
+      <c r="AN2" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="AN2" s="64" t="s">
+      <c r="AO2" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="AO2" s="64" t="s">
+      <c r="AP2" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="AP2" s="64" t="s">
+      <c r="AQ2" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="AQ2" s="61" t="s">
+      <c r="AR2" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="AR2" s="56" t="s">
+      <c r="AS2" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="AS2" s="56" t="s">
+      <c r="AT2" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="AT2" s="56" t="s">
+      <c r="AU2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="AU2" s="56" t="s">
+      <c r="AV2" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="AV2" s="56" t="s">
+      <c r="AW2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="AW2" s="56" t="s">
+      <c r="AX2" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AX2" s="56" t="s">
+      <c r="AY2" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="AY2" s="56" t="s">
+      <c r="AZ2" s="56" t="s">
         <v>258</v>
       </c>
-      <c r="AZ2" s="61" t="s">
+      <c r="BA2" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="BA2" s="57" t="s">
+      <c r="BB2" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="BB2" s="60" t="s">
+      <c r="BC2" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="BC2" s="60" t="s">
+      <c r="BD2" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="BD2" s="61" t="s">
+      <c r="BE2" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="BE2" s="63" t="s">
+      <c r="BF2" s="63" t="s">
         <v>246</v>
       </c>
-      <c r="BF2" s="63" t="s">
+      <c r="BG2" s="63" t="s">
         <v>248</v>
       </c>
-      <c r="BG2" s="63" t="s">
+      <c r="BH2" s="63" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>78</v>
       </c>
@@ -2796,102 +2809,105 @@
         <v>165</v>
       </c>
       <c r="Z3" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="AA3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="AA3" s="25" t="s">
+      <c r="AB3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AB3" s="25" t="s">
+      <c r="AC3" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="AC3" s="25" t="s">
+      <c r="AD3" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="AD3" s="25" t="s">
+      <c r="AE3" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="AE3" s="25" t="s">
+      <c r="AF3" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="AF3" s="25" t="s">
+      <c r="AG3" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="AG3" s="25" t="s">
+      <c r="AH3" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AH3" s="25" t="s">
+      <c r="AI3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AI3" s="25" t="s">
+      <c r="AJ3" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="AJ3" s="25" t="s">
+      <c r="AK3" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="AK3" s="25" t="s">
+      <c r="AL3" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="AL3" s="25" t="s">
+      <c r="AM3" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="AM3" s="25" t="s">
+      <c r="AN3" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="AN3" s="25" t="s">
+      <c r="AO3" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="AO3" s="25" t="s">
+      <c r="AP3" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="AP3" s="25" t="s">
+      <c r="AQ3" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="AQ3" s="3"/>
-      <c r="AR3" s="25" t="s">
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AS3" s="25" t="s">
+      <c r="AT3" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="AT3" s="25" t="s">
+      <c r="AU3" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AU3" s="25" t="s">
+      <c r="AV3" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="AV3" s="25" t="s">
+      <c r="AW3" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="AW3" s="25" t="s">
+      <c r="AX3" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="AX3" s="25" t="s">
+      <c r="AY3" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="AY3" s="25" t="s">
+      <c r="AZ3" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="AZ3" s="3"/>
-      <c r="BA3" s="55" t="s">
+      <c r="BA3" s="3"/>
+      <c r="BB3" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="BB3" s="3" t="s">
+      <c r="BC3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="BC3" s="3" t="s">
+      <c r="BD3" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="BE3" s="2" t="s">
+      <c r="BF3" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="BF3" s="2" t="s">
+      <c r="BG3" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="BG3" s="2" t="s">
+      <c r="BH3" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>82</v>
       </c>
@@ -2961,117 +2977,120 @@
         <v>165</v>
       </c>
       <c r="Z4" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="AA4" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="AA4" s="25" t="s">
+      <c r="AB4" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AB4" s="25" t="s">
+      <c r="AC4" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="AC4" s="25" t="s">
+      <c r="AD4" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="AD4" s="25" t="s">
+      <c r="AE4" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="AE4" s="25" t="s">
+      <c r="AF4" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="AF4" s="25" t="s">
+      <c r="AG4" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="AG4" s="25" t="s">
+      <c r="AH4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AH4" s="25" t="s">
+      <c r="AI4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AI4" s="25" t="s">
+      <c r="AJ4" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="AJ4" s="25" t="s">
+      <c r="AK4" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="AK4" s="25" t="s">
+      <c r="AL4" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="AL4" s="25" t="s">
+      <c r="AM4" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="AM4" s="25" t="s">
+      <c r="AN4" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="AN4" s="25" t="s">
+      <c r="AO4" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="AO4" s="25" t="s">
+      <c r="AP4" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="AP4" s="25" t="s">
+      <c r="AQ4" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="AQ4" s="3"/>
-      <c r="AR4" s="25" t="s">
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AS4" s="25" t="s">
+      <c r="AT4" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="AT4" s="25" t="s">
+      <c r="AU4" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AU4" s="25" t="s">
+      <c r="AV4" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="AV4" s="25" t="s">
+      <c r="AW4" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="AW4" s="25" t="s">
+      <c r="AX4" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="AX4" s="25" t="s">
+      <c r="AY4" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="AY4" s="25" t="s">
+      <c r="AZ4" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="AZ4" s="3"/>
-      <c r="BA4" s="55" t="s">
+      <c r="BA4" s="3"/>
+      <c r="BB4" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="BB4" s="3" t="s">
+      <c r="BC4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="BC4" s="3" t="s">
+      <c r="BD4" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="BE4" s="2" t="s">
+      <c r="BF4" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="BF4" s="2" t="s">
+      <c r="BG4" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="BG4" s="2" t="s">
+      <c r="BH4" s="2" t="s">
         <v>253</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:BG4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
+  <autoFilter ref="A2:BH4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
   <mergeCells count="6">
-    <mergeCell ref="BE1:BG1"/>
+    <mergeCell ref="BF1:BH1"/>
     <mergeCell ref="J1:O1"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="S1:AP1"/>
-    <mergeCell ref="AR1:AY1"/>
+    <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="S1:AQ1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
-  <conditionalFormatting sqref="BC3:BC65537">
+  <conditionalFormatting sqref="BD3:BD65537">
     <cfRule type="cellIs" dxfId="43" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB3:BB65537">
+  <conditionalFormatting sqref="BC3:BC65537">
     <cfRule type="cellIs" dxfId="42" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -3159,20 +3178,20 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" customWidth="1"/>
-    <col min="3" max="3" width="25.08984375" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" customWidth="1"/>
-    <col min="8" max="9" width="12.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="88" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="30" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" s="30" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
@@ -3204,7 +3223,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>255</v>
       </c>
@@ -3264,23 +3283,23 @@
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" customWidth="1"/>
-    <col min="8" max="11" width="11.453125" style="25" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="2.54296875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="14.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
+    <col min="8" max="11" width="11.42578125" style="25" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="2.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -3327,7 +3346,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>78</v>
       </c>
@@ -3369,7 +3388,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>82</v>
       </c>
@@ -3430,33 +3449,33 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" style="25" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" style="25" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" style="25" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="25" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="25" customWidth="1"/>
     <col min="12" max="12" width="18" style="25" customWidth="1"/>
-    <col min="13" max="14" width="14.26953125" style="25" customWidth="1"/>
-    <col min="15" max="16" width="11.453125" style="25" customWidth="1"/>
-    <col min="17" max="17" width="12.453125" style="25" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" style="25" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" style="25" customWidth="1"/>
+    <col min="13" max="14" width="14.28515625" style="25" customWidth="1"/>
+    <col min="15" max="16" width="11.42578125" style="25" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="25" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="25" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="25" customWidth="1"/>
     <col min="20" max="21" width="13" style="25" customWidth="1"/>
-    <col min="22" max="26" width="11.453125" style="25" customWidth="1"/>
-    <col min="27" max="27" width="18.1796875" style="25" customWidth="1"/>
-    <col min="28" max="28" width="15.26953125" style="25" customWidth="1"/>
-    <col min="29" max="29" width="12.54296875" style="25" customWidth="1"/>
+    <col min="22" max="26" width="11.42578125" style="25" customWidth="1"/>
+    <col min="27" max="27" width="18.140625" style="25" customWidth="1"/>
+    <col min="28" max="28" width="15.28515625" style="25" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -3545,7 +3564,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>78</v>
       </c>
@@ -3631,7 +3650,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>82</v>
       </c>
@@ -3736,19 +3755,19 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" style="2" customWidth="1"/>
-    <col min="8" max="14" width="11.453125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="2" customWidth="1"/>
+    <col min="8" max="14" width="11.42578125" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -3792,7 +3811,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>78</v>
       </c>
@@ -3834,7 +3853,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>82</v>
       </c>
@@ -3897,29 +3916,29 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.26953125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="2.81640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="2"/>
-    <col min="6" max="7" width="8.81640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.81640625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="8.81640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="2.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="75.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2"/>
+    <col min="6" max="7" width="8.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="5.54296875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.81640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.453125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" customWidth="1"/>
-    <col min="18" max="18" width="17.26953125" customWidth="1"/>
-    <col min="19" max="19" width="12.7265625" customWidth="1"/>
-    <col min="20" max="20" width="2.81640625" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
@@ -3996,7 +4015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>61</v>
       </c>
@@ -4065,11 +4084,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="R4" s="1"/>
     </row>
   </sheetData>
@@ -4093,37 +4112,37 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.26953125" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" style="67" customWidth="1"/>
+    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="67" customWidth="1"/>
     <col min="3" max="3" width="3" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="7.81640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.36328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="2.81640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.08984375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.81640625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="13.6328125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="11.1796875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="8.81640625" customWidth="1"/>
-    <col min="19" max="19" width="2.81640625" customWidth="1"/>
-    <col min="22" max="22" width="8.453125" customWidth="1"/>
-    <col min="24" max="24" width="10.36328125" customWidth="1"/>
-    <col min="25" max="25" width="12.7265625" customWidth="1"/>
-    <col min="26" max="26" width="3.1796875" customWidth="1"/>
-    <col min="28" max="28" width="10.1796875" customWidth="1"/>
-    <col min="29" max="29" width="9.26953125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" customWidth="1"/>
+    <col min="26" max="26" width="3.140625" customWidth="1"/>
+    <col min="28" max="28" width="10.140625" customWidth="1"/>
+    <col min="29" max="29" width="9.28515625" customWidth="1"/>
     <col min="31" max="31" width="10" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="8"/>
       <c r="E1" s="2"/>
       <c r="F1" s="14" t="s">
@@ -4177,7 +4196,7 @@
       <c r="AB1" s="88"/>
       <c r="AC1" s="89"/>
     </row>
-    <row r="2" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="8"/>
       <c r="E2" s="2"/>
       <c r="F2" s="38"/>
@@ -4205,7 +4224,7 @@
       <c r="AB2" s="10"/>
       <c r="AC2" s="37"/>
     </row>
-    <row r="3" spans="1:35" s="30" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:35" s="30" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>70</v>
       </c>
@@ -4292,7 +4311,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -4376,7 +4395,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C5" s="8"/>
       <c r="E5" s="2"/>
       <c r="F5"/>
@@ -4454,43 +4473,43 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.54296875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="2.81640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="32" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.453125" style="32" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7265625" style="32" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.81640625" customWidth="1"/>
-    <col min="18" max="18" width="9.54296875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="2" customWidth="1"/>
     <col min="19" max="19" width="7" style="2" customWidth="1"/>
-    <col min="20" max="20" width="7.81640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="2.81640625" customWidth="1"/>
-    <col min="22" max="22" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.90625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="2.81640625" customWidth="1"/>
-    <col min="26" max="26" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.90625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="11.26953125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="2.81640625" customWidth="1"/>
-    <col min="30" max="30" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.453125" style="2" customWidth="1"/>
-    <col min="32" max="32" width="6.36328125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="2.85546875" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="2.85546875" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.85546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="11.28515625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="2.85546875" customWidth="1"/>
+    <col min="30" max="30" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.42578125" style="2" customWidth="1"/>
+    <col min="32" max="32" width="6.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:32" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="48"/>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -4552,7 +4571,7 @@
       <c r="AE1" s="88"/>
       <c r="AF1" s="89"/>
     </row>
-    <row r="2" spans="1:32" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:32" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -4585,7 +4604,7 @@
       <c r="AE2" s="10"/>
       <c r="AF2" s="37"/>
     </row>
-    <row r="3" spans="1:32" s="70" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:32" s="70" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>17</v>
       </c>
@@ -4683,7 +4702,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>175</v>
       </c>

</xml_diff>

<commit_message>
Réorganisation des onglets #15
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -8,32 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A08B29-22D1-4531-BFB4-39962BC974DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E814D78F-738C-4062-8086-CA02E9FBE1FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="570" windowWidth="21945" windowHeight="14865" tabRatio="682" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1080" yWindow="1005" windowWidth="22230" windowHeight="15240" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
     <sheet name="Responsables" sheetId="1" r:id="rId2"/>
-    <sheet name="Alertes" sheetId="14" r:id="rId3"/>
-    <sheet name="Qualifications" sheetId="12" r:id="rId4"/>
-    <sheet name="Formations" sheetId="13" r:id="rId5"/>
-    <sheet name="Diplômes" sheetId="11" r:id="rId6"/>
-    <sheet name="Synthèse par unité" sheetId="3" r:id="rId7"/>
-    <sheet name="Quota année" sheetId="8" r:id="rId8"/>
-    <sheet name="Quota unités" sheetId="2" r:id="rId9"/>
-    <sheet name="Global" sheetId="9" r:id="rId10"/>
-    <sheet name="Général" sheetId="10" r:id="rId11"/>
+    <sheet name="Farfadets" sheetId="15" r:id="rId3"/>
+    <sheet name="Compas" sheetId="16" r:id="rId4"/>
+    <sheet name="Alertes" sheetId="14" r:id="rId5"/>
+    <sheet name="Synthèse par unité" sheetId="3" r:id="rId6"/>
+    <sheet name="Quota année" sheetId="8" r:id="rId7"/>
+    <sheet name="Quota unités" sheetId="2" r:id="rId8"/>
+    <sheet name="Global" sheetId="9" r:id="rId9"/>
+    <sheet name="Général" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alertes!$A$1:$J$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Diplômes!$A$1:$N$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Formations!$A$1:$AC$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Qualifications!$A$1:$O$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Quota année'!$A$3:$AC$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Quota unités'!$A$3:$AF$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Alertes!$A$1:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compas!$A$2:$Q$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Farfadets!$A$2:$O$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quota année'!$A$3:$AC$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Quota unités'!$A$3:$AF$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BH$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Synthèse par unité'!$A$1:$Y$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Synthèse par unité'!$A$1:$Y$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +41,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="263">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t>${unite.codestructure}</t>
-  </si>
-  <si>
-    <t>&lt;jt:if test="${chef.qualif.dirsf.pasok}"&gt;${chef.qualif.dirsf.finvalidite}&lt;/jt:if&gt;</t>
   </si>
   <si>
     <t>${global.groupe}</t>
@@ -580,15 +577,6 @@
     <t>${chef.formation.fif.datefin}</t>
   </si>
   <si>
-    <t>&lt;jt:if test="${chef.bafapotentiel}"&gt;Oui&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
-    <t>${chef.formation.fcf.datefin}&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
-    <t>${chef.diplome.buchettes4.dateobtention}&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>&lt;jt:forEach items="${unites}" var="unite" orderBy="codestructure" where="${unite.nonPrincipal}" &gt;${unite.nom}</t>
   </si>
   <si>
@@ -759,21 +747,9 @@
     <t>Toutes les données sont issues de l'intranet</t>
   </si>
   <si>
-    <t>Feuille "Formations"</t>
-  </si>
-  <si>
-    <t>colonnes "Diplômes"</t>
-  </si>
-  <si>
-    <t>Elles indiquent la date à laquelle le diplôme a été remis</t>
-  </si>
-  <si>
     <t>Feuille "Responsables"</t>
   </si>
   <si>
-    <t>Feuille "Qualifications"</t>
-  </si>
-  <si>
     <t>Feuille "Synthèse par unité"</t>
   </si>
   <si>
@@ -792,12 +768,6 @@
     <t>colonnes "Formations" &amp; "Diplômes" : Elles indiquent la date de passage de la formation ou la date d'obtention du diplôme</t>
   </si>
   <si>
-    <t>colonne "Stagiaire BAFA potentiel" : Si la personne a passé le tech ou la formation générale du BAFA il y a moins de 3 ans 1/2 et n'a pas encore passé un stage complet APPRO et n'a pas encore son BAFA</t>
-  </si>
-  <si>
-    <t>Elles indiquent la date du dernier jour de la formation</t>
-  </si>
-  <si>
     <t>Effectue un comptage total des effectifs et applique ensuite les règles d'accueil collectif de mineurs (Voir Guide règlementaire du Scoutisme Français) et indique par un fond rouge les manques éventuels. Idem avec le PSC1 (secourisme)</t>
   </si>
   <si>
@@ -856,6 +826,36 @@
   </si>
   <si>
     <t>${chef.formation.responsable_farfadets.datefin}</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${chef.agecalcule}"&gt;${chef.age}&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${chef.age18ansokcamp}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${chefs}" var="chef" where="${chef.farfadet}" orderBy="codestructure;fonction;nom"&gt;${chef.codetext}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${compas}" var="chef" where="${chef.farfadet}" orderBy="codestructure;fonction;nom"&gt;${chef.codetext}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${chefs}" var="chef" where="${chef.compa}" orderBy="codestructure;fonction;nom"&gt;${chef.codetext}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${compas}" var="chef" where="${chef.compa}" orderBy="codestructure;fonction;nom"&gt;${chef.codetext}</t>
+  </si>
+  <si>
+    <t>Feuille "Farfadets"</t>
+  </si>
+  <si>
+    <t>Feuille "Compas"</t>
+  </si>
+  <si>
+    <t>Feuille regroupant les reponsables farfadets et les parents farfadets</t>
+  </si>
+  <si>
+    <t>Feuille regroupant les compas et les accompagnateurs compas</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1175,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1240,18 +1240,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1381,6 +1375,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1427,6 +1427,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1453,7 +1465,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="107">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1671,6 +1683,636 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2212,135 +2854,120 @@
   <sheetPr codeName="Feuil10">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="155" style="52" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="52" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="52"/>
+    <col min="1" max="1" width="155" style="50" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="50" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
-        <v>238</v>
+      <c r="A1" s="51" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
-        <v>239</v>
+      <c r="A3" s="50" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
-        <v>229</v>
+      <c r="A4" s="50" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
-        <v>223</v>
+      <c r="A5" s="50" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
-        <v>224</v>
+      <c r="A7" s="52" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
-        <v>233</v>
+      <c r="A9" s="49" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
-        <v>225</v>
+      <c r="A10" s="50" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
-        <v>240</v>
+      <c r="A11" s="50" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
-        <v>254</v>
+      <c r="A12" s="50" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="s">
-        <v>234</v>
+      <c r="A14" s="49" t="s">
+        <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
-        <v>225</v>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="50" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
-        <v>241</v>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
-        <v>230</v>
+      <c r="A18" s="50" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
-        <v>242</v>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
-        <v>231</v>
+      <c r="A21" s="50" t="s">
+        <v>228</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52" t="s">
-        <v>232</v>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="49" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="51" t="s">
-        <v>235</v>
+    <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="50" t="s">
+        <v>233</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52" t="s">
-        <v>236</v>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
+        <v>223</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
-        <v>226</v>
+    <row r="27" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="50" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
-        <v>243</v>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="49" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
-        <v>237</v>
+      <c r="A30" s="50" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2350,51 +2977,13 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9364C085-89A2-4191-BD71-23274096DEBB}">
-  <sheetPr codeName="Feuil8"/>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AFD6E7-296C-4D2D-8BB3-DCE2EA8A2647}">
   <sheetPr codeName="Feuil9">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2420,10 +3009,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2455,32 +3044,32 @@
     <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
     <col min="7" max="8" width="10" style="2" customWidth="1"/>
     <col min="9" max="9" width="2.85546875" style="2" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="25" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="24" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" style="2" customWidth="1"/>
     <col min="15" max="15" width="13.5703125" style="2" customWidth="1"/>
     <col min="16" max="16" width="2.5703125" style="2" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" style="2" customWidth="1"/>
     <col min="18" max="18" width="2.85546875" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="25" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" style="25" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" style="25" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="25" customWidth="1"/>
-    <col min="23" max="23" width="18" style="25" customWidth="1"/>
-    <col min="24" max="25" width="14.28515625" style="25" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" style="25" customWidth="1"/>
-    <col min="27" max="28" width="11.42578125" style="25" customWidth="1"/>
-    <col min="29" max="29" width="12.42578125" style="25" customWidth="1"/>
-    <col min="30" max="30" width="11.42578125" style="25" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" style="25" customWidth="1"/>
-    <col min="32" max="32" width="14.42578125" style="25" customWidth="1"/>
-    <col min="33" max="33" width="13" style="25" customWidth="1"/>
-    <col min="34" max="38" width="11.42578125" style="25" customWidth="1"/>
-    <col min="39" max="39" width="18.140625" style="25" customWidth="1"/>
-    <col min="40" max="40" width="15.28515625" style="25" customWidth="1"/>
-    <col min="41" max="43" width="12.5703125" style="25" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" style="24" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" style="24" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" style="24" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="24" customWidth="1"/>
+    <col min="23" max="23" width="18" style="24" customWidth="1"/>
+    <col min="24" max="25" width="14.28515625" style="24" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" style="24" customWidth="1"/>
+    <col min="27" max="28" width="11.42578125" style="24" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" style="24" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" style="24" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" style="24" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="24" customWidth="1"/>
+    <col min="33" max="33" width="13" style="24" customWidth="1"/>
+    <col min="34" max="38" width="11.42578125" style="24" customWidth="1"/>
+    <col min="39" max="39" width="18.140625" style="24" customWidth="1"/>
+    <col min="40" max="40" width="15.28515625" style="24" customWidth="1"/>
+    <col min="41" max="43" width="12.5703125" style="24" customWidth="1"/>
     <col min="44" max="44" width="2.85546875" style="2" customWidth="1"/>
-    <col min="45" max="46" width="11.42578125" style="25" customWidth="1"/>
-    <col min="47" max="52" width="10.85546875" style="25" customWidth="1"/>
+    <col min="45" max="46" width="11.42578125" style="24" customWidth="1"/>
+    <col min="47" max="52" width="10.85546875" style="24" customWidth="1"/>
     <col min="53" max="53" width="2.85546875" style="2" customWidth="1"/>
     <col min="54" max="54" width="8.5703125" style="2" customWidth="1"/>
     <col min="55" max="55" width="11.28515625" style="2" customWidth="1"/>
@@ -2501,7 +3090,7 @@
       <c r="G1" s="78"/>
       <c r="H1" s="79"/>
       <c r="J1" s="74" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="K1" s="75"/>
       <c r="L1" s="75"/>
@@ -2510,7 +3099,7 @@
       <c r="O1" s="76"/>
       <c r="Q1" s="16"/>
       <c r="S1" s="83" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="T1" s="84"/>
       <c r="U1" s="84"/>
@@ -2537,7 +3126,7 @@
       <c r="AP1" s="84"/>
       <c r="AQ1" s="84"/>
       <c r="AS1" s="85" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="AT1" s="86"/>
       <c r="AU1" s="86"/>
@@ -2552,196 +3141,196 @@
       <c r="BC1" s="81"/>
       <c r="BD1" s="82"/>
       <c r="BF1" s="71" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="BG1" s="72"/>
       <c r="BH1" s="73"/>
     </row>
-    <row r="2" spans="1:60" s="65" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+    <row r="2" spans="1:60" s="63" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="60" t="s">
+      <c r="E2" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="60" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" s="61" t="s">
+      <c r="H2" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="62" t="s">
+      <c r="K2" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="62" t="s">
+      <c r="L2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="62" t="s">
+      <c r="M2" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="N2" s="62" t="s">
+      <c r="N2" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="P2" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="64" t="s">
-        <v>154</v>
-      </c>
-      <c r="T2" s="64" t="s">
+      <c r="R2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="T2" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="U2" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="U2" s="64" t="s">
-        <v>153</v>
-      </c>
-      <c r="V2" s="64" t="s">
+      <c r="V2" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="W2" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="X2" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="W2" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="X2" s="64" t="s">
-        <v>159</v>
-      </c>
-      <c r="Y2" s="64" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z2" s="64" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA2" s="64" t="s">
+      <c r="Y2" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z2" s="62" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA2" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="AB2" s="64" t="s">
+      <c r="AB2" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="AC2" s="64" t="s">
+      <c r="AC2" s="62" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD2" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE2" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF2" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG2" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH2" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI2" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ2" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK2" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="AD2" s="64" t="s">
-        <v>134</v>
-      </c>
-      <c r="AE2" s="64" t="s">
-        <v>141</v>
-      </c>
-      <c r="AF2" s="64" t="s">
-        <v>144</v>
-      </c>
-      <c r="AG2" s="64" t="s">
-        <v>145</v>
-      </c>
-      <c r="AH2" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI2" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ2" s="64" t="s">
+      <c r="AL2" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM2" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="AK2" s="64" t="s">
-        <v>150</v>
-      </c>
-      <c r="AL2" s="64" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM2" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="AN2" s="64" t="s">
+      <c r="AN2" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="AO2" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="AO2" s="64" t="s">
-        <v>170</v>
-      </c>
-      <c r="AP2" s="64" t="s">
-        <v>204</v>
-      </c>
-      <c r="AQ2" s="64" t="s">
-        <v>205</v>
-      </c>
-      <c r="AR2" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS2" s="56" t="s">
+      <c r="AP2" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ2" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="AR2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="AT2" s="56" t="s">
+      <c r="AT2" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="AU2" s="56" t="s">
+      <c r="AU2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="AV2" s="56" t="s">
+      <c r="AV2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="AW2" s="56" t="s">
+      <c r="AW2" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AX2" s="56" t="s">
+      <c r="AX2" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="56" t="s">
+      <c r="AY2" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="AZ2" s="56" t="s">
-        <v>258</v>
-      </c>
-      <c r="BA2" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="BB2" s="57" t="s">
+      <c r="AZ2" s="54" t="s">
+        <v>248</v>
+      </c>
+      <c r="BA2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="BC2" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="BD2" s="60" t="s">
+      <c r="BC2" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD2" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="BE2" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="BE2" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="BF2" s="63" t="s">
-        <v>246</v>
-      </c>
-      <c r="BG2" s="63" t="s">
-        <v>248</v>
-      </c>
-      <c r="BH2" s="63" t="s">
-        <v>247</v>
+      <c r="BF2" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="BG2" s="61" t="s">
+        <v>238</v>
+      </c>
+      <c r="BH2" s="61" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2753,7 +3342,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>66</v>
@@ -2762,154 +3351,154 @@
         <v>62</v>
       </c>
       <c r="H3" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="L3" s="25" t="s">
+      <c r="K3" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="L3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="24" t="s">
         <v>58</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="S3" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="T3" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="U3" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="U3" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="V3" s="25" t="s">
+      <c r="V3" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="W3" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="X3" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="W3" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="X3" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y3" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z3" s="25" t="s">
-        <v>262</v>
-      </c>
-      <c r="AA3" s="25" t="s">
+      <c r="Y3" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z3" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AB3" s="25" t="s">
+      <c r="AB3" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AC3" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD3" s="25" t="s">
+      <c r="AC3" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="AE3" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="AF3" s="25" t="s">
+      <c r="AD3" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE3" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF3" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG3" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="AG3" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="AH3" s="25" t="s">
+      <c r="AH3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="AI3" s="25" t="s">
+      <c r="AI3" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="AJ3" s="25" t="s">
+      <c r="AJ3" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK3" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="AK3" s="25" t="s">
+      <c r="AL3" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AL3" s="25" t="s">
+      <c r="AM3" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="AM3" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="AN3" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO3" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="AP3" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="AQ3" s="25" t="s">
-        <v>207</v>
+      <c r="AN3" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AO3" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="AP3" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="AQ3" s="24" t="s">
+        <v>203</v>
       </c>
       <c r="AR3" s="3"/>
-      <c r="AS3" s="25" t="s">
+      <c r="AS3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="AT3" s="25" t="s">
+      <c r="AT3" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AU3" s="25" t="s">
+      <c r="AU3" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AV3" s="25" t="s">
+      <c r="AV3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AW3" s="25" t="s">
+      <c r="AW3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AX3" s="25" t="s">
+      <c r="AX3" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AY3" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="AZ3" s="25" t="s">
-        <v>259</v>
+      <c r="AY3" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="AZ3" s="24" t="s">
+        <v>249</v>
       </c>
       <c r="BA3" s="3"/>
-      <c r="BB3" s="55" t="s">
-        <v>71</v>
+      <c r="BB3" s="53" t="s">
+        <v>70</v>
       </c>
       <c r="BC3" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BD3" s="3" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="BF3" s="2" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="BG3" s="2" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="BH3" s="2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -2921,7 +3510,7 @@
         <v>54</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>66</v>
@@ -2930,149 +3519,149 @@
         <v>62</v>
       </c>
       <c r="H4" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="K4" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="L4" s="25" t="s">
+      <c r="K4" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="L4" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="24" t="s">
         <v>58</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="S4" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="T4" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="U4" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="U4" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="V4" s="25" t="s">
+      <c r="V4" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="W4" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="X4" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="X4" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y4" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z4" s="25" t="s">
-        <v>262</v>
-      </c>
-      <c r="AA4" s="25" t="s">
+      <c r="Y4" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z4" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AB4" s="25" t="s">
+      <c r="AB4" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AC4" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD4" s="25" t="s">
+      <c r="AC4" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="AE4" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="AF4" s="25" t="s">
+      <c r="AD4" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE4" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF4" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG4" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="AG4" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="AH4" s="25" t="s">
+      <c r="AH4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="AI4" s="25" t="s">
+      <c r="AI4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="AJ4" s="25" t="s">
+      <c r="AJ4" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK4" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="AK4" s="25" t="s">
+      <c r="AL4" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AL4" s="25" t="s">
+      <c r="AM4" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="AM4" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="AN4" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO4" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="AP4" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="AQ4" s="25" t="s">
-        <v>207</v>
+      <c r="AN4" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AO4" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="AP4" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="AQ4" s="24" t="s">
+        <v>203</v>
       </c>
       <c r="AR4" s="3"/>
-      <c r="AS4" s="25" t="s">
+      <c r="AS4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="AT4" s="25" t="s">
+      <c r="AT4" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AU4" s="25" t="s">
+      <c r="AU4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AV4" s="25" t="s">
+      <c r="AV4" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AW4" s="25" t="s">
+      <c r="AW4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AX4" s="25" t="s">
+      <c r="AX4" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AY4" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="AZ4" s="25" t="s">
-        <v>259</v>
+      <c r="AY4" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="AZ4" s="24" t="s">
+        <v>249</v>
       </c>
       <c r="BA4" s="3"/>
-      <c r="BB4" s="55" t="s">
-        <v>71</v>
+      <c r="BB4" s="53" t="s">
+        <v>70</v>
       </c>
       <c r="BC4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BD4" s="3" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="BF4" s="2" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="BG4" s="2" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="BH4" s="2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3086,76 +3675,76 @@
     <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <conditionalFormatting sqref="BD3:BD65537">
-    <cfRule type="cellIs" dxfId="43" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC3:BC65537">
-    <cfRule type="cellIs" dxfId="42" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G65537">
-    <cfRule type="beginsWith" dxfId="41" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="82" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(G3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="44" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="81" priority="44" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(G3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="39" priority="45" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="80" priority="45" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(G3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="46" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="79" priority="46" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(G3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="37" priority="81" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="78" priority="81" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(G3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="82" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="77" priority="82" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(G3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="35" priority="83" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="76" priority="83" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(G3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="84" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="75" priority="84" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(G3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="33" priority="85" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="74" priority="85" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(G3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="32" priority="86" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="73" priority="86" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(G3,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H65537">
-    <cfRule type="beginsWith" dxfId="31" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="72" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(H3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="71" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(H3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="29" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="70" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(H3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="69" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(H3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="27" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="68" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(H3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="67" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(H3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="25" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="66" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(H3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="65" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(H3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="23" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="64" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(H3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="63" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(H3,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3165,6 +3754,544 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4AF4D88-A2FE-49F7-BA56-67537EE8F9C0}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="24" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="77"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
+      <c r="J1" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="L1" s="85" t="s">
+        <v>195</v>
+      </c>
+      <c r="M1" s="86"/>
+      <c r="O1" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="63" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="62" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="53" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="53" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:O4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="L1:M1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G3:G65537">
+    <cfRule type="beginsWith" dxfId="62" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
+      <formula>LEFT(G3,LEN("14"))="14"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="61" priority="14" stopIfTrue="1" operator="beginsWith" text="6">
+      <formula>LEFT(G3,LEN("6"))="6"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="60" priority="15" stopIfTrue="1" operator="beginsWith" text="5">
+      <formula>LEFT(G3,LEN("5"))="5"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="59" priority="16" stopIfTrue="1" operator="beginsWith" text="4">
+      <formula>LEFT(G3,LEN("4"))="4"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="58" priority="17" stopIfTrue="1" operator="beginsWith" text="24">
+      <formula>LEFT(G3,LEN("24"))="24"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="57" priority="18" stopIfTrue="1" operator="beginsWith" text="27">
+      <formula>LEFT(G3,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="56" priority="19" stopIfTrue="1" operator="beginsWith" text="3">
+      <formula>LEFT(G3,LEN("3"))="3"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="55" priority="20" stopIfTrue="1" operator="beginsWith" text="23">
+      <formula>LEFT(G3,LEN("23"))="23"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="54" priority="21" stopIfTrue="1" operator="beginsWith" text="22">
+      <formula>LEFT(G3,LEN("22"))="22"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="53" priority="22" stopIfTrue="1" operator="beginsWith" text="21">
+      <formula>LEFT(G3,LEN("21"))="21"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H65537">
+    <cfRule type="beginsWith" dxfId="52" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+      <formula>LEFT(H3,LEN("14"))="14"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="51" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+      <formula>LEFT(H3,LEN("6"))="6"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="50" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+      <formula>LEFT(H3,LEN("5"))="5"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="49" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+      <formula>LEFT(H3,LEN("4"))="4"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="48" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+      <formula>LEFT(H3,LEN("24"))="24"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="47" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+      <formula>LEFT(H3,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="46" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+      <formula>LEFT(H3,LEN("3"))="3"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="45" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+      <formula>LEFT(H3,LEN("23"))="23"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="44" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+      <formula>LEFT(H3,LEN("22"))="22"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="43" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+      <formula>LEFT(H3,LEN("21"))="21"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9262F3-02D4-4D2E-B770-3ACC77A93DB9}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="2" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" style="2" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" style="24" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="77"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
+      <c r="J1" s="87" t="s">
+        <v>194</v>
+      </c>
+      <c r="K1" s="88"/>
+      <c r="M1" s="89" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" s="90"/>
+      <c r="P1" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="82"/>
+    </row>
+    <row r="2" spans="1:17" s="63" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="K2" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="L2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:Q4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="Q3:Q65537">
+    <cfRule type="cellIs" dxfId="42" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G65537">
+    <cfRule type="beginsWith" dxfId="41" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
+      <formula>LEFT(G3,LEN("14"))="14"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="40" priority="14" stopIfTrue="1" operator="beginsWith" text="6">
+      <formula>LEFT(G3,LEN("6"))="6"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="39" priority="15" stopIfTrue="1" operator="beginsWith" text="5">
+      <formula>LEFT(G3,LEN("5"))="5"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="38" priority="16" stopIfTrue="1" operator="beginsWith" text="4">
+      <formula>LEFT(G3,LEN("4"))="4"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="37" priority="17" stopIfTrue="1" operator="beginsWith" text="24">
+      <formula>LEFT(G3,LEN("24"))="24"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="36" priority="18" stopIfTrue="1" operator="beginsWith" text="27">
+      <formula>LEFT(G3,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="35" priority="19" stopIfTrue="1" operator="beginsWith" text="3">
+      <formula>LEFT(G3,LEN("3"))="3"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="34" priority="20" stopIfTrue="1" operator="beginsWith" text="23">
+      <formula>LEFT(G3,LEN("23"))="23"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="33" priority="21" stopIfTrue="1" operator="beginsWith" text="22">
+      <formula>LEFT(G3,LEN("22"))="22"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="32" priority="22" stopIfTrue="1" operator="beginsWith" text="21">
+      <formula>LEFT(G3,LEN("21"))="21"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H65537">
+    <cfRule type="beginsWith" dxfId="31" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+      <formula>LEFT(H3,LEN("14"))="14"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="30" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+      <formula>LEFT(H3,LEN("6"))="6"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="29" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+      <formula>LEFT(H3,LEN("5"))="5"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="28" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+      <formula>LEFT(H3,LEN("4"))="4"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="27" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+      <formula>LEFT(H3,LEN("24"))="24"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="26" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+      <formula>LEFT(H3,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="25" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+      <formula>LEFT(H3,LEN("3"))="3"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="24" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+      <formula>LEFT(H3,LEN("23"))="23"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="23" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+      <formula>LEFT(H3,LEN("22"))="22"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="22" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+      <formula>LEFT(H3,LEN("21"))="21"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7538287E-FE68-490E-9491-325968B2172B}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -3175,7 +4302,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3191,7 +4318,7 @@
     <col min="10" max="10" width="88" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="30" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="28" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
@@ -3205,51 +4332,51 @@
         <v>17</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="66" t="s">
-        <v>73</v>
+      <c r="G1" s="64" t="s">
+        <v>72</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="I2" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="J2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -3271,638 +4398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E839BC-6F29-4F14-B58D-1E2088939687}">
-  <sheetPr codeName="Feuil2">
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="8" max="11" width="11.42578125" style="25" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="2.5703125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:O3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B21C5B7-5B9C-4DD6-AED7-1EA1BDB21D53}">
-  <sheetPr codeName="Feuil3">
-    <tabColor theme="8" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:AC3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="25" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="25" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="25" customWidth="1"/>
-    <col min="12" max="12" width="18" style="25" customWidth="1"/>
-    <col min="13" max="14" width="14.28515625" style="25" customWidth="1"/>
-    <col min="15" max="16" width="11.42578125" style="25" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="25" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="25" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" style="25" customWidth="1"/>
-    <col min="20" max="21" width="13" style="25" customWidth="1"/>
-    <col min="22" max="26" width="11.42578125" style="25" customWidth="1"/>
-    <col min="27" max="27" width="18.140625" style="25" customWidth="1"/>
-    <col min="28" max="28" width="15.28515625" style="25" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" style="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="X1" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y1" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z1" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA1" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="AC1" s="26" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="R2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="S2" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="T2" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="U2" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="V2" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="W2" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="X2" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y2" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z2" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA2" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB2" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC2" s="25" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="M3" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="O3" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="R3" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="S3" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="T3" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="U3" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="V3" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="W3" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="X3" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y3" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z3" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA3" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB3" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC3" s="25" t="s">
-        <v>173</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:AC3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC055CEB-F8BF-4FEF-96B7-58AA4EBF5327}">
-  <sheetPr codeName="Feuil4">
-    <tabColor theme="9" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:N3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="2" customWidth="1"/>
-    <col min="8" max="14" width="11.42578125" style="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:N3" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626E417A-45EE-4D6C-95FD-A71D343FE19B}">
   <sheetPr codeName="Feuil5">
     <tabColor rgb="FFFFC000"/>
@@ -3943,13 +4439,13 @@
         <v>17</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>65</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>18</v>
@@ -3961,7 +4457,7 @@
         <v>20</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>22</v>
@@ -3970,9 +4466,9 @@
         <v>21</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="17" t="s">
@@ -3982,22 +4478,22 @@
         <v>9</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="R1" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="S1" s="26" t="s">
-        <v>145</v>
-      </c>
       <c r="T1" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U1" s="18" t="s">
         <v>26</v>
@@ -4020,7 +4516,7 @@
         <v>61</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>67</v>
@@ -4053,19 +4549,19 @@
         <v>29</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="2" t="s">
@@ -4081,7 +4577,7 @@
         <v>34</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4098,7 +4594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86524C9-1323-498D-ABE2-77D2F4C73D5A}">
   <sheetPr codeName="Feuil6">
     <tabColor theme="4"/>
@@ -4115,7 +4611,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="67" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="65" customWidth="1"/>
     <col min="3" max="3" width="3" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
@@ -4146,177 +4642,177 @@
       <c r="C1" s="8"/>
       <c r="E1" s="2"/>
       <c r="F1" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="87" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
+        <v>72</v>
+      </c>
+      <c r="L1" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="92"/>
+      <c r="N1" s="93"/>
       <c r="O1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="P1" s="87" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="95"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="91" t="s">
+        <v>128</v>
+      </c>
+      <c r="U1" s="94"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="94" t="s">
         <v>129</v>
       </c>
-      <c r="U1" s="90"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="90" t="s">
-        <v>130</v>
-      </c>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="91"/>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="95"/>
       <c r="Z1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA1" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA1" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="89"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="93"/>
     </row>
     <row r="2" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="8"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="39"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="34"/>
+      <c r="L2" s="32"/>
       <c r="M2" s="10"/>
-      <c r="N2" s="37"/>
+      <c r="N2" s="35"/>
       <c r="O2" s="20"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="35"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="20"/>
-      <c r="AA2" s="36"/>
+      <c r="AA2" s="34"/>
       <c r="AB2" s="10"/>
-      <c r="AC2" s="37"/>
+      <c r="AC2" s="35"/>
     </row>
-    <row r="3" spans="1:35" s="30" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" s="28" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="40" t="s">
+      <c r="O3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="P3" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="Q3" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="P3" s="40" t="s">
+      <c r="R3" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="T3" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="40" t="s">
+      <c r="U3" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="S3" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="T3" s="40" t="s">
+      <c r="V3" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="W3" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="U3" s="40" t="s">
+      <c r="X3" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="W3" s="31" t="s">
+      <c r="Y3" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA3" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="X3" s="40" t="s">
+      <c r="AB3" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Y3" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z3" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA3" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB3" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC3" s="40" t="s">
-        <v>94</v>
+      <c r="AC3" s="38" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>208</v>
-      </c>
-      <c r="B4" s="67" t="s">
-        <v>213</v>
+        <v>204</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>209</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
@@ -4326,73 +4822,73 @@
         <v>55</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="N4" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2">
         <v>1</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="AI4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -4459,7 +4955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64634AA-9071-4111-8E53-9AF735BF36D3}">
   <sheetPr codeName="Feuil7">
     <tabColor theme="4"/>
@@ -4470,7 +4966,7 @@
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4488,9 +4984,9 @@
     <col min="11" max="11" width="12.42578125" style="2" customWidth="1"/>
     <col min="12" max="12" width="7.5703125" style="2" customWidth="1"/>
     <col min="13" max="13" width="2.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" style="30" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="2.85546875" customWidth="1"/>
     <col min="18" max="18" width="9.5703125" style="2" customWidth="1"/>
     <col min="19" max="19" width="7" style="2" customWidth="1"/>
@@ -4510,210 +5006,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50"/>
+      <c r="A1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>26</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="88"/>
-      <c r="P1" s="89"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="93"/>
       <c r="Q1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="87" t="s">
-        <v>133</v>
-      </c>
-      <c r="S1" s="90"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="87" t="s">
-        <v>191</v>
-      </c>
-      <c r="W1" s="90"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="87" t="s">
-        <v>192</v>
-      </c>
-      <c r="AA1" s="90"/>
-      <c r="AB1" s="91"/>
+        <v>72</v>
+      </c>
+      <c r="R1" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="94"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="91" t="s">
+        <v>187</v>
+      </c>
+      <c r="W1" s="94"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA1" s="94"/>
+      <c r="AB1" s="95"/>
       <c r="AC1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD1" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD1" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="89"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="93"/>
     </row>
     <row r="2" spans="1:32" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="39"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="45"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="37"/>
       <c r="M2" s="20"/>
-      <c r="N2" s="36"/>
+      <c r="N2" s="34"/>
       <c r="O2" s="10"/>
-      <c r="P2" s="37"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="20"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="35"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="33"/>
       <c r="AC2" s="20"/>
-      <c r="AD2" s="36"/>
+      <c r="AD2" s="34"/>
       <c r="AE2" s="10"/>
-      <c r="AF2" s="37"/>
+      <c r="AF2" s="35"/>
     </row>
-    <row r="3" spans="1:32" s="70" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:32" s="68" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="42" t="s">
         <v>65</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="E3" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="42" t="s">
+      <c r="G3" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="J3" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="K3" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="L3" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="N3" s="69" t="s">
+      <c r="M3" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="69" t="s">
+      <c r="O3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="69" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q3" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="R3" s="69" t="s">
+      <c r="P3" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q3" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="R3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="S3" s="69" t="s">
+      <c r="S3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="T3" s="69" t="s">
-        <v>94</v>
-      </c>
-      <c r="U3" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="V3" s="69" t="s">
+      <c r="T3" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="U3" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="V3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="W3" s="69" t="s">
+      <c r="W3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="69" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y3" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z3" s="69" t="s">
+      <c r="X3" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y3" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="AA3" s="69" t="s">
+      <c r="AA3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="AB3" s="69" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC3" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD3" s="69" t="s">
+      <c r="AB3" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC3" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="AE3" s="69" t="s">
+      <c r="AE3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="AF3" s="69" t="s">
-        <v>94</v>
+      <c r="AF3" s="67" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>25</v>
@@ -4722,65 +5218,65 @@
         <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="M4" s="1"/>
+      <c r="N4" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="R4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="S4" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="V4" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB4" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="O4" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="S4" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="AD4" s="2">
         <v>1</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4845,4 +5341,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9364C085-89A2-4191-BD71-23274096DEBB}">
+  <sheetPr codeName="Feuil8"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fusion PSC1/AFPS dans "Synthèse par unité" #17
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E814D78F-738C-4062-8086-CA02E9FBE1FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43A564C-3952-42AA-AD55-8272DFF21E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1005" windowWidth="22230" windowHeight="15240" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="750" yWindow="525" windowWidth="22230" windowHeight="15240" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quota année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Quota unités'!$A$3:$AF$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BH$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Synthèse par unité'!$A$1:$Y$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Synthèse par unité'!$A$1:$X$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="261">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -141,12 +141,6 @@
   </si>
   <si>
     <t>${unite.appro}</t>
-  </si>
-  <si>
-    <t>${unite.psc1}</t>
-  </si>
-  <si>
-    <t>${unite.afps}</t>
   </si>
   <si>
     <t>${unite.dirsf}</t>
@@ -1465,7 +1459,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="107">
+  <dxfs count="85">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2253,226 +2247,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF007E39"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF007E39"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2867,107 +2641,107 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="50" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="50" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="50" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="50" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2993,7 +2767,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="23">
         <v>43766</v>
@@ -3001,18 +2775,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3090,7 +2864,7 @@
       <c r="G1" s="78"/>
       <c r="H1" s="79"/>
       <c r="J1" s="74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K1" s="75"/>
       <c r="L1" s="75"/>
@@ -3099,7 +2873,7 @@
       <c r="O1" s="76"/>
       <c r="Q1" s="16"/>
       <c r="S1" s="83" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="T1" s="84"/>
       <c r="U1" s="84"/>
@@ -3126,7 +2900,7 @@
       <c r="AP1" s="84"/>
       <c r="AQ1" s="84"/>
       <c r="AS1" s="85" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AT1" s="86"/>
       <c r="AU1" s="86"/>
@@ -3141,7 +2915,7 @@
       <c r="BC1" s="81"/>
       <c r="BD1" s="82"/>
       <c r="BF1" s="71" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BG1" s="72"/>
       <c r="BH1" s="73"/>
@@ -3160,70 +2934,70 @@
         <v>17</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H2" s="58" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I2" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="60" t="s">
+      <c r="L2" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="60" t="s">
+      <c r="M2" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="60" t="s">
-        <v>76</v>
-      </c>
       <c r="N2" s="60" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O2" s="60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="61" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S2" s="62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="T2" s="62" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U2" s="62" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="V2" s="62" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="W2" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="X2" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y2" s="62" t="s">
         <v>161</v>
       </c>
-      <c r="X2" s="62" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y2" s="62" t="s">
-        <v>163</v>
-      </c>
       <c r="Z2" s="62" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AA2" s="62" t="s">
         <v>8</v>
@@ -3232,19 +3006,19 @@
         <v>9</v>
       </c>
       <c r="AC2" s="62" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AD2" s="62" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AE2" s="62" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AF2" s="62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AG2" s="62" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AH2" s="62" t="s">
         <v>10</v>
@@ -3253,31 +3027,31 @@
         <v>11</v>
       </c>
       <c r="AJ2" s="62" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AK2" s="62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AL2" s="62" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AM2" s="62" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AN2" s="62" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AO2" s="62" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AP2" s="62" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AQ2" s="62" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AR2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AS2" s="54" t="s">
         <v>12</v>
@@ -3301,36 +3075,36 @@
         <v>16</v>
       </c>
       <c r="AZ2" s="54" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="BA2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="BB2" s="55" t="s">
         <v>5</v>
       </c>
       <c r="BC2" s="58" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="BD2" s="58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="BE2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="BF2" s="61" t="s">
+        <v>234</v>
+      </c>
+      <c r="BG2" s="61" t="s">
         <v>236</v>
       </c>
-      <c r="BG2" s="61" t="s">
-        <v>238</v>
-      </c>
       <c r="BH2" s="61" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3339,166 +3113,166 @@
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="S3" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="T3" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="U3" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="T3" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>156</v>
-      </c>
       <c r="V3" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="W3" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="X3" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y3" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="X3" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y3" s="24" t="s">
-        <v>164</v>
-      </c>
       <c r="Z3" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AA3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC3" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD3" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE3" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF3" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG3" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AB3" s="24" t="s">
+      <c r="AI3" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AC3" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD3" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="AE3" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="AF3" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG3" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI3" s="24" t="s">
-        <v>45</v>
-      </c>
       <c r="AJ3" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK3" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL3" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="AK3" s="24" t="s">
+      <c r="AM3" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="AL3" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM3" s="24" t="s">
-        <v>111</v>
-      </c>
       <c r="AN3" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AO3" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AP3" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AQ3" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AR3" s="3"/>
       <c r="AS3" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT3" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="AT3" s="24" t="s">
+      <c r="AV3" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AU3" s="24" t="s">
+      <c r="AW3" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX3" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AV3" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="AW3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX3" s="24" t="s">
-        <v>50</v>
-      </c>
       <c r="AY3" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AZ3" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="BA3" s="3"/>
       <c r="BB3" s="53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BC3" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="BD3" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="BG3" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="BF3" s="2" t="s">
+      <c r="BH3" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="BG3" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="BH3" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3507,161 +3281,161 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="S4" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="T4" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="U4" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="T4" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="U4" s="24" t="s">
-        <v>156</v>
-      </c>
       <c r="V4" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="W4" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="X4" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y4" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="X4" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y4" s="24" t="s">
-        <v>164</v>
-      </c>
       <c r="Z4" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AA4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB4" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC4" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD4" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE4" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF4" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG4" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AB4" s="24" t="s">
+      <c r="AI4" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AC4" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD4" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="AE4" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="AF4" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG4" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH4" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI4" s="24" t="s">
-        <v>45</v>
-      </c>
       <c r="AJ4" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK4" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL4" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="AK4" s="24" t="s">
+      <c r="AM4" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="AL4" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM4" s="24" t="s">
-        <v>111</v>
-      </c>
       <c r="AN4" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AO4" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AP4" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AQ4" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AR4" s="3"/>
       <c r="AS4" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT4" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="AT4" s="24" t="s">
+      <c r="AV4" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AU4" s="24" t="s">
+      <c r="AW4" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="AV4" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="AW4" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX4" s="24" t="s">
-        <v>50</v>
-      </c>
       <c r="AY4" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AZ4" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="BA4" s="3"/>
       <c r="BB4" s="53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BC4" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="BD4" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="BG4" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="BF4" s="2" t="s">
+      <c r="BH4" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="BG4" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="BH4" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3794,10 +3568,10 @@
       <c r="G1" s="78"/>
       <c r="H1" s="79"/>
       <c r="J1" s="69" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M1" s="86"/>
       <c r="O1" s="70" t="s">
@@ -3818,25 +3592,25 @@
         <v>17</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H2" s="58" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J2" s="62" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L2" s="54" t="s">
         <v>12</v>
@@ -3845,7 +3619,7 @@
         <v>26</v>
       </c>
       <c r="N2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O2" s="55" t="s">
         <v>5</v>
@@ -3853,7 +3627,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3862,39 +3636,39 @@
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="53" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3903,34 +3677,34 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="53" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4050,11 +3824,11 @@
       <c r="G1" s="78"/>
       <c r="H1" s="79"/>
       <c r="J1" s="87" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K1" s="88"/>
       <c r="M1" s="89" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N1" s="90"/>
       <c r="P1" s="80" t="s">
@@ -4076,28 +3850,28 @@
         <v>17</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H2" s="58" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J2" s="62" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K2" s="62" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M2" s="54" t="s">
         <v>12</v>
@@ -4106,18 +3880,18 @@
         <v>26</v>
       </c>
       <c r="O2" s="59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P2" s="55" t="s">
         <v>5</v>
       </c>
       <c r="Q2" s="58" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4126,45 +3900,45 @@
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N3" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4173,40 +3947,40 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -4332,51 +4106,51 @@
         <v>17</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G1" s="64" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="J2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -4403,7 +4177,7 @@
   <sheetPr codeName="Feuil5">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
@@ -4434,18 +4208,18 @@
     <col min="20" max="20" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>18</v>
@@ -4457,7 +4231,7 @@
         <v>20</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>22</v>
@@ -4466,7 +4240,7 @@
         <v>21</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>7</v>
@@ -4478,48 +4252,45 @@
         <v>9</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Q1" s="25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="R1" s="25" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="S1" s="25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="T1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y1" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
@@ -4529,14 +4300,14 @@
         <v>24</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="2" t="s">
@@ -4549,46 +4320,43 @@
         <v>29</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="R4" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y1" xr:uid="{66A8F9AA-9955-4F38-8C09-E2219E483C8B}"/>
+  <autoFilter ref="A1:X1" xr:uid="{66A8F9AA-9955-4F38-8C09-E2219E483C8B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4642,52 +4410,52 @@
       <c r="C1" s="8"/>
       <c r="E1" s="2"/>
       <c r="F1" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L1" s="91" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M1" s="92"/>
       <c r="N1" s="93"/>
       <c r="O1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P1" s="91" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q1" s="94"/>
       <c r="R1" s="95"/>
       <c r="S1" s="26"/>
       <c r="T1" s="91" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U1" s="94"/>
       <c r="V1" s="95"/>
       <c r="W1" s="94" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="X1" s="94"/>
       <c r="Y1" s="95"/>
       <c r="Z1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA1" s="96" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AB1" s="92"/>
       <c r="AC1" s="93"/>
@@ -4722,173 +4490,173 @@
     </row>
     <row r="3" spans="1:35" s="28" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="38" t="s">
-        <v>93</v>
-      </c>
       <c r="O3" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P3" s="38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q3" s="38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R3" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="S3" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="T3" s="38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U3" s="38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="V3" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W3" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X3" s="38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Y3" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Z3" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA3" s="38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AB3" s="38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AC3" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2">
         <v>1</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="AE4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI4" t="s">
         <v>205</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -5013,56 +4781,56 @@
       <c r="E1" s="47"/>
       <c r="F1" s="48"/>
       <c r="G1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I1" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>184</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>186</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>26</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N1" s="96" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O1" s="92"/>
       <c r="P1" s="93"/>
       <c r="Q1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R1" s="91" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S1" s="94"/>
       <c r="T1" s="95"/>
       <c r="U1" s="26"/>
       <c r="V1" s="91" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="W1" s="94"/>
       <c r="X1" s="95"/>
       <c r="Y1" s="39"/>
       <c r="Z1" s="91" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA1" s="94"/>
       <c r="AB1" s="95"/>
       <c r="AC1" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AD1" s="96" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AE1" s="92"/>
       <c r="AF1" s="93"/>
@@ -5105,13 +4873,13 @@
         <v>17</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>18</v>
@@ -5120,96 +4888,96 @@
         <v>19</v>
       </c>
       <c r="G3" s="66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H3" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="K3" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="L3" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="L3" s="40" t="s">
-        <v>97</v>
-      </c>
       <c r="M3" s="66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N3" s="67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O3" s="67" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P3" s="67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R3" s="67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S3" s="67" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T3" s="67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="U3" s="66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="V3" s="67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W3" s="67" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="X3" s="67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Y3" s="66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z3" s="67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AA3" s="67" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB3" s="67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AC3" s="66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AD3" s="67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AE3" s="67" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AF3" s="67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>173</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>25</v>
@@ -5218,65 +4986,65 @@
         <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O4" s="30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="S4" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="S4" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="T4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB4" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="AD4" s="2">
         <v>1</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -5358,19 +5126,19 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout d'une option "DDCS" #45
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8268E41E-9D07-43BC-B21F-33F164A9E06C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A516EB-2665-45B6-8418-C202C4404ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="735" windowWidth="24630" windowHeight="13710" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="900" yWindow="705" windowWidth="24630" windowHeight="13710" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -21,12 +21,14 @@
     <sheet name="Synthèse par unité" sheetId="3" r:id="rId6"/>
     <sheet name="Quota année" sheetId="8" r:id="rId7"/>
     <sheet name="Quota unités" sheetId="2" r:id="rId8"/>
-    <sheet name="Global" sheetId="9" r:id="rId9"/>
-    <sheet name="Général" sheetId="10" r:id="rId10"/>
+    <sheet name="Déclaration DDCS" sheetId="17" r:id="rId9"/>
+    <sheet name="Global" sheetId="9" r:id="rId10"/>
+    <sheet name="Général" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Alertes!$A$1:$K$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compas!$A$2:$P$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Déclaration DDCS'!$A$2:$S$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Farfadets!$A$2:$N$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quota année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Quota unités'!$A$3:$AG$3</definedName>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="271">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -874,6 +876,12 @@
   </si>
   <si>
     <t>${unite.branche}</t>
+  </si>
+  <si>
+    <t>Feuille "Déclaration DDCS"</t>
+  </si>
+  <si>
+    <t>Indique les éléments à utiliser pour la déclaration trimestrielle de la DDCS</t>
   </si>
 </sst>
 </file>
@@ -1507,7 +1515,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="123">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1524,6 +1562,66 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
@@ -1554,6 +1652,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
@@ -1574,6 +1682,76 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1584,6 +1762,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1674,6 +1872,106 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
@@ -1734,6 +2032,36 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1744,6 +2072,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1754,467 +2102,17 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3166,7 +3064,7 @@
   <sheetPr codeName="Feuil10">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -3282,6 +3180,16 @@
         <v>220</v>
       </c>
     </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="43" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="44" t="s">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3289,6 +3197,42 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9364C085-89A2-4191-BD71-23274096DEBB}">
+  <sheetPr codeName="Feuil8"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AFD6E7-296C-4D2D-8BB3-DCE2EA8A2647}">
   <sheetPr codeName="Feuil9">
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -4009,76 +3953,76 @@
     <mergeCell ref="BE1:BF1"/>
   </mergeCells>
   <conditionalFormatting sqref="BC3:BF65537">
-    <cfRule type="cellIs" dxfId="133" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB3:BB65537">
-    <cfRule type="cellIs" dxfId="132" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G65537">
-    <cfRule type="beginsWith" dxfId="131" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="120" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(G3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="44" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="119" priority="44" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(G3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="129" priority="45" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="118" priority="45" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(G3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="128" priority="46" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="117" priority="46" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(G3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="127" priority="81" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="116" priority="81" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(G3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="126" priority="82" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="115" priority="82" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(G3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="125" priority="83" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="114" priority="83" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(G3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="124" priority="84" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="113" priority="84" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(G3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="123" priority="85" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="112" priority="85" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(G3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="122" priority="86" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="111" priority="86" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(G3,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H65537">
-    <cfRule type="beginsWith" dxfId="121" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="110" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(H3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="120" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="109" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(H3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="119" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="108" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(H3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="118" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="107" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(H3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="117" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="106" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(H3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="116" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="105" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(H3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="115" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="104" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(H3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="114" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="103" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(H3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="113" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="102" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(H3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="112" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="101" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(H3,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4264,66 +4208,66 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G65537">
-    <cfRule type="beginsWith" dxfId="111" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="100" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(G3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="110" priority="14" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="99" priority="14" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(G3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="109" priority="15" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="98" priority="15" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(G3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="108" priority="16" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="97" priority="16" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(G3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="107" priority="17" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="96" priority="17" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(G3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="106" priority="18" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="95" priority="18" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(G3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="105" priority="19" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="94" priority="19" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(G3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="104" priority="20" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="93" priority="20" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(G3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="103" priority="21" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="92" priority="21" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(G3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="22" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="91" priority="22" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(G3,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H65537">
-    <cfRule type="beginsWith" dxfId="101" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="90" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(H3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="100" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="89" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(H3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="99" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="88" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(H3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="87" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(H3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="97" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="86" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(H3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="85" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(H3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="95" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="84" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(H3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="83" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(H3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="93" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="82" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(H3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="92" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="81" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(H3,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4532,71 +4476,71 @@
     <mergeCell ref="O1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="P3:P65537">
-    <cfRule type="cellIs" dxfId="91" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G65537">
-    <cfRule type="beginsWith" dxfId="90" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="79" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(G3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="89" priority="14" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="78" priority="14" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(G3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="15" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="77" priority="15" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(G3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="87" priority="16" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="76" priority="16" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(G3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="17" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="75" priority="17" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(G3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="85" priority="18" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="74" priority="18" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(G3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="84" priority="19" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="73" priority="19" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(G3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="83" priority="20" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="72" priority="20" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(G3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="82" priority="21" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="71" priority="21" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(G3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="81" priority="22" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="70" priority="22" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(G3,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H65537">
-    <cfRule type="beginsWith" dxfId="80" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="69" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(H3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="79" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="68" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(H3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="67" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(H3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="77" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="66" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(H3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="65" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(H3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="75" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="64" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(H3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="74" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="63" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(H3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="73" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="62" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(H3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="72" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="61" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(H3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="71" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="60" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(H3,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4705,35 +4649,35 @@
   </sheetData>
   <autoFilter ref="A1:K2" xr:uid="{F7D2DF7B-F46F-4C0B-92A8-F09F30ADB8E7}"/>
   <conditionalFormatting sqref="I2:I1000000">
-    <cfRule type="containsText" dxfId="61" priority="7" stopIfTrue="1" operator="containsText" text="BASSE">
+    <cfRule type="containsText" dxfId="59" priority="7" stopIfTrue="1" operator="containsText" text="BASSE">
       <formula>NOT(ISERROR(SEARCH("BASSE",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="8" stopIfTrue="1" operator="containsText" text="MOYENNE">
+    <cfRule type="containsText" dxfId="58" priority="8" stopIfTrue="1" operator="containsText" text="MOYENNE">
       <formula>NOT(ISERROR(SEARCH("MOYENNE",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="9" stopIfTrue="1" operator="containsText" text="HAUTE">
+    <cfRule type="containsText" dxfId="57" priority="9" stopIfTrue="1" operator="containsText" text="HAUTE">
       <formula>NOT(ISERROR(SEARCH("HAUTE",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="beginsWith" dxfId="58" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="56" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(G2,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="57" priority="3" stopIfTrue="1" operator="beginsWith" text="F">
+    <cfRule type="beginsWith" dxfId="55" priority="3" stopIfTrue="1" operator="beginsWith" text="F">
       <formula>LEFT(G2,LEN("F"))="F"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="54" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(G2,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="55" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="53" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(G2,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="52" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(G2,LEN("LJ"))="LJ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="beginsWith" dxfId="53" priority="1" stopIfTrue="1" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="51" priority="1" stopIfTrue="1" operator="beginsWith" text="R">
       <formula>LEFT(G2,LEN("R"))="R"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4944,24 +4888,24 @@
   </sheetData>
   <autoFilter ref="A1:Z1" xr:uid="{66A8F9AA-9955-4F38-8C09-E2219E483C8B}"/>
   <conditionalFormatting sqref="D2:D65536">
-    <cfRule type="beginsWith" dxfId="43" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="50" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(D2,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="3" stopIfTrue="1" operator="beginsWith" text="F">
+    <cfRule type="beginsWith" dxfId="49" priority="3" stopIfTrue="1" operator="beginsWith" text="F">
       <formula>LEFT(D2,LEN("F"))="F"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="41" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="48" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(D2,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="47" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(D2,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="39" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="46" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(D2,LEN("LJ"))="LJ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D65536">
-    <cfRule type="beginsWith" dxfId="38" priority="1" stopIfTrue="1" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="45" priority="1" stopIfTrue="1" operator="beginsWith" text="R">
       <formula>LEFT(D2,LEN("R"))="R"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5283,47 +5227,47 @@
     <mergeCell ref="AA1:AC1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F65536">
-    <cfRule type="cellIs" dxfId="70" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G65536">
-    <cfRule type="cellIs" dxfId="69" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H65536">
-    <cfRule type="cellIs" dxfId="68" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I65536">
-    <cfRule type="cellIs" dxfId="67" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J65536">
-    <cfRule type="cellIs" dxfId="66" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N65536">
-    <cfRule type="cellIs" dxfId="65" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:V65536">
-    <cfRule type="cellIs" dxfId="64" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4:Y65536">
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC65536">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5677,74 +5621,74 @@
     <mergeCell ref="S1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="Q4:Q65537">
-    <cfRule type="cellIs" dxfId="31" priority="20" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="20" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4:U65537">
-    <cfRule type="cellIs" dxfId="30" priority="19" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="19" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4:Y65537">
-    <cfRule type="cellIs" dxfId="29" priority="18" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="18" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC65537">
-    <cfRule type="cellIs" dxfId="28" priority="17" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4:AG65537">
-    <cfRule type="cellIs" dxfId="27" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I65537">
-    <cfRule type="cellIs" dxfId="26" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J65537">
-    <cfRule type="cellIs" dxfId="25" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K65537">
-    <cfRule type="cellIs" dxfId="24" priority="9" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="9" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L65537">
-    <cfRule type="cellIs" dxfId="23" priority="8" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="8" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M65537">
-    <cfRule type="cellIs" dxfId="22" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E65536">
-    <cfRule type="beginsWith" dxfId="21" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="25" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(E4,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="3" stopIfTrue="1" operator="beginsWith" text="F">
+    <cfRule type="beginsWith" dxfId="24" priority="3" stopIfTrue="1" operator="beginsWith" text="F">
       <formula>LEFT(E4,LEN("F"))="F"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="23" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(E4,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="22" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(E4,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="17" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="21" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(E4,LEN("LJ"))="LJ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E65536">
-    <cfRule type="beginsWith" dxfId="16" priority="1" stopIfTrue="1" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text="R">
       <formula>LEFT(E4,LEN("R"))="R"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5755,36 +5699,295 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9364C085-89A2-4191-BD71-23274096DEBB}">
-  <sheetPr codeName="Feuil8"/>
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99FD4D1-5177-41C0-A1EF-29F4D55301FA}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="2" customWidth="1"/>
+    <col min="10" max="13" width="11.42578125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="2.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="6"/>
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="78"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
+      <c r="J1" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="O1" s="16"/>
+      <c r="Q1" s="72" t="s">
+        <v>230</v>
+      </c>
+      <c r="R1" s="73"/>
+      <c r="S1" s="74"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
+    <row r="2" spans="1:19" s="57" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="S2" s="55" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:S4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
+  <mergeCells count="3">
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G3:G65537">
+    <cfRule type="beginsWith" dxfId="19" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
+      <formula>LEFT(G3,LEN("14"))="14"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="18" priority="14" stopIfTrue="1" operator="beginsWith" text="6">
+      <formula>LEFT(G3,LEN("6"))="6"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="17" priority="15" stopIfTrue="1" operator="beginsWith" text="5">
+      <formula>LEFT(G3,LEN("5"))="5"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="16" stopIfTrue="1" operator="beginsWith" text="4">
+      <formula>LEFT(G3,LEN("4"))="4"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="15" priority="17" stopIfTrue="1" operator="beginsWith" text="24">
+      <formula>LEFT(G3,LEN("24"))="24"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="14" priority="18" stopIfTrue="1" operator="beginsWith" text="27">
+      <formula>LEFT(G3,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="13" priority="19" stopIfTrue="1" operator="beginsWith" text="3">
+      <formula>LEFT(G3,LEN("3"))="3"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="12" priority="20" stopIfTrue="1" operator="beginsWith" text="23">
+      <formula>LEFT(G3,LEN("23"))="23"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="11" priority="21" stopIfTrue="1" operator="beginsWith" text="22">
+      <formula>LEFT(G3,LEN("22"))="22"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="10" priority="22" stopIfTrue="1" operator="beginsWith" text="21">
+      <formula>LEFT(G3,LEN("21"))="21"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H65537">
+    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
+      <formula>LEFT(H3,LEN("14"))="14"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+      <formula>LEFT(H3,LEN("6"))="6"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="7" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+      <formula>LEFT(H3,LEN("5"))="5"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="6" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+      <formula>LEFT(H3,LEN("4"))="4"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+      <formula>LEFT(H3,LEN("24"))="24"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+      <formula>LEFT(H3,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+      <formula>LEFT(H3,LEN("3"))="3"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+      <formula>LEFT(H3,LEN("23"))="23"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+      <formula>LEFT(H3,LEN("22"))="22"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+      <formula>LEFT(H3,LEN("21"))="21"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout de couleur #43
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A516EB-2665-45B6-8418-C202C4404ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899B9538-C761-4D41-BA3A-6086E151E169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="705" windowWidth="24630" windowHeight="13710" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="24630" windowHeight="13710" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="267">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -564,36 +564,6 @@
     <t>${unite.codebranche}</t>
   </si>
   <si>
-    <t>$[P4]</t>
-  </si>
-  <si>
-    <t>$[T4]</t>
-  </si>
-  <si>
-    <t>$[X4]</t>
-  </si>
-  <si>
-    <t>$[AB4]</t>
-  </si>
-  <si>
-    <t>$[AF4]</t>
-  </si>
-  <si>
-    <t>$[O4-N4]</t>
-  </si>
-  <si>
-    <t>$[S4-R4]</t>
-  </si>
-  <si>
-    <t>$[W4-V4]</t>
-  </si>
-  <si>
-    <t>$[AA4-Z4]</t>
-  </si>
-  <si>
-    <t>$[AE4-AD4]&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>Nb animateurs et 1 dir (sauf unité rouge)</t>
   </si>
   <si>
@@ -638,15 +608,6 @@
     <t>$[F4]</t>
   </si>
   <si>
-    <t>$[CEILING($E4/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
-  </si>
-  <si>
-    <t>$[CEILING($E4*0.5/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
-  </si>
-  <si>
-    <t>$[CEILING($E4*0.8/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
-  </si>
-  <si>
     <t>FC1</t>
   </si>
   <si>
@@ -882,6 +843,33 @@
   </si>
   <si>
     <t>Indique les éléments à utiliser pour la déclaration trimestrielle de la DDCS</t>
+  </si>
+  <si>
+    <t>$[CEILING($F4/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
+  </si>
+  <si>
+    <t>$[T4-S4]</t>
+  </si>
+  <si>
+    <t>$[CEILING($F4*0.5/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
+  </si>
+  <si>
+    <t>$[CEILING($F4*0.8/12,1)+IF(ROUND((VALUE(C4)-VALUE(B4))/10,0)=3,0,1)]</t>
+  </si>
+  <si>
+    <t>$[AF4-AE4]&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>$[Q4]</t>
+  </si>
+  <si>
+    <t>$[U4]</t>
+  </si>
+  <si>
+    <t>$[AG4]</t>
+  </si>
+  <si>
+    <t>$[P4-O4]</t>
   </si>
 </sst>
 </file>
@@ -3077,117 +3065,117 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3349,7 +3337,7 @@
       <c r="G1" s="79"/>
       <c r="H1" s="80"/>
       <c r="J1" s="75" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="K1" s="76"/>
       <c r="L1" s="76"/>
@@ -3358,7 +3346,7 @@
       <c r="O1" s="77"/>
       <c r="Q1" s="16"/>
       <c r="S1" s="84" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="T1" s="85"/>
       <c r="U1" s="85"/>
@@ -3385,7 +3373,7 @@
       <c r="AP1" s="85"/>
       <c r="AQ1" s="85"/>
       <c r="AS1" s="86" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="AT1" s="87"/>
       <c r="AU1" s="87"/>
@@ -3400,11 +3388,11 @@
       <c r="BC1" s="83"/>
       <c r="BD1"/>
       <c r="BE1" s="89" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="BF1" s="90"/>
       <c r="BH1" s="72" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="BI1" s="73"/>
       <c r="BJ1" s="74"/>
@@ -3486,7 +3474,7 @@
         <v>156</v>
       </c>
       <c r="Z2" s="56" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="AA2" s="56" t="s">
         <v>8</v>
@@ -3534,16 +3522,16 @@
         <v>161</v>
       </c>
       <c r="AP2" s="56" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="AQ2" s="56" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="AR2" s="53" t="s">
         <v>65</v>
       </c>
       <c r="AS2" s="48" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="AT2" s="48" t="s">
         <v>6</v>
@@ -3561,7 +3549,7 @@
         <v>15</v>
       </c>
       <c r="AY2" s="48" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="AZ2" s="53" t="s">
         <v>65</v>
@@ -3579,22 +3567,22 @@
         <v>65</v>
       </c>
       <c r="BE2" s="65" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="BF2" s="65" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="BG2" s="53" t="s">
         <v>65</v>
       </c>
       <c r="BH2" s="55" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="BI2" s="55" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="BJ2" s="55" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.25">
@@ -3624,10 +3612,10 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>50</v>
@@ -3643,7 +3631,7 @@
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="S3" s="24" t="s">
         <v>147</v>
@@ -3667,7 +3655,7 @@
         <v>157</v>
       </c>
       <c r="Z3" s="24" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="AA3" s="24" t="s">
         <v>37</v>
@@ -3712,17 +3700,17 @@
         <v>162</v>
       </c>
       <c r="AO3" s="24" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="AP3" s="24" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="AQ3" s="24" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="AR3" s="3"/>
       <c r="AS3" s="24" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="AT3" s="24" t="s">
         <v>41</v>
@@ -3737,10 +3725,10 @@
         <v>43</v>
       </c>
       <c r="AX3" s="24" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="AY3" s="24" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="AZ3" s="3"/>
       <c r="BA3" s="47" t="s">
@@ -3750,23 +3738,23 @@
         <v>77</v>
       </c>
       <c r="BC3" s="3" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="BD3" s="3"/>
       <c r="BE3" s="3" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="BF3" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="BH3" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="BI3" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="BJ3" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
@@ -3796,10 +3784,10 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>50</v>
@@ -3815,7 +3803,7 @@
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="S4" s="24" t="s">
         <v>147</v>
@@ -3839,7 +3827,7 @@
         <v>157</v>
       </c>
       <c r="Z4" s="24" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="AA4" s="24" t="s">
         <v>37</v>
@@ -3884,17 +3872,17 @@
         <v>162</v>
       </c>
       <c r="AO4" s="24" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="AP4" s="24" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="AQ4" s="24" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="AR4" s="3"/>
       <c r="AS4" s="24" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="AT4" s="24" t="s">
         <v>41</v>
@@ -3909,10 +3897,10 @@
         <v>43</v>
       </c>
       <c r="AX4" s="24" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="AY4" s="24" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="AZ4" s="3"/>
       <c r="BA4" s="47" t="s">
@@ -3922,23 +3910,23 @@
         <v>77</v>
       </c>
       <c r="BC4" s="3" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="BD4" s="3"/>
       <c r="BE4" s="3" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="BF4" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="BH4" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="BI4" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="BJ4" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4073,10 +4061,10 @@
       <c r="G1" s="79"/>
       <c r="H1" s="80"/>
       <c r="J1" s="62" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="L1" s="64" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="N1" s="63" t="s">
         <v>5</v>
@@ -4111,13 +4099,13 @@
         <v>65</v>
       </c>
       <c r="J2" s="56" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="K2" s="53" t="s">
         <v>65</v>
       </c>
       <c r="L2" s="48" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="M2" s="53" t="s">
         <v>65</v>
@@ -4128,7 +4116,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4153,20 +4141,20 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="24" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="47" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4191,15 +4179,15 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="24" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="47" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -4319,11 +4307,11 @@
       <c r="G1" s="79"/>
       <c r="H1" s="80"/>
       <c r="J1" s="91" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="K1" s="92"/>
       <c r="M1" s="64" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="O1" s="81" t="s">
         <v>5</v>
@@ -4359,16 +4347,16 @@
         <v>65</v>
       </c>
       <c r="J2" s="56" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="K2" s="56" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="L2" s="53" t="s">
         <v>65</v>
       </c>
       <c r="M2" s="48" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="N2" s="53" t="s">
         <v>65</v>
@@ -4382,7 +4370,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4407,26 +4395,26 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="24" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="47" t="s">
         <v>63</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4451,21 +4439,21 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="24" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="47" t="s">
         <v>63</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -4598,51 +4586,51 @@
         <v>58</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="H1" s="58" t="s">
         <v>65</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="K2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="L2" s="1"/>
     </row>
@@ -4736,7 +4724,7 @@
         <v>58</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>65</v>
@@ -4784,7 +4772,7 @@
         <v>136</v>
       </c>
       <c r="T1" s="25" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="U1" s="25" t="s">
         <v>137</v>
@@ -4793,7 +4781,7 @@
         <v>65</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="X1" s="18" t="s">
         <v>10</v>
@@ -4816,7 +4804,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4" t="s">
@@ -4858,7 +4846,7 @@
         <v>139</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>140</v>
@@ -4874,7 +4862,7 @@
         <v>30</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -4972,10 +4960,10 @@
         <v>97</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="K1" s="20" t="s">
         <v>65</v>
@@ -5008,7 +4996,7 @@
         <v>65</v>
       </c>
       <c r="AA1" s="98" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="AB1" s="94"/>
       <c r="AC1" s="95"/>
@@ -5130,10 +5118,10 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
@@ -5162,7 +5150,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>110</v>
@@ -5203,13 +5191,13 @@
         <v>92</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="AI4" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -5343,16 +5331,16 @@
         <v>124</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N1" s="20" t="s">
         <v>65</v>
@@ -5372,13 +5360,13 @@
       <c r="U1" s="97"/>
       <c r="V1" s="26"/>
       <c r="W1" s="93" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="X1" s="96"/>
       <c r="Y1" s="97"/>
       <c r="Z1" s="39"/>
       <c r="AA1" s="93" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="AB1" s="96"/>
       <c r="AC1" s="97"/>
@@ -5386,7 +5374,7 @@
         <v>65</v>
       </c>
       <c r="AE1" s="98" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="AF1" s="94"/>
       <c r="AG1" s="95"/>
@@ -5439,7 +5427,7 @@
         <v>164</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="F3" s="42" t="s">
         <v>17</v>
@@ -5540,7 +5528,7 @@
         <v>165</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>24</v>
@@ -5549,19 +5537,19 @@
         <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>166</v>
+        <v>263</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>167</v>
+        <v>264</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>170</v>
+        <v>265</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="30" t="s">
@@ -5571,34 +5559,34 @@
         <v>28</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>171</v>
+        <v>266</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>189</v>
+        <v>258</v>
       </c>
       <c r="T4" s="30" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>172</v>
+        <v>259</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>190</v>
+        <v>260</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>105</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>173</v>
+        <v>113</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>191</v>
+        <v>261</v>
       </c>
       <c r="AB4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="AE4" s="2">
         <v>1</v>
@@ -5607,7 +5595,7 @@
         <v>95</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -5741,14 +5729,14 @@
       <c r="G1" s="79"/>
       <c r="H1" s="80"/>
       <c r="J1" s="75" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="K1" s="76"/>
       <c r="L1" s="76"/>
       <c r="M1" s="76"/>
       <c r="O1" s="16"/>
       <c r="Q1" s="72" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="R1" s="73"/>
       <c r="S1" s="74"/>
@@ -5803,13 +5791,13 @@
         <v>65</v>
       </c>
       <c r="Q2" s="55" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="R2" s="55" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="S2" s="55" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -5839,10 +5827,10 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>50</v>
@@ -5852,16 +5840,16 @@
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -5891,10 +5879,10 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>50</v>
@@ -5904,16 +5892,16 @@
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de FIRG #41
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Perso\dev\outilssgdf\fichiers\conf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D404BA4F-E6E6-4E0D-853B-37FD79AEF57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE96DD7E-847B-4924-ACA4-39189D26A89B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="1590" windowWidth="27030" windowHeight="16080" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1230" yWindow="495" windowWidth="23070" windowHeight="12465" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Farfadets!$A$2:$N$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quota année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Quota unités'!$A$3:$AG$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BJ$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BK$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Synthèse par unité'!$A$1:$Z$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="272">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -876,6 +876,15 @@
   </si>
   <si>
     <t>&lt;jt:forEach items="${compas}" var="chef" orderBy="codegroupe;nom;prenom"&gt;${chef.codetext}</t>
+  </si>
+  <si>
+    <t>FORMATION INITIALE RG</t>
+  </si>
+  <si>
+    <t>${chef.formation.firg.datefin}</t>
+  </si>
+  <si>
+    <t>Identification</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1216,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1434,15 +1443,6 @@
     <xf numFmtId="14" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1507,7 +1507,7 @@
   <cellStyles count="3">
     <cellStyle name="Filler1" xfId="2" xr:uid="{23D6D387-F5AE-44CD-BDE2-B1DB25CA5EB4}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="123">
     <dxf>
@@ -2759,7 +2759,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3062,7 +3062,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="155" style="44" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="44" customWidth="1"/>
@@ -3197,7 +3197,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -3235,7 +3235,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
@@ -3275,7 +3275,7 @@
   <sheetPr codeName="Feuil1">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:BJ4"/>
+  <dimension ref="A1:BK4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -3284,7 +3284,7 @@
       <selection pane="bottomRight" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -3305,36 +3305,38 @@
     <col min="21" max="21" width="14.28515625" style="24" customWidth="1"/>
     <col min="22" max="22" width="11.42578125" style="24" customWidth="1"/>
     <col min="23" max="23" width="18" style="24" customWidth="1"/>
-    <col min="24" max="25" width="14.28515625" style="24" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" style="24" customWidth="1"/>
-    <col min="27" max="28" width="11.42578125" style="24" customWidth="1"/>
-    <col min="29" max="29" width="12.42578125" style="24" customWidth="1"/>
-    <col min="30" max="30" width="11.42578125" style="24" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" style="24" customWidth="1"/>
-    <col min="32" max="32" width="14.42578125" style="24" customWidth="1"/>
-    <col min="33" max="33" width="13" style="24" customWidth="1"/>
-    <col min="34" max="38" width="11.42578125" style="24" customWidth="1"/>
-    <col min="39" max="39" width="18.140625" style="24" customWidth="1"/>
-    <col min="40" max="40" width="15.28515625" style="24" customWidth="1"/>
-    <col min="41" max="43" width="12.5703125" style="24" customWidth="1"/>
-    <col min="44" max="44" width="2.85546875" style="2" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" style="24" customWidth="1"/>
-    <col min="46" max="51" width="10.85546875" style="24" customWidth="1"/>
-    <col min="52" max="52" width="2.85546875" style="2" customWidth="1"/>
-    <col min="53" max="53" width="8.5703125" style="2" customWidth="1"/>
-    <col min="54" max="54" width="11.28515625" style="2" customWidth="1"/>
-    <col min="55" max="55" width="10.42578125" style="2" customWidth="1"/>
-    <col min="56" max="56" width="2.85546875" style="2" customWidth="1"/>
-    <col min="57" max="57" width="8" style="2" customWidth="1"/>
-    <col min="58" max="58" width="11.42578125" style="2" customWidth="1"/>
-    <col min="59" max="59" width="2.85546875" customWidth="1"/>
-    <col min="60" max="60" width="13.5703125" style="2" customWidth="1"/>
-    <col min="61" max="61" width="17.5703125" style="2" customWidth="1"/>
-    <col min="62" max="62" width="27.85546875" style="2" customWidth="1"/>
+    <col min="24" max="26" width="14.28515625" style="24" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" style="24" customWidth="1"/>
+    <col min="28" max="29" width="11.42578125" style="24" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" style="24" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="24" customWidth="1"/>
+    <col min="32" max="32" width="14.140625" style="24" customWidth="1"/>
+    <col min="33" max="33" width="14.42578125" style="24" customWidth="1"/>
+    <col min="34" max="34" width="13" style="24" customWidth="1"/>
+    <col min="35" max="39" width="11.42578125" style="24" customWidth="1"/>
+    <col min="40" max="40" width="18.140625" style="24" customWidth="1"/>
+    <col min="41" max="41" width="15.28515625" style="24" customWidth="1"/>
+    <col min="42" max="44" width="12.5703125" style="24" customWidth="1"/>
+    <col min="45" max="45" width="2.85546875" style="2" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" style="24" customWidth="1"/>
+    <col min="47" max="52" width="10.85546875" style="24" customWidth="1"/>
+    <col min="53" max="53" width="2.85546875" style="2" customWidth="1"/>
+    <col min="54" max="54" width="8.5703125" style="2" customWidth="1"/>
+    <col min="55" max="55" width="11.28515625" style="2" customWidth="1"/>
+    <col min="56" max="56" width="10.42578125" style="2" customWidth="1"/>
+    <col min="57" max="57" width="2.85546875" style="2" customWidth="1"/>
+    <col min="58" max="58" width="8" style="2" customWidth="1"/>
+    <col min="59" max="59" width="11.42578125" style="2" customWidth="1"/>
+    <col min="60" max="60" width="2.85546875" customWidth="1"/>
+    <col min="61" max="61" width="13.5703125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="17.5703125" style="2" customWidth="1"/>
+    <col min="63" max="63" width="27.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78"/>
+    <row r="1" spans="1:63" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="78" t="s">
+        <v>271</v>
+      </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
       <c r="D1" s="79"/>
@@ -3351,59 +3353,60 @@
       <c r="N1" s="76"/>
       <c r="O1" s="77"/>
       <c r="Q1" s="16"/>
-      <c r="S1" s="84" t="s">
+      <c r="S1" s="81" t="s">
         <v>176</v>
       </c>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="85"/>
-      <c r="AI1" s="85"/>
-      <c r="AJ1" s="85"/>
-      <c r="AK1" s="85"/>
-      <c r="AL1" s="85"/>
-      <c r="AM1" s="85"/>
-      <c r="AN1" s="85"/>
-      <c r="AO1" s="85"/>
-      <c r="AP1" s="85"/>
-      <c r="AQ1" s="85"/>
-      <c r="AS1" s="86" t="s">
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="82"/>
+      <c r="AC1" s="82"/>
+      <c r="AD1" s="82"/>
+      <c r="AE1" s="82"/>
+      <c r="AF1" s="82"/>
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="82"/>
+      <c r="AI1" s="82"/>
+      <c r="AJ1" s="82"/>
+      <c r="AK1" s="82"/>
+      <c r="AL1" s="82"/>
+      <c r="AM1" s="82"/>
+      <c r="AN1" s="82"/>
+      <c r="AO1" s="82"/>
+      <c r="AP1" s="82"/>
+      <c r="AQ1" s="82"/>
+      <c r="AR1" s="82"/>
+      <c r="AT1" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AT1" s="87"/>
-      <c r="AU1" s="87"/>
-      <c r="AV1" s="87"/>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="87"/>
-      <c r="AY1" s="88"/>
-      <c r="BA1" s="81" t="s">
+      <c r="AU1" s="84"/>
+      <c r="AV1" s="84"/>
+      <c r="AW1" s="84"/>
+      <c r="AX1" s="84"/>
+      <c r="AY1" s="84"/>
+      <c r="AZ1" s="85"/>
+      <c r="BB1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="BB1" s="82"/>
-      <c r="BC1" s="83"/>
-      <c r="BD1"/>
-      <c r="BE1" s="89" t="s">
+      <c r="BC1" s="79"/>
+      <c r="BD1" s="80"/>
+      <c r="BE1"/>
+      <c r="BF1" s="86" t="s">
         <v>245</v>
       </c>
-      <c r="BF1" s="90"/>
-      <c r="BH1" s="72" t="s">
+      <c r="BG1" s="87"/>
+      <c r="BI1" s="72" t="s">
         <v>217</v>
       </c>
-      <c r="BI1" s="73"/>
-      <c r="BJ1" s="74"/>
+      <c r="BJ1" s="73"/>
+      <c r="BK1" s="74"/>
     </row>
-    <row r="2" spans="1:62" s="57" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" s="57" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>2</v>
       </c>
@@ -3477,121 +3480,124 @@
         <v>151</v>
       </c>
       <c r="Y2" s="56" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z2" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="Z2" s="56" t="s">
+      <c r="AA2" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="AA2" s="56" t="s">
+      <c r="AB2" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="AB2" s="56" t="s">
+      <c r="AC2" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="AC2" s="56" t="s">
+      <c r="AD2" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="AD2" s="56" t="s">
+      <c r="AE2" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="AE2" s="56" t="s">
+      <c r="AF2" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="AF2" s="56" t="s">
+      <c r="AG2" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="AG2" s="56" t="s">
+      <c r="AH2" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="AH2" s="56" t="s">
+      <c r="AI2" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="56" t="s">
+      <c r="AJ2" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="AJ2" s="56" t="s">
+      <c r="AK2" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="AK2" s="56" t="s">
+      <c r="AL2" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="AL2" s="56" t="s">
+      <c r="AM2" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="AM2" s="56" t="s">
+      <c r="AN2" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="AN2" s="56" t="s">
+      <c r="AO2" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="AO2" s="56" t="s">
+      <c r="AP2" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="AP2" s="56" t="s">
+      <c r="AQ2" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="AQ2" s="56" t="s">
+      <c r="AR2" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="AR2" s="53" t="s">
+      <c r="AS2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="AS2" s="48" t="s">
+      <c r="AT2" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="AT2" s="48" t="s">
+      <c r="AU2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AU2" s="48" t="s">
+      <c r="AV2" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AV2" s="48" t="s">
+      <c r="AW2" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="AW2" s="48" t="s">
+      <c r="AX2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="AX2" s="48" t="s">
+      <c r="AY2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="48" t="s">
+      <c r="AZ2" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="AZ2" s="53" t="s">
+      <c r="BA2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="BA2" s="49" t="s">
+      <c r="BB2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="BB2" s="52" t="s">
+      <c r="BC2" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="BC2" s="52" t="s">
+      <c r="BD2" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="BD2" s="53" t="s">
+      <c r="BE2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="BE2" s="65" t="s">
+      <c r="BF2" s="65" t="s">
         <v>246</v>
       </c>
-      <c r="BF2" s="65" t="s">
+      <c r="BG2" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="BG2" s="53" t="s">
+      <c r="BH2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="BH2" s="55" t="s">
+      <c r="BI2" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="BI2" s="55" t="s">
+      <c r="BJ2" s="55" t="s">
         <v>216</v>
       </c>
-      <c r="BJ2" s="55" t="s">
+      <c r="BK2" s="55" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>70</v>
       </c>
@@ -3658,112 +3664,115 @@
         <v>153</v>
       </c>
       <c r="Y3" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="Z3" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="Z3" s="24" t="s">
+      <c r="AA3" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="AA3" s="24" t="s">
+      <c r="AB3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AB3" s="24" t="s">
+      <c r="AC3" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AC3" s="24" t="s">
+      <c r="AD3" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="AD3" s="24" t="s">
+      <c r="AE3" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="AE3" s="24" t="s">
+      <c r="AF3" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="AF3" s="24" t="s">
+      <c r="AG3" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="AG3" s="24" t="s">
+      <c r="AH3" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="AH3" s="24" t="s">
+      <c r="AI3" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AI3" s="24" t="s">
+      <c r="AJ3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AJ3" s="24" t="s">
+      <c r="AK3" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="AK3" s="24" t="s">
+      <c r="AL3" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="AL3" s="24" t="s">
+      <c r="AM3" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="AM3" s="24" t="s">
+      <c r="AN3" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="AN3" s="24" t="s">
+      <c r="AO3" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="AO3" s="24" t="s">
+      <c r="AP3" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="AP3" s="24" t="s">
+      <c r="AQ3" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="AQ3" s="24" t="s">
+      <c r="AR3" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="AR3" s="3"/>
-      <c r="AS3" s="24" t="s">
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="AT3" s="24" t="s">
+      <c r="AU3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AU3" s="24" t="s">
+      <c r="AV3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AV3" s="24" t="s">
+      <c r="AW3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="AW3" s="24" t="s">
+      <c r="AX3" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AX3" s="24" t="s">
+      <c r="AY3" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="AY3" s="24" t="s">
+      <c r="AZ3" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="AZ3" s="3"/>
-      <c r="BA3" s="47" t="s">
+      <c r="BA3" s="3"/>
+      <c r="BB3" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="BB3" s="3" t="s">
+      <c r="BC3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="BC3" s="3" t="s">
+      <c r="BD3" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="BD3" s="3"/>
-      <c r="BE3" s="3" t="s">
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="BF3" s="3" t="s">
+      <c r="BG3" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="BH3" s="2" t="s">
+      <c r="BI3" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="BI3" s="2" t="s">
+      <c r="BJ3" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="BJ3" s="2" t="s">
+      <c r="BK3" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>74</v>
       </c>
@@ -3830,128 +3839,131 @@
         <v>153</v>
       </c>
       <c r="Y4" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="Z4" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="Z4" s="24" t="s">
+      <c r="AA4" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="AA4" s="24" t="s">
+      <c r="AB4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AB4" s="24" t="s">
+      <c r="AC4" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AC4" s="24" t="s">
+      <c r="AD4" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="AD4" s="24" t="s">
+      <c r="AE4" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="AE4" s="24" t="s">
+      <c r="AF4" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="AF4" s="24" t="s">
+      <c r="AG4" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="AG4" s="24" t="s">
+      <c r="AH4" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="AH4" s="24" t="s">
+      <c r="AI4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AI4" s="24" t="s">
+      <c r="AJ4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AJ4" s="24" t="s">
+      <c r="AK4" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="AK4" s="24" t="s">
+      <c r="AL4" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="AL4" s="24" t="s">
+      <c r="AM4" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="AM4" s="24" t="s">
+      <c r="AN4" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="AN4" s="24" t="s">
+      <c r="AO4" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="AO4" s="24" t="s">
+      <c r="AP4" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="AP4" s="24" t="s">
+      <c r="AQ4" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="AQ4" s="24" t="s">
+      <c r="AR4" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="AR4" s="3"/>
-      <c r="AS4" s="24" t="s">
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="AT4" s="24" t="s">
+      <c r="AU4" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AU4" s="24" t="s">
+      <c r="AV4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AV4" s="24" t="s">
+      <c r="AW4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="AW4" s="24" t="s">
+      <c r="AX4" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AX4" s="24" t="s">
+      <c r="AY4" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="AY4" s="24" t="s">
+      <c r="AZ4" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="AZ4" s="3"/>
-      <c r="BA4" s="47" t="s">
+      <c r="BA4" s="3"/>
+      <c r="BB4" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="BB4" s="3" t="s">
+      <c r="BC4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="BC4" s="3" t="s">
+      <c r="BD4" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="BD4" s="3"/>
-      <c r="BE4" s="3" t="s">
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="BF4" s="3" t="s">
+      <c r="BG4" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="BH4" s="2" t="s">
+      <c r="BI4" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="BI4" s="2" t="s">
+      <c r="BJ4" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="BJ4" s="2" t="s">
+      <c r="BK4" s="2" t="s">
         <v>221</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:BJ4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
+  <autoFilter ref="A2:BK4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
   <mergeCells count="7">
-    <mergeCell ref="BH1:BJ1"/>
+    <mergeCell ref="BI1:BK1"/>
     <mergeCell ref="J1:O1"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="S1:AQ1"/>
-    <mergeCell ref="AS1:AY1"/>
-    <mergeCell ref="BE1:BF1"/>
+    <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="AT1:AZ1"/>
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="S1:AR1"/>
   </mergeCells>
-  <conditionalFormatting sqref="BC3:BF65537">
+  <conditionalFormatting sqref="BD3:BG65537">
     <cfRule type="cellIs" dxfId="122" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB3:BB65537">
+  <conditionalFormatting sqref="BC3:BC65537">
     <cfRule type="cellIs" dxfId="121" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
@@ -4040,7 +4052,7 @@
       <selection pane="bottomRight" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -4058,7 +4070,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78"/>
+      <c r="A1" s="78" t="s">
+        <v>271</v>
+      </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
       <c r="D1" s="79"/>
@@ -4285,7 +4299,7 @@
       <selection pane="bottomRight" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -4304,7 +4318,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78"/>
+      <c r="A1" s="78" t="s">
+        <v>271</v>
+      </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
       <c r="D1" s="79"/>
@@ -4312,17 +4328,17 @@
       <c r="F1" s="79"/>
       <c r="G1" s="79"/>
       <c r="H1" s="80"/>
-      <c r="J1" s="91" t="s">
+      <c r="J1" s="88" t="s">
         <v>176</v>
       </c>
-      <c r="K1" s="92"/>
+      <c r="K1" s="89"/>
       <c r="M1" s="64" t="s">
         <v>177</v>
       </c>
-      <c r="O1" s="81" t="s">
+      <c r="O1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="83"/>
+      <c r="P1" s="80"/>
     </row>
     <row r="2" spans="1:16" s="57" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
@@ -4558,7 +4574,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
@@ -4695,7 +4711,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
@@ -4923,7 +4939,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="30" customWidth="1"/>
@@ -4974,38 +4990,38 @@
       <c r="K1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="93" t="s">
+      <c r="L1" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="94"/>
-      <c r="N1" s="95"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="92"/>
       <c r="O1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="93" t="s">
+      <c r="P1" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="97"/>
+      <c r="Q1" s="93"/>
+      <c r="R1" s="94"/>
       <c r="S1" s="26"/>
-      <c r="T1" s="93" t="s">
+      <c r="T1" s="90" t="s">
         <v>121</v>
       </c>
-      <c r="U1" s="96"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="96" t="s">
+      <c r="U1" s="93"/>
+      <c r="V1" s="94"/>
+      <c r="W1" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="97"/>
+      <c r="X1" s="93"/>
+      <c r="Y1" s="94"/>
       <c r="Z1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="AA1" s="98" t="s">
+      <c r="AA1" s="95" t="s">
         <v>244</v>
       </c>
-      <c r="AB1" s="94"/>
-      <c r="AC1" s="95"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="92"/>
     </row>
     <row r="2" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="8"/>
@@ -5285,7 +5301,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
@@ -5326,9 +5342,9 @@
       <c r="A1" s="66"/>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
       <c r="G1" s="68"/>
       <c r="H1" s="20" t="s">
         <v>65</v>
@@ -5351,47 +5367,47 @@
       <c r="N1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="98" t="s">
+      <c r="O1" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="95"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="92"/>
       <c r="R1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="S1" s="93" t="s">
+      <c r="S1" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="T1" s="96"/>
-      <c r="U1" s="97"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="94"/>
       <c r="V1" s="26"/>
-      <c r="W1" s="93" t="s">
+      <c r="W1" s="90" t="s">
         <v>169</v>
       </c>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="97"/>
+      <c r="X1" s="93"/>
+      <c r="Y1" s="94"/>
       <c r="Z1" s="39"/>
-      <c r="AA1" s="93" t="s">
+      <c r="AA1" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="AB1" s="96"/>
-      <c r="AC1" s="97"/>
+      <c r="AB1" s="93"/>
+      <c r="AC1" s="94"/>
       <c r="AD1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="AE1" s="98" t="s">
+      <c r="AE1" s="95" t="s">
         <v>244</v>
       </c>
-      <c r="AF1" s="94"/>
-      <c r="AG1" s="95"/>
+      <c r="AF1" s="91"/>
+      <c r="AG1" s="92"/>
     </row>
     <row r="2" spans="1:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
       <c r="G2" s="71"/>
       <c r="I2" s="36"/>
       <c r="J2" s="31"/>
@@ -5706,7 +5722,7 @@
       <selection pane="bottomRight" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -5726,7 +5742,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78"/>
+      <c r="A1" s="78" t="s">
+        <v>271</v>
+      </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
       <c r="D1" s="79"/>

</xml_diff>

<commit_message>
Correction de quotas #48
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE96DD7E-847B-4924-ACA4-39189D26A89B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494D8940-6A9E-4E5F-9C07-99552DDD5D2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="495" windowWidth="23070" windowHeight="12465" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="3105" yWindow="900" windowWidth="23715" windowHeight="13530" tabRatio="698" activeTab="7" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -605,9 +605,6 @@
     <t>Diplomes</t>
   </si>
   <si>
-    <t>$[F4]</t>
-  </si>
-  <si>
     <t>FC1</t>
   </si>
   <si>
@@ -885,6 +882,9 @@
   </si>
   <si>
     <t>Identification</t>
+  </si>
+  <si>
+    <t>$[G4]</t>
   </si>
 </sst>
 </file>
@@ -1452,26 +1452,26 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="10" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3071,117 +3071,117 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3277,7 +3277,7 @@
   </sheetPr>
   <dimension ref="A1:BK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3335,7 +3335,7 @@
   <sheetData>
     <row r="1" spans="1:63" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -3353,55 +3353,55 @@
       <c r="N1" s="76"/>
       <c r="O1" s="77"/>
       <c r="Q1" s="16"/>
-      <c r="S1" s="81" t="s">
+      <c r="S1" s="86" t="s">
         <v>176</v>
       </c>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="82"/>
-      <c r="AG1" s="82"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="82"/>
-      <c r="AJ1" s="82"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="82"/>
-      <c r="AM1" s="82"/>
-      <c r="AN1" s="82"/>
-      <c r="AO1" s="82"/>
-      <c r="AP1" s="82"/>
-      <c r="AQ1" s="82"/>
-      <c r="AR1" s="82"/>
-      <c r="AT1" s="83" t="s">
+      <c r="T1" s="87"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="87"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="87"/>
+      <c r="Z1" s="87"/>
+      <c r="AA1" s="87"/>
+      <c r="AB1" s="87"/>
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="87"/>
+      <c r="AE1" s="87"/>
+      <c r="AF1" s="87"/>
+      <c r="AG1" s="87"/>
+      <c r="AH1" s="87"/>
+      <c r="AI1" s="87"/>
+      <c r="AJ1" s="87"/>
+      <c r="AK1" s="87"/>
+      <c r="AL1" s="87"/>
+      <c r="AM1" s="87"/>
+      <c r="AN1" s="87"/>
+      <c r="AO1" s="87"/>
+      <c r="AP1" s="87"/>
+      <c r="AQ1" s="87"/>
+      <c r="AR1" s="87"/>
+      <c r="AT1" s="81" t="s">
         <v>177</v>
       </c>
-      <c r="AU1" s="84"/>
-      <c r="AV1" s="84"/>
-      <c r="AW1" s="84"/>
-      <c r="AX1" s="84"/>
-      <c r="AY1" s="84"/>
-      <c r="AZ1" s="85"/>
+      <c r="AU1" s="82"/>
+      <c r="AV1" s="82"/>
+      <c r="AW1" s="82"/>
+      <c r="AX1" s="82"/>
+      <c r="AY1" s="82"/>
+      <c r="AZ1" s="83"/>
       <c r="BB1" s="78" t="s">
         <v>5</v>
       </c>
       <c r="BC1" s="79"/>
       <c r="BD1" s="80"/>
       <c r="BE1"/>
-      <c r="BF1" s="86" t="s">
-        <v>245</v>
-      </c>
-      <c r="BG1" s="87"/>
+      <c r="BF1" s="84" t="s">
+        <v>244</v>
+      </c>
+      <c r="BG1" s="85"/>
       <c r="BI1" s="72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="BJ1" s="73"/>
       <c r="BK1" s="74"/>
@@ -3480,13 +3480,13 @@
         <v>151</v>
       </c>
       <c r="Y2" s="56" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z2" s="56" t="s">
         <v>156</v>
       </c>
       <c r="AA2" s="56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AB2" s="56" t="s">
         <v>8</v>
@@ -3534,16 +3534,16 @@
         <v>161</v>
       </c>
       <c r="AQ2" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="AR2" s="56" t="s">
         <v>179</v>
-      </c>
-      <c r="AR2" s="56" t="s">
-        <v>180</v>
       </c>
       <c r="AS2" s="53" t="s">
         <v>65</v>
       </c>
       <c r="AT2" s="48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AU2" s="48" t="s">
         <v>6</v>
@@ -3561,7 +3561,7 @@
         <v>15</v>
       </c>
       <c r="AZ2" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BA2" s="53" t="s">
         <v>65</v>
@@ -3579,22 +3579,22 @@
         <v>65</v>
       </c>
       <c r="BF2" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="BG2" s="65" t="s">
         <v>246</v>
-      </c>
-      <c r="BG2" s="65" t="s">
-        <v>247</v>
       </c>
       <c r="BH2" s="53" t="s">
         <v>65</v>
       </c>
       <c r="BI2" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="BJ2" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="BK2" s="55" t="s">
         <v>214</v>
-      </c>
-      <c r="BJ2" s="55" t="s">
-        <v>216</v>
-      </c>
-      <c r="BK2" s="55" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:63" x14ac:dyDescent="0.25">
@@ -3624,10 +3624,10 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="K3" s="24" t="s">
         <v>250</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>251</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>50</v>
@@ -3664,13 +3664,13 @@
         <v>153</v>
       </c>
       <c r="Y3" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z3" s="24" t="s">
         <v>157</v>
       </c>
       <c r="AA3" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AB3" s="24" t="s">
         <v>37</v>
@@ -3718,14 +3718,14 @@
         <v>173</v>
       </c>
       <c r="AQ3" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="AR3" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="AR3" s="24" t="s">
-        <v>182</v>
       </c>
       <c r="AS3" s="3"/>
       <c r="AT3" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AU3" s="24" t="s">
         <v>41</v>
@@ -3743,7 +3743,7 @@
         <v>172</v>
       </c>
       <c r="AZ3" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="BA3" s="3"/>
       <c r="BB3" s="47" t="s">
@@ -3753,23 +3753,23 @@
         <v>77</v>
       </c>
       <c r="BD3" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="BE3" s="3"/>
       <c r="BF3" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="BG3" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="BG3" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="BI3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="BJ3" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="BJ3" s="2" t="s">
+      <c r="BK3" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="BK3" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:63" x14ac:dyDescent="0.25">
@@ -3799,10 +3799,10 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="K4" s="24" t="s">
         <v>250</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>251</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>50</v>
@@ -3839,13 +3839,13 @@
         <v>153</v>
       </c>
       <c r="Y4" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z4" s="24" t="s">
         <v>157</v>
       </c>
       <c r="AA4" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AB4" s="24" t="s">
         <v>37</v>
@@ -3893,14 +3893,14 @@
         <v>173</v>
       </c>
       <c r="AQ4" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="AR4" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="AR4" s="24" t="s">
-        <v>182</v>
       </c>
       <c r="AS4" s="3"/>
       <c r="AT4" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AU4" s="24" t="s">
         <v>41</v>
@@ -3918,7 +3918,7 @@
         <v>172</v>
       </c>
       <c r="AZ4" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="BA4" s="3"/>
       <c r="BB4" s="47" t="s">
@@ -3928,23 +3928,23 @@
         <v>77</v>
       </c>
       <c r="BD4" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="BE4" s="3"/>
       <c r="BF4" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="BG4" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="BG4" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="BI4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="BJ4" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="BJ4" s="2" t="s">
+      <c r="BK4" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="BK4" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4071,7 +4071,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -4084,7 +4084,7 @@
         <v>176</v>
       </c>
       <c r="L1" s="64" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N1" s="63" t="s">
         <v>5</v>
@@ -4119,13 +4119,13 @@
         <v>65</v>
       </c>
       <c r="J2" s="56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K2" s="53" t="s">
         <v>65</v>
       </c>
       <c r="L2" s="48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M2" s="53" t="s">
         <v>65</v>
@@ -4136,7 +4136,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4161,20 +4161,20 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="47" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4199,15 +4199,15 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="47" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -4319,7 +4319,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -4369,16 +4369,16 @@
         <v>65</v>
       </c>
       <c r="J2" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="K2" s="56" t="s">
         <v>179</v>
-      </c>
-      <c r="K2" s="56" t="s">
-        <v>180</v>
       </c>
       <c r="L2" s="53" t="s">
         <v>65</v>
       </c>
       <c r="M2" s="48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N2" s="53" t="s">
         <v>65</v>
@@ -4392,7 +4392,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4417,26 +4417,26 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>182</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="47" t="s">
         <v>63</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4461,21 +4461,21 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="K4" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>182</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="47" t="s">
         <v>63</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -4608,51 +4608,51 @@
         <v>58</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H1" s="58" t="s">
         <v>65</v>
       </c>
       <c r="I1" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>190</v>
-      </c>
       <c r="K1" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" t="s">
         <v>194</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="K2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L2" s="1"/>
     </row>
@@ -4746,7 +4746,7 @@
         <v>58</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>65</v>
@@ -4794,7 +4794,7 @@
         <v>136</v>
       </c>
       <c r="T1" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U1" s="25" t="s">
         <v>137</v>
@@ -4803,7 +4803,7 @@
         <v>65</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="X1" s="18" t="s">
         <v>10</v>
@@ -4826,7 +4826,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4" t="s">
@@ -4868,7 +4868,7 @@
         <v>139</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>140</v>
@@ -4982,10 +4982,10 @@
         <v>97</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K1" s="20" t="s">
         <v>65</v>
@@ -5018,7 +5018,7 @@
         <v>65</v>
       </c>
       <c r="AA1" s="95" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AB1" s="91"/>
       <c r="AC1" s="92"/>
@@ -5140,10 +5140,10 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
@@ -5172,7 +5172,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>110</v>
@@ -5213,13 +5213,13 @@
         <v>92</v>
       </c>
       <c r="AC4" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AI4" t="s">
         <v>185</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -5294,7 +5294,7 @@
   </sheetPr>
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="8" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -5362,7 +5362,7 @@
         <v>168</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N1" s="20" t="s">
         <v>65</v>
@@ -5396,7 +5396,7 @@
         <v>65</v>
       </c>
       <c r="AE1" s="95" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AF1" s="91"/>
       <c r="AG1" s="92"/>
@@ -5449,7 +5449,7 @@
         <v>164</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F3" s="42" t="s">
         <v>17</v>
@@ -5550,7 +5550,7 @@
         <v>165</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>24</v>
@@ -5559,10 +5559,10 @@
         <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>117</v>
@@ -5571,7 +5571,7 @@
         <v>118</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="30" t="s">
@@ -5581,19 +5581,19 @@
         <v>28</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="S4" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="T4" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="T4" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="U4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>105</v>
@@ -5602,13 +5602,13 @@
         <v>113</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AB4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AE4" s="2">
         <v>1</v>
@@ -5617,7 +5617,7 @@
         <v>95</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -5743,7 +5743,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -5760,7 +5760,7 @@
       <c r="M1" s="76"/>
       <c r="O1" s="16"/>
       <c r="Q1" s="72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="R1" s="73"/>
       <c r="S1" s="74"/>
@@ -5815,18 +5815,18 @@
         <v>65</v>
       </c>
       <c r="Q2" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="S2" s="55" t="s">
         <v>214</v>
-      </c>
-      <c r="R2" s="55" t="s">
-        <v>216</v>
-      </c>
-      <c r="S2" s="55" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5851,10 +5851,10 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="K3" s="24" t="s">
         <v>250</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>251</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>50</v>
@@ -5867,18 +5867,18 @@
         <v>174</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -5903,10 +5903,10 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="K4" s="24" t="s">
         <v>250</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>251</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>50</v>
@@ -5919,13 +5919,13 @@
         <v>174</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#60 Option pour inclure les préinscrits
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_responsables.xlsx
+++ b/fichiers/conf/modele_responsables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AC83C4-0CFA-4C8D-80D7-299D1AD853F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C136789-6083-4384-A561-43108A0B70BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="825" windowWidth="24945" windowHeight="13740" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="698" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Farfadets!$A$2:$N$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Quota année'!$A$3:$AC$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Quota unités'!$A$3:$AG$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BK$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Responsables!$A$2:$BM$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Synthèse par unité'!$A$1:$Z$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="276">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -885,6 +885,18 @@
   </si>
   <si>
     <t>Feuille regroupant les responsables farfadets et les parents farfadets</t>
+  </si>
+  <si>
+    <t>${chef.qualitejs}</t>
+  </si>
+  <si>
+    <t>&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>Adhésion</t>
+  </si>
+  <si>
+    <t>${chef.typeadhesion}</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1031,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1065,6 +1077,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDABE5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1230,7 +1248,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1426,84 +1444,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1535,6 +1475,90 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Filler1" xfId="2" xr:uid="{23D6D387-F5AE-44CD-BDE2-B1DB25CA5EB4}"/>
@@ -1548,6 +1572,106 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="8" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
@@ -1568,6 +1692,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
@@ -1598,6 +1732,226 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
@@ -1608,6 +1962,36 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
@@ -1628,6 +2012,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
@@ -1638,6 +2042,116 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
@@ -1648,6 +2162,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
@@ -1658,12 +2192,52 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1678,6 +2252,106 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="8" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
@@ -1689,656 +2363,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF007E39"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2476,6 +2500,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEDABE5"/>
+      <color rgb="FFDEBABA"/>
       <color rgb="FF007E39"/>
     </mruColors>
   </colors>
@@ -3009,7 +3035,7 @@
   <sheetPr codeName="Feuil1">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:BK4"/>
+  <dimension ref="A1:BN4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -3065,82 +3091,87 @@
     <col min="61" max="61" width="13.5703125" style="2" customWidth="1"/>
     <col min="62" max="62" width="17.5703125" style="2" customWidth="1"/>
     <col min="63" max="63" width="27.85546875" style="2" customWidth="1"/>
+    <col min="64" max="64" width="2.85546875" customWidth="1"/>
+    <col min="65" max="65" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:66" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="88" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="75"/>
-      <c r="J1" s="70" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
+      <c r="J1" s="85" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="72"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="87"/>
       <c r="Q1" s="12"/>
-      <c r="S1" s="81" t="s">
+      <c r="S1" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="82"/>
-      <c r="AG1" s="82"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="82"/>
-      <c r="AJ1" s="82"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="82"/>
-      <c r="AM1" s="82"/>
-      <c r="AN1" s="82"/>
-      <c r="AO1" s="82"/>
-      <c r="AP1" s="82"/>
-      <c r="AQ1" s="82"/>
-      <c r="AR1" s="82"/>
-      <c r="AT1" s="76" t="s">
+      <c r="T1" s="97"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97"/>
+      <c r="AA1" s="97"/>
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97"/>
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="97"/>
+      <c r="AI1" s="97"/>
+      <c r="AJ1" s="97"/>
+      <c r="AK1" s="97"/>
+      <c r="AL1" s="97"/>
+      <c r="AM1" s="97"/>
+      <c r="AN1" s="97"/>
+      <c r="AO1" s="97"/>
+      <c r="AP1" s="97"/>
+      <c r="AQ1" s="97"/>
+      <c r="AR1" s="97"/>
+      <c r="AT1" s="91" t="s">
         <v>177</v>
       </c>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="77"/>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="77"/>
-      <c r="AZ1" s="78"/>
-      <c r="BB1" s="73" t="s">
+      <c r="AU1" s="92"/>
+      <c r="AV1" s="92"/>
+      <c r="AW1" s="92"/>
+      <c r="AX1" s="92"/>
+      <c r="AY1" s="92"/>
+      <c r="AZ1" s="93"/>
+      <c r="BB1" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="BC1" s="74"/>
-      <c r="BD1" s="75"/>
+      <c r="BC1" s="89"/>
+      <c r="BD1" s="90"/>
       <c r="BE1"/>
-      <c r="BF1" s="79" t="s">
+      <c r="BF1" s="94" t="s">
         <v>243</v>
       </c>
-      <c r="BG1" s="80"/>
-      <c r="BI1" s="67" t="s">
+      <c r="BG1" s="95"/>
+      <c r="BI1" s="82" t="s">
         <v>216</v>
       </c>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="69"/>
-    </row>
-    <row r="2" spans="1:63" s="52" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BJ1" s="83"/>
+      <c r="BK1" s="84"/>
+      <c r="BM1" s="81" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:66" s="52" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>2</v>
       </c>
@@ -3330,359 +3361,374 @@
       <c r="BK2" s="50" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="3" spans="1:63" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="93" t="s">
+      <c r="BM2" s="80" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:66" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="93" t="s">
+      <c r="H3" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="97" t="s">
+      <c r="I3" s="70"/>
+      <c r="J3" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="K3" s="71" t="s">
         <v>249</v>
       </c>
-      <c r="L3" s="97" t="s">
+      <c r="L3" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="97" t="s">
+      <c r="M3" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="98" t="s">
+      <c r="N3" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="O3" s="98" t="s">
+      <c r="O3" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="96" t="s">
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="S3" s="97" t="s">
+      <c r="S3" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="T3" s="97" t="s">
+      <c r="T3" s="71" t="s">
         <v>148</v>
       </c>
-      <c r="U3" s="97" t="s">
+      <c r="U3" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="V3" s="97" t="s">
+      <c r="V3" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="W3" s="97" t="s">
+      <c r="W3" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="X3" s="97" t="s">
+      <c r="X3" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="Y3" s="97" t="s">
+      <c r="Y3" s="71" t="s">
         <v>268</v>
       </c>
-      <c r="Z3" s="97" t="s">
+      <c r="Z3" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="AA3" s="97" t="s">
+      <c r="AA3" s="71" t="s">
         <v>228</v>
       </c>
-      <c r="AB3" s="97" t="s">
+      <c r="AB3" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="97" t="s">
+      <c r="AC3" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="AD3" s="97" t="s">
+      <c r="AD3" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="AE3" s="97" t="s">
+      <c r="AE3" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="AF3" s="97" t="s">
+      <c r="AF3" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="AG3" s="97" t="s">
+      <c r="AG3" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="AH3" s="97" t="s">
+      <c r="AH3" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="AI3" s="97" t="s">
+      <c r="AI3" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="AJ3" s="97" t="s">
+      <c r="AJ3" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="AK3" s="97" t="s">
+      <c r="AK3" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="AL3" s="97" t="s">
+      <c r="AL3" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="AM3" s="97" t="s">
+      <c r="AM3" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="AN3" s="97" t="s">
+      <c r="AN3" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="AO3" s="97" t="s">
+      <c r="AO3" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="AP3" s="97" t="s">
+      <c r="AP3" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="AQ3" s="97" t="s">
+      <c r="AQ3" s="71" t="s">
         <v>180</v>
       </c>
-      <c r="AR3" s="97" t="s">
+      <c r="AR3" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="AS3" s="96"/>
-      <c r="AT3" s="97" t="s">
+      <c r="AS3" s="70"/>
+      <c r="AT3" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="AU3" s="97" t="s">
+      <c r="AU3" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="AV3" s="97" t="s">
+      <c r="AV3" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="AW3" s="97" t="s">
+      <c r="AW3" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="AX3" s="97" t="s">
+      <c r="AX3" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="AY3" s="97" t="s">
+      <c r="AY3" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="AZ3" s="97" t="s">
+      <c r="AZ3" s="71" t="s">
         <v>225</v>
       </c>
-      <c r="BA3" s="96"/>
-      <c r="BB3" s="99" t="s">
+      <c r="BA3" s="70"/>
+      <c r="BB3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="BC3" s="96" t="s">
+      <c r="BC3" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="BD3" s="96" t="s">
+      <c r="BD3" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="BE3" s="96"/>
-      <c r="BF3" s="96" t="s">
+      <c r="BE3" s="70"/>
+      <c r="BF3" s="70" t="s">
         <v>246</v>
       </c>
-      <c r="BG3" s="96" t="s">
+      <c r="BG3" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="BI3" s="98" t="s">
+      <c r="BI3" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="BJ3" s="98" t="s">
+      <c r="BJ3" s="72" t="s">
         <v>219</v>
       </c>
-      <c r="BK3" s="98" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:63" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
+      <c r="BK3" s="72" t="s">
+        <v>272</v>
+      </c>
+      <c r="BM3" s="72" t="s">
+        <v>275</v>
+      </c>
+      <c r="BN3" s="68" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:66" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="K4" s="97" t="s">
+      <c r="K4" s="71" t="s">
         <v>249</v>
       </c>
-      <c r="L4" s="97" t="s">
+      <c r="L4" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="97" t="s">
+      <c r="M4" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="98" t="s">
+      <c r="N4" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="98" t="s">
+      <c r="O4" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="96" t="s">
+      <c r="P4" s="70"/>
+      <c r="Q4" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="T4" s="97" t="s">
+      <c r="T4" s="71" t="s">
         <v>148</v>
       </c>
-      <c r="U4" s="97" t="s">
+      <c r="U4" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="V4" s="97" t="s">
+      <c r="V4" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="W4" s="97" t="s">
+      <c r="W4" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="X4" s="97" t="s">
+      <c r="X4" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="Y4" s="97" t="s">
+      <c r="Y4" s="71" t="s">
         <v>268</v>
       </c>
-      <c r="Z4" s="97" t="s">
+      <c r="Z4" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="AA4" s="97" t="s">
+      <c r="AA4" s="71" t="s">
         <v>228</v>
       </c>
-      <c r="AB4" s="97" t="s">
+      <c r="AB4" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="AC4" s="97" t="s">
+      <c r="AC4" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="97" t="s">
+      <c r="AD4" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="AE4" s="97" t="s">
+      <c r="AE4" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="AF4" s="97" t="s">
+      <c r="AF4" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="AG4" s="97" t="s">
+      <c r="AG4" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="AH4" s="97" t="s">
+      <c r="AH4" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="AI4" s="97" t="s">
+      <c r="AI4" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="AJ4" s="97" t="s">
+      <c r="AJ4" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="AK4" s="97" t="s">
+      <c r="AK4" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="AL4" s="97" t="s">
+      <c r="AL4" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="AM4" s="97" t="s">
+      <c r="AM4" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="AN4" s="97" t="s">
+      <c r="AN4" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="AO4" s="97" t="s">
+      <c r="AO4" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="AP4" s="97" t="s">
+      <c r="AP4" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="AQ4" s="97" t="s">
+      <c r="AQ4" s="71" t="s">
         <v>180</v>
       </c>
-      <c r="AR4" s="97" t="s">
+      <c r="AR4" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="97" t="s">
+      <c r="AS4" s="70"/>
+      <c r="AT4" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="AU4" s="97" t="s">
+      <c r="AU4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="AV4" s="97" t="s">
+      <c r="AV4" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="AW4" s="97" t="s">
+      <c r="AW4" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="AX4" s="97" t="s">
+      <c r="AX4" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="AY4" s="97" t="s">
+      <c r="AY4" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="AZ4" s="97" t="s">
+      <c r="AZ4" s="71" t="s">
         <v>225</v>
       </c>
-      <c r="BA4" s="96"/>
-      <c r="BB4" s="99" t="s">
+      <c r="BA4" s="70"/>
+      <c r="BB4" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="BC4" s="96" t="s">
+      <c r="BC4" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="BD4" s="96" t="s">
+      <c r="BD4" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="BE4" s="96"/>
-      <c r="BF4" s="96" t="s">
+      <c r="BE4" s="70"/>
+      <c r="BF4" s="70" t="s">
         <v>246</v>
       </c>
-      <c r="BG4" s="96" t="s">
+      <c r="BG4" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="BI4" s="98" t="s">
+      <c r="BI4" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="BJ4" s="98" t="s">
+      <c r="BJ4" s="72" t="s">
         <v>219</v>
       </c>
-      <c r="BK4" s="98" t="s">
-        <v>220</v>
+      <c r="BK4" s="72" t="s">
+        <v>272</v>
+      </c>
+      <c r="BM4" s="72" t="s">
+        <v>275</v>
+      </c>
+      <c r="BN4" s="68" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:BK4" xr:uid="{A1D75911-FC2B-48DF-8A5A-1EFB88E8A4FD}"/>
+  <autoFilter ref="A2:BM2" xr:uid="{0DC98E3C-D20C-45B8-BB40-041AE1587316}"/>
   <mergeCells count="7">
     <mergeCell ref="BI1:BK1"/>
     <mergeCell ref="J1:O1"/>
@@ -3754,7 +3800,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:H1"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3775,16 +3821,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="88" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="75"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
       <c r="J1" s="57" t="s">
         <v>176</v>
       </c>
@@ -3839,79 +3885,79 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="93" t="s">
+    <row r="3" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="93" t="s">
+      <c r="H3" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="97" t="s">
+      <c r="I3" s="70"/>
+      <c r="J3" s="71" t="s">
         <v>228</v>
       </c>
-      <c r="K3" s="96"/>
-      <c r="L3" s="97" t="s">
+      <c r="K3" s="70"/>
+      <c r="L3" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="M3" s="96"/>
-      <c r="N3" s="99" t="s">
+      <c r="M3" s="70"/>
+      <c r="N3" s="73" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
+    <row r="4" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>232</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="71" t="s">
         <v>228</v>
       </c>
-      <c r="K4" s="96"/>
-      <c r="L4" s="97" t="s">
+      <c r="K4" s="70"/>
+      <c r="L4" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="M4" s="96"/>
-      <c r="N4" s="99" t="s">
+      <c r="M4" s="70"/>
+      <c r="N4" s="73" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3921,41 +3967,41 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H65537">
-    <cfRule type="beginsWith" dxfId="79" priority="3" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="79" priority="1" stopIfTrue="1" operator="beginsWith" text="19">
+      <formula>LEFT(G3,LEN("19"))="19"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="78" priority="2" stopIfTrue="1" operator="beginsWith" text="29">
+      <formula>LEFT(G3,LEN("29"))="29"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="77" priority="3" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(G3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="4" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="76" priority="4" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(G3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="77" priority="5" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="75" priority="5" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(G3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="6" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="74" priority="6" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(G3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="75" priority="7" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="73" priority="7" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(G3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="74" priority="8" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="72" priority="8" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(G3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="73" priority="9" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="71" priority="9" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(G3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="72" priority="10" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="70" priority="10" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(G3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="71" priority="11" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="69" priority="11" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(G3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="70" priority="12" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="68" priority="12" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(G3,LEN("21"))="21"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="69" priority="2" stopIfTrue="1" operator="beginsWith" text="29">
-      <formula>LEFT(G3,LEN("29"))="29"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="68" priority="1" stopIfTrue="1" operator="beginsWith" text="19">
-      <formula>LEFT(G3,LEN("19"))="19"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="1" gridLines="1"/>
@@ -3997,27 +4043,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="88" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="75"/>
-      <c r="J1" s="83" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
+      <c r="J1" s="98" t="s">
         <v>176</v>
       </c>
-      <c r="K1" s="84"/>
+      <c r="K1" s="99"/>
       <c r="M1" s="59" t="s">
         <v>177</v>
       </c>
-      <c r="O1" s="73" t="s">
+      <c r="O1" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="75"/>
+      <c r="P1" s="90"/>
     </row>
     <row r="2" spans="1:16" s="52" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
@@ -4069,91 +4115,91 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="93" t="s">
+    <row r="3" spans="1:16" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="93" t="s">
+      <c r="H3" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="97" t="s">
+      <c r="I3" s="70"/>
+      <c r="J3" s="71" t="s">
         <v>180</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="K3" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="L3" s="96"/>
-      <c r="M3" s="97" t="s">
+      <c r="L3" s="70"/>
+      <c r="M3" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="N3" s="96"/>
-      <c r="O3" s="99" t="s">
+      <c r="N3" s="70"/>
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="96" t="s">
+      <c r="P3" s="70" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
+    <row r="4" spans="1:16" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>234</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="71" t="s">
         <v>180</v>
       </c>
-      <c r="K4" s="97" t="s">
+      <c r="K4" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="L4" s="96"/>
-      <c r="M4" s="97" t="s">
+      <c r="L4" s="70"/>
+      <c r="M4" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="N4" s="96"/>
-      <c r="O4" s="99" t="s">
+      <c r="N4" s="70"/>
+      <c r="O4" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P4" s="96" t="s">
+      <c r="P4" s="70" t="s">
         <v>230</v>
       </c>
     </row>
@@ -4165,46 +4211,46 @@
     <mergeCell ref="O1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="P3:P65537">
-    <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H65537">
-    <cfRule type="beginsWith" dxfId="11" priority="3" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="66" priority="1" stopIfTrue="1" operator="beginsWith" text="19">
+      <formula>LEFT(G3,LEN("19"))="19"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="65" priority="2" stopIfTrue="1" operator="beginsWith" text="29">
+      <formula>LEFT(G3,LEN("29"))="29"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="64" priority="3" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(G3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="4" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="63" priority="4" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(G3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="5" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="62" priority="5" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(G3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="6" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="61" priority="6" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(G3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="7" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="60" priority="7" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(G3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="8" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="59" priority="8" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(G3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="9" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="58" priority="9" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(G3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="10" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="57" priority="10" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(G3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="11" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="56" priority="11" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(G3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="55" priority="12" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(G3,LEN("21"))="21"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="29">
-      <formula>LEFT(G3,LEN("29"))="29"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="beginsWith" text="19">
-      <formula>LEFT(G3,LEN("19"))="19"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="1" gridLines="1"/>
@@ -4276,76 +4322,76 @@
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+    <row r="2" spans="1:12" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="72" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="68" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E2" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="G2" s="96" t="s">
+      <c r="G2" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="I2" s="98" t="s">
+      <c r="I2" s="72" t="s">
         <v>195</v>
       </c>
-      <c r="J2" s="98" t="s">
+      <c r="J2" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="K2" s="94" t="s">
+      <c r="K2" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="L2" s="103"/>
+      <c r="L2" s="77"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K2" xr:uid="{F7D2DF7B-F46F-4C0B-92A8-F09F30ADB8E7}"/>
   <conditionalFormatting sqref="I2:I1000000">
-    <cfRule type="containsText" dxfId="67" priority="8" stopIfTrue="1" operator="containsText" text="BASSE">
+    <cfRule type="containsText" dxfId="54" priority="8" stopIfTrue="1" operator="containsText" text="BASSE">
       <formula>NOT(ISERROR(SEARCH("BASSE",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="9" stopIfTrue="1" operator="containsText" text="MOYENNE">
+    <cfRule type="containsText" dxfId="53" priority="9" stopIfTrue="1" operator="containsText" text="MOYENNE">
       <formula>NOT(ISERROR(SEARCH("MOYENNE",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="10" stopIfTrue="1" operator="containsText" text="HAUTE">
+    <cfRule type="containsText" dxfId="52" priority="10" stopIfTrue="1" operator="containsText" text="HAUTE">
       <formula>NOT(ISERROR(SEARCH("HAUTE",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="beginsWith" dxfId="64" priority="3" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="51" priority="3" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(G2,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="63" priority="4" stopIfTrue="1" operator="beginsWith" text="F">
+    <cfRule type="beginsWith" dxfId="50" priority="4" stopIfTrue="1" operator="beginsWith" text="F">
       <formula>LEFT(G2,LEN("F"))="F"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="62" priority="5" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="49" priority="5" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(G2,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="61" priority="6" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="48" priority="6" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(G2,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="7" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="47" priority="7" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(G2,LEN("LJ"))="LJ"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="beginsWith" dxfId="59" priority="2" stopIfTrue="1" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="46" priority="2" stopIfTrue="1" operator="beginsWith" text="R">
       <formula>LEFT(G2,LEN("R"))="R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H65537">
-    <cfRule type="beginsWith" dxfId="58" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
+    <cfRule type="beginsWith" dxfId="45" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
       <formula>LEFT(G3,LEN("V"))="V"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4473,75 +4519,75 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+    <row r="2" spans="1:26" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="96" t="s">
+      <c r="D2" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="E2" s="102"/>
-      <c r="F2" s="101" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="101" t="s">
+      <c r="G2" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="102" t="s">
+      <c r="H2" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="102"/>
-      <c r="J2" s="98" t="s">
+      <c r="I2" s="76"/>
+      <c r="J2" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="98" t="s">
+      <c r="K2" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="98" t="s">
+      <c r="L2" s="70"/>
+      <c r="M2" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="98" t="s">
+      <c r="N2" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="98" t="s">
+      <c r="O2" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="98" t="s">
+      <c r="P2" s="72" t="s">
         <v>131</v>
       </c>
-      <c r="Q2" s="98" t="s">
+      <c r="Q2" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="R2" s="98" t="s">
+      <c r="R2" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="S2" s="98" t="s">
+      <c r="S2" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="T2" s="98" t="s">
+      <c r="T2" s="72" t="s">
         <v>238</v>
       </c>
-      <c r="U2" s="98" t="s">
+      <c r="U2" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="V2" s="96"/>
-      <c r="W2" s="98" t="s">
+      <c r="V2" s="70"/>
+      <c r="W2" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="X2" s="98" t="s">
+      <c r="X2" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" s="98" t="s">
+      <c r="Y2" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="98" t="s">
+      <c r="Z2" s="72" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4556,27 +4602,27 @@
   </sheetData>
   <autoFilter ref="A1:Z1" xr:uid="{66A8F9AA-9955-4F38-8C09-E2219E483C8B}"/>
   <conditionalFormatting sqref="D2:D65536">
-    <cfRule type="beginsWith" dxfId="57" priority="3" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="44" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
+      <formula>LEFT(D2,LEN("V"))="V"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="43" priority="3" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(D2,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="4" stopIfTrue="1" operator="beginsWith" text="F">
+    <cfRule type="beginsWith" dxfId="42" priority="4" stopIfTrue="1" operator="beginsWith" text="F">
       <formula>LEFT(D2,LEN("F"))="F"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="55" priority="5" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="41" priority="5" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(D2,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="6" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="40" priority="6" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(D2,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="53" priority="7" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="39" priority="7" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(D2,LEN("LJ"))="LJ"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
-      <formula>LEFT(D2,LEN("V"))="V"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D65536">
-    <cfRule type="beginsWith" dxfId="51" priority="2" stopIfTrue="1" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="38" priority="2" stopIfTrue="1" operator="beginsWith" text="R">
       <formula>LEFT(D2,LEN("R"))="R"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4651,38 +4697,38 @@
       <c r="K1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="85" t="s">
+      <c r="L1" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="86"/>
-      <c r="N1" s="87"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="102"/>
       <c r="O1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="85" t="s">
+      <c r="P1" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="104"/>
       <c r="S1" s="22"/>
-      <c r="T1" s="85" t="s">
+      <c r="T1" s="100" t="s">
         <v>121</v>
       </c>
-      <c r="U1" s="88"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="88" t="s">
+      <c r="U1" s="103"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="89"/>
+      <c r="X1" s="103"/>
+      <c r="Y1" s="104"/>
       <c r="Z1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AA1" s="90" t="s">
+      <c r="AA1" s="105" t="s">
         <v>242</v>
       </c>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="87"/>
+      <c r="AB1" s="101"/>
+      <c r="AC1" s="102"/>
     </row>
     <row r="2" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="6"/>
@@ -4799,88 +4845,88 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+    <row r="4" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="68" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="78" t="s">
         <v>187</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="98" t="s">
+      <c r="E4" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="101" t="s">
+      <c r="G4" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="H4" s="101" t="s">
+      <c r="H4" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="101" t="s">
+      <c r="I4" s="75" t="s">
         <v>117</v>
       </c>
-      <c r="J4" s="101" t="s">
+      <c r="J4" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="K4" s="105"/>
-      <c r="L4" s="98">
+      <c r="K4" s="79"/>
+      <c r="L4" s="72">
         <v>1</v>
       </c>
-      <c r="M4" s="98" t="s">
+      <c r="M4" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="N4" s="101" t="s">
+      <c r="N4" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="O4" s="98"/>
-      <c r="P4" s="98" t="s">
+      <c r="O4" s="72"/>
+      <c r="P4" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="Q4" s="98" t="s">
+      <c r="Q4" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="R4" s="98" t="s">
+      <c r="R4" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="S4" s="98"/>
-      <c r="T4" s="98" t="s">
+      <c r="S4" s="72"/>
+      <c r="T4" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="V4" s="101" t="s">
+      <c r="V4" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="W4" s="98" t="s">
+      <c r="W4" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="X4" s="98" t="s">
+      <c r="X4" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="Y4" s="101" t="s">
+      <c r="Y4" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="Z4" s="98"/>
-      <c r="AA4" s="98">
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72">
         <v>1</v>
       </c>
-      <c r="AB4" s="98" t="s">
+      <c r="AB4" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="AC4" s="101" t="s">
+      <c r="AC4" s="75" t="s">
         <v>184</v>
       </c>
-      <c r="AE4" s="98" t="s">
+      <c r="AE4" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="AI4" s="94" t="s">
+      <c r="AI4" s="68" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4899,47 +4945,47 @@
     <mergeCell ref="AA1:AC1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F65536">
-    <cfRule type="cellIs" dxfId="50" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G65536">
-    <cfRule type="cellIs" dxfId="49" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H65536">
-    <cfRule type="cellIs" dxfId="48" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I65536">
-    <cfRule type="cellIs" dxfId="47" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J65536">
-    <cfRule type="cellIs" dxfId="46" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N65536">
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:V65536">
-    <cfRule type="cellIs" dxfId="44" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4:Y65536">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC65536">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5004,9 +5050,9 @@
       <c r="A1" s="61"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
       <c r="G1" s="63"/>
       <c r="H1" s="16" t="s">
         <v>65</v>
@@ -5029,47 +5075,47 @@
       <c r="N1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="90" t="s">
+      <c r="O1" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="87"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="102"/>
       <c r="R1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="S1" s="85" t="s">
+      <c r="S1" s="100" t="s">
         <v>125</v>
       </c>
-      <c r="T1" s="88"/>
-      <c r="U1" s="89"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="104"/>
       <c r="V1" s="22"/>
-      <c r="W1" s="85" t="s">
+      <c r="W1" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="89"/>
+      <c r="X1" s="103"/>
+      <c r="Y1" s="104"/>
       <c r="Z1" s="35"/>
-      <c r="AA1" s="85" t="s">
+      <c r="AA1" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="89"/>
+      <c r="AB1" s="103"/>
+      <c r="AC1" s="104"/>
       <c r="AD1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="AE1" s="90" t="s">
+      <c r="AE1" s="105" t="s">
         <v>242</v>
       </c>
-      <c r="AF1" s="86"/>
-      <c r="AG1" s="87"/>
+      <c r="AF1" s="101"/>
+      <c r="AG1" s="102"/>
     </row>
     <row r="2" spans="1:33" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="64"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
       <c r="G2" s="66"/>
       <c r="I2" s="32"/>
       <c r="J2" s="27"/>
@@ -5198,88 +5244,88 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+    <row r="4" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="68" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="101" t="s">
+      <c r="G4" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98" t="s">
+      <c r="H4" s="72"/>
+      <c r="I4" s="72" t="s">
         <v>261</v>
       </c>
-      <c r="J4" s="98" t="s">
+      <c r="J4" s="72" t="s">
         <v>262</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="L4" s="98" t="s">
+      <c r="L4" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="M4" s="98" t="s">
+      <c r="M4" s="72" t="s">
         <v>263</v>
       </c>
-      <c r="N4" s="105"/>
-      <c r="O4" s="104" t="s">
+      <c r="N4" s="79"/>
+      <c r="O4" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="P4" s="104" t="s">
+      <c r="P4" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="98" t="s">
+      <c r="Q4" s="72" t="s">
         <v>264</v>
       </c>
-      <c r="S4" s="98" t="s">
+      <c r="S4" s="72" t="s">
         <v>256</v>
       </c>
-      <c r="T4" s="104" t="s">
+      <c r="T4" s="78" t="s">
         <v>270</v>
       </c>
-      <c r="U4" s="98" t="s">
+      <c r="U4" s="72" t="s">
         <v>257</v>
       </c>
-      <c r="W4" s="98" t="s">
+      <c r="W4" s="72" t="s">
         <v>258</v>
       </c>
-      <c r="X4" s="98" t="s">
+      <c r="X4" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="Y4" s="98" t="s">
+      <c r="Y4" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="AA4" s="98" t="s">
+      <c r="AA4" s="72" t="s">
         <v>259</v>
       </c>
-      <c r="AB4" s="98" t="s">
+      <c r="AB4" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="AC4" s="98" t="s">
+      <c r="AC4" s="72" t="s">
         <v>184</v>
       </c>
-      <c r="AE4" s="98">
+      <c r="AE4" s="72">
         <v>1</v>
       </c>
-      <c r="AF4" s="98" t="s">
+      <c r="AF4" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="AG4" s="98" t="s">
+      <c r="AG4" s="72" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5294,77 +5340,77 @@
     <mergeCell ref="S1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="Q4:Q65537">
-    <cfRule type="cellIs" dxfId="41" priority="21" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="21" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4:U65537">
-    <cfRule type="cellIs" dxfId="40" priority="20" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="20" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4:Y65537">
-    <cfRule type="cellIs" dxfId="39" priority="19" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="19" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC65537">
-    <cfRule type="cellIs" dxfId="38" priority="18" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="18" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4:AG65537">
-    <cfRule type="cellIs" dxfId="37" priority="17" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I65537">
-    <cfRule type="cellIs" dxfId="36" priority="12" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="12" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J65537">
-    <cfRule type="cellIs" dxfId="35" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K65537">
-    <cfRule type="cellIs" dxfId="34" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L65537">
-    <cfRule type="cellIs" dxfId="33" priority="9" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="9" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M65537">
-    <cfRule type="cellIs" dxfId="32" priority="8" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="8" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E65536">
-    <cfRule type="beginsWith" dxfId="31" priority="3" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="18" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
+      <formula>LEFT(E4,LEN("V"))="V"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="17" priority="3" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(E4,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="4" stopIfTrue="1" operator="beginsWith" text="F">
+    <cfRule type="beginsWith" dxfId="16" priority="4" stopIfTrue="1" operator="beginsWith" text="F">
       <formula>LEFT(E4,LEN("F"))="F"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="29" priority="5" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="15" priority="5" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(E4,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="6" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="14" priority="6" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(E4,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="27" priority="7" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="13" priority="7" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(E4,LEN("LJ"))="LJ"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
-      <formula>LEFT(E4,LEN("V"))="V"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E65536">
-    <cfRule type="beginsWith" dxfId="25" priority="2" stopIfTrue="1" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="12" priority="2" stopIfTrue="1" operator="beginsWith" text="R">
       <formula>LEFT(E4,LEN("R"))="R"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5408,28 +5454,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="88" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="75"/>
-      <c r="J1" s="70" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
+      <c r="J1" s="85" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
       <c r="O1" s="12"/>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="82" t="s">
         <v>216</v>
       </c>
-      <c r="R1" s="68"/>
-      <c r="S1" s="69"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="84"/>
     </row>
     <row r="2" spans="1:19" s="52" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
@@ -5490,107 +5536,107 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="93" t="s">
+    <row r="3" spans="1:19" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>265</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="93" t="s">
+      <c r="H3" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="97" t="s">
+      <c r="I3" s="70"/>
+      <c r="J3" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="K3" s="71" t="s">
         <v>249</v>
       </c>
-      <c r="L3" s="97" t="s">
+      <c r="L3" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="97" t="s">
+      <c r="M3" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96" t="s">
+      <c r="N3" s="70"/>
+      <c r="O3" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="Q3" s="98" t="s">
+      <c r="Q3" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="R3" s="98" t="s">
+      <c r="R3" s="72" t="s">
         <v>219</v>
       </c>
-      <c r="S3" s="98" t="s">
+      <c r="S3" s="72" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
+    <row r="4" spans="1:19" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>266</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="K4" s="97" t="s">
+      <c r="K4" s="71" t="s">
         <v>249</v>
       </c>
-      <c r="L4" s="97" t="s">
+      <c r="L4" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="97" t="s">
+      <c r="M4" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="96"/>
-      <c r="O4" s="96" t="s">
+      <c r="N4" s="70"/>
+      <c r="O4" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="Q4" s="98" t="s">
+      <c r="Q4" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="R4" s="98" t="s">
+      <c r="R4" s="72" t="s">
         <v>219</v>
       </c>
-      <c r="S4" s="98" t="s">
+      <c r="S4" s="72" t="s">
         <v>220</v>
       </c>
     </row>
@@ -5602,41 +5648,41 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H65537">
-    <cfRule type="beginsWith" dxfId="24" priority="3" stopIfTrue="1" operator="beginsWith" text="14">
+    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="19">
+      <formula>LEFT(G3,LEN("19"))="19"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="29">
+      <formula>LEFT(G3,LEN("29"))="29"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="14">
       <formula>LEFT(G3,LEN("14"))="14"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="23" priority="4" stopIfTrue="1" operator="beginsWith" text="6">
+    <cfRule type="beginsWith" dxfId="8" priority="4" stopIfTrue="1" operator="beginsWith" text="6">
       <formula>LEFT(G3,LEN("6"))="6"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="5" stopIfTrue="1" operator="beginsWith" text="5">
+    <cfRule type="beginsWith" dxfId="7" priority="5" stopIfTrue="1" operator="beginsWith" text="5">
       <formula>LEFT(G3,LEN("5"))="5"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="6" stopIfTrue="1" operator="beginsWith" text="4">
+    <cfRule type="beginsWith" dxfId="6" priority="6" stopIfTrue="1" operator="beginsWith" text="4">
       <formula>LEFT(G3,LEN("4"))="4"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="7" stopIfTrue="1" operator="beginsWith" text="24">
+    <cfRule type="beginsWith" dxfId="5" priority="7" stopIfTrue="1" operator="beginsWith" text="24">
       <formula>LEFT(G3,LEN("24"))="24"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="8" stopIfTrue="1" operator="beginsWith" text="27">
+    <cfRule type="beginsWith" dxfId="4" priority="8" stopIfTrue="1" operator="beginsWith" text="27">
       <formula>LEFT(G3,LEN("27"))="27"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="9" stopIfTrue="1" operator="beginsWith" text="3">
+    <cfRule type="beginsWith" dxfId="3" priority="9" stopIfTrue="1" operator="beginsWith" text="3">
       <formula>LEFT(G3,LEN("3"))="3"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="17" priority="10" stopIfTrue="1" operator="beginsWith" text="23">
+    <cfRule type="beginsWith" dxfId="2" priority="10" stopIfTrue="1" operator="beginsWith" text="23">
       <formula>LEFT(G3,LEN("23"))="23"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="11" stopIfTrue="1" operator="beginsWith" text="22">
+    <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="beginsWith" text="22">
       <formula>LEFT(G3,LEN("22"))="22"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="15" priority="12" stopIfTrue="1" operator="beginsWith" text="21">
+    <cfRule type="beginsWith" dxfId="0" priority="12" stopIfTrue="1" operator="beginsWith" text="21">
       <formula>LEFT(G3,LEN("21"))="21"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="2" stopIfTrue="1" operator="beginsWith" text="29">
-      <formula>LEFT(G3,LEN("29"))="29"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="1" stopIfTrue="1" operator="beginsWith" text="19">
-      <formula>LEFT(G3,LEN("19"))="19"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>